<commit_message>
Kadaster config: KadasterNEN3610 schemarules for NEN3610
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -1328,10 +1328,10 @@
   <dimension ref="A1:N116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K94" sqref="K94"/>
+      <selection pane="bottomRight" activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2990,7 +2990,7 @@
         <v>26</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>26</v>
+        <v>250</v>
       </c>
       <c r="N74" s="8" t="s">
         <v>239</v>

</xml_diff>

<commit_message>
Added gml version and codelistoption; datalocation read from tv
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="299">
   <si>
     <t>Name</t>
   </si>
@@ -892,6 +892,36 @@
   </si>
   <si>
     <t>validatetvoccurs</t>
+  </si>
+  <si>
+    <t>GM_SENTINEL</t>
+  </si>
+  <si>
+    <t>gmlversion</t>
+  </si>
+  <si>
+    <t>versionID</t>
+  </si>
+  <si>
+    <t>The GML version to be used for ISO19136 schemas. Example: "3.3".</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>Standaard op 3.2.1 gezet.</t>
+  </si>
+  <si>
+    <t>codelistoption</t>
+  </si>
+  <si>
+    <t>Option1..Option5</t>
+  </si>
+  <si>
+    <t>The codelist option to apply in the ISO19136 schema.</t>
+  </si>
+  <si>
+    <t>Option1</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1038,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1037,6 +1067,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1325,13 +1367,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N116"/>
+  <dimension ref="A1:N118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I74" sqref="I74"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1502,16 +1544,16 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="12" t="b">
+      <c r="D7" s="14" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1522,10 +1564,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
@@ -1610,284 +1652,276 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="N13"/>
+    </row>
+    <row r="14" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="D14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N14" s="8" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2" t="s">
+      <c r="D15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="D17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="D20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="D21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D21" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" s="2" t="s">
+      <c r="D22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A22" s="7" t="s">
+      <c r="K22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" s="7" t="s">
+      <c r="D23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D23" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
+      <c r="D24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D24" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D25" s="2" t="b">
         <v>0</v>
@@ -1899,7 +1933,7 @@
         <v>17</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>4</v>
@@ -1908,18 +1942,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2" t="b">
         <v>1</v>
@@ -1928,7 +1962,7 @@
         <v>17</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>4</v>
@@ -1936,22 +1970,19 @@
       <c r="M26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N26" s="8" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="D27" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2" t="b">
         <v>1</v>
@@ -1960,7 +1991,7 @@
         <v>17</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>4</v>
@@ -1968,16 +1999,19 @@
       <c r="M27" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="N27" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>151</v>
       </c>
       <c r="D28" s="2" t="b">
         <v>0</v>
@@ -1985,39 +2019,51 @@
       <c r="E28" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>217</v>
+      <c r="J28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D29" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="D30" s="2" t="b">
         <v>0</v>
@@ -2028,42 +2074,30 @@
     </row>
     <row r="31" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D31" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A32" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
@@ -2084,302 +2118,311 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2" t="s">
+      <c r="D34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D35" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="D36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A36" s="7" t="s">
+    <row r="37" spans="1:14" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A37" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="7" t="s">
+      <c r="B37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36" s="7" t="s">
+      <c r="D37" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N36" s="7" t="s">
+      <c r="N37" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A37" s="7" t="s">
+    <row r="38" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A38" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" s="7" t="s">
+      <c r="D38" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N37" s="7" t="s">
+      <c r="N38" s="7" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="12" t="s">
+    <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="12" t="s">
+      <c r="B39" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
+      <c r="D39" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+    </row>
+    <row r="41" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D40" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
+      <c r="D41" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D41" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A42" s="2" t="s">
+      <c r="D42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="6" t="s">
+      <c r="D43" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="N42" s="2" t="s">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="N43" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6" t="s">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H44" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I43" s="6" t="s">
+      <c r="I44" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="7" t="s">
+      <c r="B45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D44" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="N44" s="8" t="s">
+      <c r="D45" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N45" s="8" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A45" s="7" t="s">
+    <row r="46" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A46" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B46" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D45" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" s="7" t="s">
+      <c r="D46" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D47" s="2" t="b">
         <v>0</v>
@@ -2391,282 +2434,289 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A48" s="7" t="s">
+    <row r="48" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A49" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="7" t="s">
+      <c r="B49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F48" s="7" t="s">
+      <c r="D49" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N48" s="7" t="s">
+      <c r="N49" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D49" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" s="2" t="s">
+      <c r="D50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
+    <row r="51" spans="1:14" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B51" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="N50" s="7" t="s">
+      <c r="D51" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N51" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A51" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D51" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N51" s="7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="N52" s="2" t="s">
-        <v>230</v>
+    <row r="52" spans="1:14" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A52" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="D52" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D53" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N53" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D53" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E53" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F53" s="7" t="s">
+      <c r="D55" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N53" s="7" t="s">
+      <c r="N55" s="7" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A54" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D54" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="N54" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
-        <v>198</v>
+        <v>70</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>199</v>
+        <v>71</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
       <c r="D56" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E56" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>247</v>
+      </c>
+      <c r="N56" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D57" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>250</v>
+      <c r="F57" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D58" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E58" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N59" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A59" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="60" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
-        <v>260</v>
+        <v>201</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>275</v>
+        <v>202</v>
       </c>
       <c r="D60" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" s="2" t="b">
         <v>0</v>
@@ -2675,336 +2725,327 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="2" t="s">
+    <row r="61" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N61" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D62" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="B63" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D61" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
+      <c r="D63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G62" s="2" t="s">
+      <c r="D64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H64" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="I64" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
+    <row r="65" spans="1:14" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A65" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="2" t="s">
+      <c r="D65" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="64" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="7" t="s">
+    <row r="66" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B66" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C66" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D64" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="7" t="s">
+      <c r="D66" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N64" s="7" t="s">
+      <c r="N66" s="7" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="65" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
+    <row r="67" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="2" t="s">
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A66" s="7" t="s">
+    <row r="68" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A68" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B68" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C68" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="D66" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="7" t="s">
+      <c r="D68" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="N66" s="8" t="s">
+      <c r="N68" s="8" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="2" t="s">
+    <row r="69" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D67" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G67" s="2" t="s">
+      <c r="D69" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="68" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
+    <row r="70" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D68" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" s="2" t="s">
+      <c r="D70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:14" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A69" s="7" t="s">
+    <row r="71" spans="1:14" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A71" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D69" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="7" t="s">
+      <c r="D71" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="N69" s="8" t="s">
+      <c r="N71" s="8" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="70" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A70" s="7" t="s">
+    <row r="72" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A72" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="7" t="s">
+      <c r="B72" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D70" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="7" t="s">
+      <c r="D72" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N70" s="7" t="s">
+      <c r="N72" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="71" spans="1:14" s="2" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
+    <row r="73" spans="1:14" s="2" customFormat="1" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D71" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="2" t="s">
+      <c r="D73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
+    <row r="74" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J72" s="2" t="s">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N73" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A74" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D74" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="N74" s="8" t="s">
-        <v>239</v>
+      <c r="L74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>209</v>
+        <v>5</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
@@ -3012,18 +3053,28 @@
       <c r="E75" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="F75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N75" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
+        <v>101</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="D76" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E76" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>26</v>
@@ -3032,61 +3083,63 @@
         <v>26</v>
       </c>
       <c r="I76" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="N76" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="2" t="s">
+      <c r="H78" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="2" t="s">
+      <c r="B79" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D77" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="N78" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D79" s="2" t="b">
         <v>0</v>
@@ -3098,298 +3151,289 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:14" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N80" s="8" t="s">
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N82" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="81" spans="1:14" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
+    <row r="83" spans="1:14" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A83" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="D83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N81" s="8" t="s">
+      <c r="N83" s="8" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="82" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A82" s="2" t="s">
+    <row r="84" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G82" s="2" t="s">
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H84" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="I84" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="N82" s="2" t="s">
+      <c r="N84" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="83" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A83" s="7" t="s">
+    <row r="85" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A85" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B85" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C85" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D83" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F83" s="7" t="s">
+      <c r="D85" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N83" s="7" t="s">
+      <c r="N85" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="84" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="7" t="s">
+    <row r="86" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="B86" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C86" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D84" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="7" t="s">
+      <c r="D86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="N84" s="7" t="s">
+      <c r="N86" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="85" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
+    <row r="87" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B85" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="7" t="s">
+      <c r="B87" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="7" t="s">
+      <c r="D87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N85" s="7" t="s">
+      <c r="N87" s="7" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M86" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D87" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J87" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L87" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M87" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M88" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M89" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2" t="s">
+      <c r="B90" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J88" s="2" t="s">
+      <c r="D90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M88" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
+      <c r="K90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="2" t="s">
+      <c r="B91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J89" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K89" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L89" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M89" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N90" s="7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="D91" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" s="2" t="b">
         <v>1</v>
@@ -3398,7 +3442,7 @@
         <v>17</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>4</v>
@@ -3406,93 +3450,139 @@
       <c r="M91" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N91" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J92" s="2" t="s">
+    </row>
+    <row r="92" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D92" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M92" s="2" t="s">
-        <v>4</v>
+      <c r="N92" s="7" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="93" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D93" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J93" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L93" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M93" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N93" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M94" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G93" s="2" t="s">
+      <c r="D95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H93" s="2" t="s">
+      <c r="H95" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I93" s="2" t="s">
+      <c r="I95" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:14" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
+    <row r="96" spans="1:14" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F94" s="2" t="s">
+      <c r="D96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="N94" s="2" t="s">
+      <c r="N96" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="N95"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="N96"/>
     </row>
     <row r="97" spans="14:14" x14ac:dyDescent="0.4">
       <c r="N97"/>
@@ -3553,6 +3643,12 @@
     </row>
     <row r="116" spans="14:14" x14ac:dyDescent="0.4">
       <c r="N116"/>
+    </row>
+    <row r="117" spans="14:14" x14ac:dyDescent="0.4">
+      <c r="N117"/>
+    </row>
+    <row r="118" spans="14:14" x14ac:dyDescent="0.4">
+      <c r="N118"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3560,14 +3656,14 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F19" r:id="rId1"/>
-    <hyperlink ref="F20" r:id="rId2"/>
+    <hyperlink ref="F20" r:id="rId1"/>
+    <hyperlink ref="F21" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId3"/>

</xml_diff>

<commit_message>
Simple Feature Profile conformance opgenomen. Via sfconformance parameter. In XSD het Simple Feature Profile conformance level op kunnen nemen
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="303">
   <si>
     <t>Name</t>
   </si>
@@ -894,9 +894,6 @@
     <t>validatetvoccurs</t>
   </si>
   <si>
-    <t>GM_SENTINEL</t>
-  </si>
-  <si>
     <t>gmlversion</t>
   </si>
   <si>
@@ -922,6 +919,21 @@
   </si>
   <si>
     <t>Option1</t>
+  </si>
+  <si>
+    <t>sfconformance</t>
+  </si>
+  <si>
+    <t>level nr</t>
+  </si>
+  <si>
+    <t>The GM 3.2 Simple Feature profile conformance level. Possible values are 0, 1 2.</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>GM_SENTINEL;GMLSF_SENTINEL</t>
   </si>
 </sst>
 </file>
@@ -1038,7 +1050,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1079,6 +1091,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1367,13 +1382,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N118"/>
+  <dimension ref="A1:N119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomRight" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1544,16 +1559,16 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="14" t="b">
+      <c r="D7" s="17" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1564,10 +1579,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
@@ -1654,22 +1669,22 @@
     </row>
     <row r="13" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>297</v>
-      </c>
-      <c r="D13" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>298</v>
       </c>
       <c r="N13"/>
     </row>
@@ -2263,16 +2278,16 @@
       </c>
     </row>
     <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="14" t="s">
+      <c r="B39" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="14" t="b">
+      <c r="D39" s="17" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="2" t="b">
@@ -2283,10 +2298,10 @@
       </c>
     </row>
     <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
     </row>
     <row r="41" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
@@ -2516,22 +2531,22 @@
     </row>
     <row r="52" spans="1:14" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A52" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="B52" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="C52" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="D52" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="16" t="s">
         <v>292</v>
-      </c>
-      <c r="D52" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>293</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
@@ -2541,7 +2556,7 @@
       <c r="L52" s="16"/>
       <c r="M52" s="16"/>
       <c r="N52" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="53" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2679,7 +2694,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="59" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>74</v>
       </c>
@@ -3106,198 +3121,195 @@
         <v>1</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A78" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="D78" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G78" s="2" t="s">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:14" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:14" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="2" t="s">
+      <c r="B80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="2" t="s">
+      <c r="D80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:14" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
+    <row r="81" spans="1:14" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="6" t="s">
+      <c r="D81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="N80" s="2" t="s">
+      <c r="N81" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
+    <row r="82" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="2" t="s">
+      <c r="B83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N82" s="8" t="s">
+      <c r="D83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N83" s="8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="83" spans="1:14" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
+    <row r="84" spans="1:14" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F83" s="2" t="s">
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N83" s="8" t="s">
+      <c r="N84" s="8" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
+    <row r="85" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G84" s="2" t="s">
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G85" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="H85" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I85" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="N84" s="2" t="s">
+      <c r="N85" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
+    <row r="86" spans="1:14" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B86" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C86" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="D85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="N85" s="7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="D86" s="7" t="b">
         <v>1</v>
@@ -3309,73 +3321,67 @@
         <v>261</v>
       </c>
       <c r="N86" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="87" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="N87" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="7" t="s">
+      <c r="B88" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="7" t="s">
+      <c r="D88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N87" s="7" t="s">
+      <c r="N88" s="7" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M88" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D89" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" s="2" t="b">
         <v>1</v>
@@ -3395,42 +3401,42 @@
     </row>
     <row r="90" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M90" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="2" t="s">
+      <c r="B91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D90" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L90" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M90" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="D91" s="2" t="b">
         <v>0</v>
@@ -3442,79 +3448,76 @@
         <v>17</v>
       </c>
       <c r="K91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M91" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D92" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J92" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M91" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="7" t="s">
+      <c r="K92" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M92" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B93" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C93" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D92" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F92" s="7" t="s">
+      <c r="D93" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N92" s="7" t="s">
+      <c r="N93" s="7" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J93" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N93" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>288</v>
+        <v>130</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D94" s="2" t="b">
         <v>1</v>
@@ -3534,102 +3537,131 @@
       <c r="M94" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="N94" s="2" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="95" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M95" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G95" s="2" t="s">
+      <c r="D96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G96" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H95" s="2" t="s">
+      <c r="H96" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I95" s="2" t="s">
+      <c r="I96" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:14" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:14" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" s="2" t="s">
+      <c r="D97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="N96" s="2" t="s">
+      <c r="N97" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="97" spans="14:14" x14ac:dyDescent="0.4">
-      <c r="N97"/>
-    </row>
-    <row r="98" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N98"/>
     </row>
-    <row r="99" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N99"/>
     </row>
-    <row r="100" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N100"/>
     </row>
-    <row r="101" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N101"/>
     </row>
-    <row r="102" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N102"/>
     </row>
-    <row r="103" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N103"/>
     </row>
-    <row r="104" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N104"/>
     </row>
-    <row r="105" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N105"/>
     </row>
-    <row r="106" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N106"/>
     </row>
-    <row r="107" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N107"/>
     </row>
-    <row r="108" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N108"/>
     </row>
-    <row r="109" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N109"/>
     </row>
-    <row r="110" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N110"/>
     </row>
-    <row r="111" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N111"/>
     </row>
-    <row r="112" spans="14:14" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.4">
       <c r="N112"/>
     </row>
     <row r="113" spans="14:14" x14ac:dyDescent="0.4">
@@ -3649,6 +3681,9 @@
     </row>
     <row r="118" spans="14:14" x14ac:dyDescent="0.4">
       <c r="N118"/>
+    </row>
+    <row r="119" spans="14:14" x14ac:dyDescent="0.4">
+      <c r="N119"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Json genereren op losse EP step #57
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\gitprojects\Imvertor-Maven\src\main\resources\input\Kadaster\props\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Kadaster\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="324">
   <si>
     <t>Name</t>
   </si>
@@ -985,6 +985,18 @@
   </si>
   <si>
     <t>[work/xsd-application]_[work/xsd-domain]_v[work/xsd-version].xsd</t>
+  </si>
+  <si>
+    <t>createjsonschema</t>
+  </si>
+  <si>
+    <t>Yes if JSON schema must be generated</t>
+  </si>
+  <si>
+    <t>jsonschemaname</t>
+  </si>
+  <si>
+    <t>The name of the json schema generated</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1126,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1189,6 +1201,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1482,13 +1497,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V122"/>
+  <dimension ref="A1:V124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B93" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F99" sqref="F99"/>
+      <selection pane="bottomRight" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1765,16 +1780,16 @@
       <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="30" t="b">
+      <c r="D8" s="31" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
@@ -1796,10 +1811,10 @@
       </c>
     </row>
     <row r="9" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
       <c r="G9" s="21"/>
       <c r="L9" s="21"/>
       <c r="M9" s="17"/>
@@ -2561,55 +2576,80 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="2" t="s">
-        <v>213</v>
+    <row r="30" spans="1:22" s="30" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="30" t="s">
+        <v>320</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="D30" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" s="29"/>
+      <c r="M30" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="O30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="S30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="T30" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="U30" s="30" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>174</v>
+        <v>34</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>175</v>
+        <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>176</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="G31" s="21"/>
       <c r="L31" s="21"/>
@@ -2622,16 +2662,19 @@
       <c r="S31" s="17"/>
       <c r="T31" s="17"/>
       <c r="U31" s="17"/>
-    </row>
-    <row r="32" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="V31" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
@@ -2653,69 +2696,41 @@
     </row>
     <row r="33" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+    </row>
+    <row r="34" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33" s="21"/>
-      <c r="H33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L33" s="21"/>
-      <c r="M33" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N33" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O33" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P33" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="S33" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="T33" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="U33" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2" t="b">
         <v>0</v>
@@ -2763,159 +2778,189 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:22" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G35" s="21"/>
+      <c r="H35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L35" s="21"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
+      <c r="M35" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N35" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O35" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P35" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q35" s="21"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="17"/>
-    </row>
-    <row r="36" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R35" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S35" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="T35" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="U35" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D36" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G36" s="21"/>
-      <c r="H36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L36" s="21"/>
-      <c r="M36" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P36" s="17" t="s">
-        <v>4</v>
-      </c>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
       <c r="Q36" s="21"/>
-      <c r="R36" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="S36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="T36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="U36" s="17" t="s">
-        <v>4</v>
-      </c>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
     </row>
     <row r="37" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="H37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L37" s="21"/>
+      <c r="M37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="T37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="U37" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D37" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="17"/>
-      <c r="S37" s="17"/>
-      <c r="T37" s="17"/>
-      <c r="U37" s="17"/>
-    </row>
-    <row r="38" spans="1:22" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A38" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F38" s="7" t="s">
+      <c r="D38" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G38" s="21"/>
       <c r="L38" s="21"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
       <c r="Q38" s="21"/>
-      <c r="V38" s="7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+    </row>
+    <row r="39" spans="1:22" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A39" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D39" s="7" t="b">
         <v>1</v>
@@ -2924,51 +2969,60 @@
         <v>0</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>254</v>
+        <v>16</v>
       </c>
       <c r="G39" s="21"/>
       <c r="L39" s="21"/>
       <c r="Q39" s="21"/>
       <c r="V39" s="7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D40" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>16</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A40" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>254</v>
       </c>
       <c r="G40" s="21"/>
       <c r="L40" s="21"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="17"/>
-      <c r="S40" s="17"/>
-      <c r="T40" s="17"/>
-      <c r="U40" s="17"/>
+      <c r="V40" s="7" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="41" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
+      <c r="A41" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G41" s="21"/>
       <c r="L41" s="21"/>
       <c r="M41" s="17"/>
@@ -2981,22 +3035,11 @@
       <c r="T41" s="17"/>
       <c r="U41" s="17"/>
     </row>
-    <row r="42" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A42" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D42" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
       <c r="G42" s="21"/>
       <c r="L42" s="21"/>
       <c r="M42" s="17"/>
@@ -3009,21 +3052,21 @@
       <c r="T42" s="17"/>
       <c r="U42" s="17"/>
     </row>
-    <row r="43" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>182</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>5</v>
+        <v>183</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="D43" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="21"/>
       <c r="L43" s="21"/>
@@ -3037,15 +3080,15 @@
       <c r="T43" s="17"/>
       <c r="U43" s="17"/>
     </row>
-    <row r="44" spans="1:22" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D44" s="2" t="b">
         <v>0</v>
@@ -3053,38 +3096,36 @@
       <c r="E44" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="G44" s="22"/>
-      <c r="L44" s="22"/>
+      <c r="G44" s="21"/>
+      <c r="L44" s="21"/>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
       <c r="O44" s="17"/>
       <c r="P44" s="17"/>
-      <c r="Q44" s="22"/>
+      <c r="Q44" s="21"/>
       <c r="R44" s="17"/>
       <c r="S44" s="17"/>
       <c r="T44" s="17"/>
       <c r="U44" s="17"/>
-      <c r="V44" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="45" spans="1:22" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
+        <v>55</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="D45" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>25</v>
+        <v>221</v>
       </c>
       <c r="G45" s="22"/>
       <c r="L45" s="22"/>
@@ -3097,43 +3138,47 @@
       <c r="S45" s="17"/>
       <c r="T45" s="17"/>
       <c r="U45" s="17"/>
-    </row>
-    <row r="46" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="7" t="s">
+      <c r="V45" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="17"/>
+      <c r="U46" s="17"/>
+    </row>
+    <row r="47" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B47" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C47" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="D46" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G46" s="21"/>
-      <c r="L46" s="21"/>
-      <c r="Q46" s="21"/>
-      <c r="V46" s="8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A47" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>189</v>
-      </c>
       <c r="D47" s="7" t="b">
         <v>0</v>
       </c>
@@ -3141,52 +3186,47 @@
         <v>1</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>242</v>
+        <v>4</v>
       </c>
       <c r="G47" s="21"/>
       <c r="L47" s="21"/>
       <c r="Q47" s="21"/>
-    </row>
-    <row r="48" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>16</v>
+      <c r="V47" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A48" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D48" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="G48" s="21"/>
       <c r="L48" s="21"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="17"/>
       <c r="Q48" s="21"/>
-      <c r="R48" s="17"/>
-      <c r="S48" s="17"/>
-      <c r="T48" s="17"/>
-      <c r="U48" s="17"/>
     </row>
     <row r="49" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D49" s="2" t="b">
         <v>0</v>
@@ -3209,293 +3249,279 @@
       <c r="T49" s="17"/>
       <c r="U49" s="17"/>
     </row>
-    <row r="50" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" s="7" t="s">
+    <row r="50" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" s="7" t="s">
+      <c r="C50" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G50" s="21"/>
       <c r="L50" s="21"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
       <c r="Q50" s="21"/>
-      <c r="V50" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B51" s="2" t="s">
+      <c r="R50" s="17"/>
+      <c r="S50" s="17"/>
+      <c r="T50" s="17"/>
+      <c r="U50" s="17"/>
+    </row>
+    <row r="51" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D51" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="2" t="s">
+      <c r="C51" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G51" s="21"/>
       <c r="L51" s="21"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="17"/>
-      <c r="O51" s="17"/>
-      <c r="P51" s="17"/>
       <c r="Q51" s="21"/>
-      <c r="R51" s="17"/>
-      <c r="S51" s="17"/>
-      <c r="T51" s="17"/>
-      <c r="U51" s="17"/>
-    </row>
-    <row r="52" spans="1:22" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A52" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D52" s="7" t="b">
-        <v>0</v>
+      <c r="V51" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G52" s="21"/>
       <c r="L52" s="21"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
       <c r="Q52" s="21"/>
-      <c r="V52" s="7" t="s">
+      <c r="R52" s="17"/>
+      <c r="S52" s="17"/>
+      <c r="T52" s="17"/>
+      <c r="U52" s="17"/>
+    </row>
+    <row r="53" spans="1:22" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A53" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="Q53" s="21"/>
+      <c r="V53" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A53" s="16" t="s">
+    <row r="54" spans="1:22" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A54" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B54" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C54" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="D53" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="16" t="s">
+      <c r="D54" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="G53" s="23"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="16"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16"/>
-      <c r="L53" s="23"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="16"/>
-      <c r="O53" s="16"/>
-      <c r="P53" s="16"/>
-      <c r="Q53" s="23"/>
-      <c r="R53" s="16"/>
-      <c r="S53" s="16"/>
-      <c r="T53" s="16"/>
-      <c r="U53" s="16"/>
-      <c r="V53" s="16" t="s">
+      <c r="G54" s="23"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="23"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="23"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+      <c r="T54" s="16"/>
+      <c r="U54" s="16"/>
+      <c r="V54" s="16" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="54" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A54" s="7" t="s">
+    <row r="55" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F54" s="7" t="s">
+      <c r="D55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G54" s="21"/>
-      <c r="L54" s="21"/>
-      <c r="Q54" s="21"/>
-      <c r="V54" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="G55" s="21"/>
       <c r="L55" s="21"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="17"/>
       <c r="Q55" s="21"/>
-      <c r="R55" s="17"/>
-      <c r="S55" s="17"/>
-      <c r="T55" s="17"/>
-      <c r="U55" s="17"/>
-      <c r="V55" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A56" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D56" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E56" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>254</v>
+      <c r="V55" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="G56" s="21"/>
       <c r="L56" s="21"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
       <c r="Q56" s="21"/>
-      <c r="V56" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D57" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>243</v>
+      <c r="R56" s="17"/>
+      <c r="S56" s="17"/>
+      <c r="T56" s="17"/>
+      <c r="U56" s="17"/>
+      <c r="V56" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>254</v>
       </c>
       <c r="G57" s="21"/>
       <c r="L57" s="21"/>
-      <c r="M57" s="17"/>
-      <c r="N57" s="17"/>
-      <c r="O57" s="17"/>
-      <c r="P57" s="17"/>
       <c r="Q57" s="21"/>
-      <c r="R57" s="17"/>
-      <c r="S57" s="17"/>
-      <c r="T57" s="17"/>
-      <c r="U57" s="17"/>
-      <c r="V57" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="58" spans="1:22" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A58" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G58" s="21"/>
-      <c r="L58" s="21"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="17"/>
-      <c r="Q58" s="21"/>
-      <c r="R58" s="17"/>
-      <c r="S58" s="17"/>
-      <c r="T58" s="17"/>
-      <c r="U58" s="17"/>
-      <c r="V58" s="2" t="s">
-        <v>228</v>
-      </c>
+      <c r="V57" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>322</v>
+      </c>
+      <c r="B58" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" t="s">
+        <v>323</v>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>264</v>
+      </c>
+      <c r="G58" s="29"/>
+      <c r="L58" s="29"/>
+      <c r="Q58" s="29"/>
     </row>
     <row r="59" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
-        <v>197</v>
+        <v>69</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>198</v>
+        <v>70</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>199</v>
+        <v>151</v>
       </c>
       <c r="D59" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E59" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="G59" s="21"/>
       <c r="L59" s="21"/>
@@ -3508,145 +3534,156 @@
       <c r="S59" s="17"/>
       <c r="T59" s="17"/>
       <c r="U59" s="17"/>
-    </row>
-    <row r="60" spans="1:22" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="D60" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="25" t="s">
-        <v>311</v>
+      <c r="V59" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A60" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="G60" s="21"/>
       <c r="L60" s="21"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="17"/>
+      <c r="P60" s="17"/>
       <c r="Q60" s="21"/>
-      <c r="V60" s="25" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="61" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R60" s="17"/>
+      <c r="S60" s="17"/>
+      <c r="T60" s="17"/>
+      <c r="U60" s="17"/>
+      <c r="V60" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
-        <v>73</v>
+        <v>197</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>10</v>
+        <v>198</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>74</v>
+        <v>199</v>
       </c>
       <c r="D61" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="G61" s="21"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
       <c r="L61" s="21"/>
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
       <c r="O61" s="17"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="21"/>
-      <c r="R61" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="S61" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="T61" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="U61" s="18" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="62" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B62" s="2" t="s">
+      <c r="R61" s="17"/>
+      <c r="S61" s="17"/>
+      <c r="T61" s="17"/>
+      <c r="U61" s="17"/>
+    </row>
+    <row r="62" spans="1:22" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="B62" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>16</v>
+      <c r="C62" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="D62" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="25" t="s">
+        <v>311</v>
       </c>
       <c r="G62" s="21"/>
       <c r="L62" s="21"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="17"/>
       <c r="Q62" s="21"/>
-      <c r="R62" s="17"/>
-      <c r="S62" s="17"/>
-      <c r="T62" s="17"/>
-      <c r="U62" s="17"/>
-    </row>
-    <row r="63" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D63" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>16</v>
+      <c r="V62" s="25" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="G63" s="21"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
       <c r="L63" s="21"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
       <c r="Q63" s="21"/>
-      <c r="V63" s="7" t="s">
-        <v>230</v>
+      <c r="R63" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="S63" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="T63" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="U63" s="18" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
-        <v>253</v>
+        <v>200</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>268</v>
+        <v>201</v>
       </c>
       <c r="D64" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" s="2" t="b">
         <v>0</v>
@@ -3666,46 +3703,41 @@
       <c r="T64" s="17"/>
       <c r="U64" s="17"/>
     </row>
-    <row r="65" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B65" s="2" t="s">
+    <row r="65" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>4</v>
+      <c r="C65" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G65" s="21"/>
       <c r="L65" s="21"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
-      <c r="O65" s="17"/>
-      <c r="P65" s="17"/>
       <c r="Q65" s="21"/>
-      <c r="R65" s="17"/>
-      <c r="S65" s="17"/>
-      <c r="T65" s="17"/>
-      <c r="U65" s="17"/>
-    </row>
-    <row r="66" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="V65" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>79</v>
+        <v>253</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>80</v>
+        <v>268</v>
       </c>
       <c r="D66" s="2" t="b">
         <v>1</v>
@@ -3713,55 +3745,30 @@
       <c r="E66" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F66" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G66" s="21"/>
-      <c r="H66" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I66" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J66" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K66" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="L66" s="21"/>
-      <c r="M66" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="N66" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="O66" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="P66" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="M66" s="17"/>
+      <c r="N66" s="17"/>
+      <c r="O66" s="17"/>
+      <c r="P66" s="17"/>
       <c r="Q66" s="21"/>
-      <c r="R66" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="S66" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="T66" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="U66" s="18" t="s">
-        <v>297</v>
-      </c>
+      <c r="R66" s="17"/>
+      <c r="S66" s="17"/>
+      <c r="T66" s="17"/>
+      <c r="U66" s="17"/>
     </row>
     <row r="67" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
@@ -3770,7 +3777,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>153</v>
+        <v>4</v>
       </c>
       <c r="G67" s="21"/>
       <c r="L67" s="21"/>
@@ -3784,41 +3791,71 @@
       <c r="T67" s="17"/>
       <c r="U67" s="17"/>
     </row>
-    <row r="68" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B68" s="7" t="s">
+    <row r="68" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D68" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="7" t="s">
+      <c r="C68" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" s="21"/>
+      <c r="H68" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G68" s="21"/>
+      <c r="I68" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J68" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K68" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="L68" s="21"/>
+      <c r="M68" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N68" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O68" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P68" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="Q68" s="21"/>
-      <c r="V68" s="7" t="s">
-        <v>270</v>
+      <c r="R68" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="S68" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="T68" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="U68" s="18" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="69" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>202</v>
+        <v>81</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>203</v>
+        <v>82</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>204</v>
+        <v>83</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
@@ -3827,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="G69" s="21"/>
       <c r="L69" s="21"/>
@@ -3841,272 +3878,246 @@
       <c r="T69" s="17"/>
       <c r="U69" s="17"/>
     </row>
-    <row r="70" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A70" s="7" t="s">
-        <v>205</v>
+        <v>84</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>183</v>
+        <v>10</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>206</v>
+        <v>85</v>
       </c>
       <c r="D70" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>244</v>
+        <v>25</v>
       </c>
       <c r="G70" s="21"/>
       <c r="L70" s="21"/>
       <c r="Q70" s="21"/>
-      <c r="V70" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="71" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="V70" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>86</v>
+        <v>202</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="D71" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F71" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G71" s="21"/>
-      <c r="H71" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J71" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="K71" s="17" t="s">
-        <v>87</v>
-      </c>
       <c r="L71" s="21"/>
-      <c r="M71" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="N71" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="O71" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="P71" s="17" t="s">
-        <v>247</v>
-      </c>
+      <c r="M71" s="17"/>
+      <c r="N71" s="17"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="17"/>
       <c r="Q71" s="21"/>
-      <c r="R71" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="S71" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="T71" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="U71" s="17" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="72" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>90</v>
+      <c r="R71" s="17"/>
+      <c r="S71" s="17"/>
+      <c r="T71" s="17"/>
+      <c r="U71" s="17"/>
+    </row>
+    <row r="72" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A72" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D72" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="G72" s="21"/>
       <c r="L72" s="21"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
       <c r="Q72" s="21"/>
-      <c r="R72" s="17"/>
-      <c r="S72" s="17"/>
-      <c r="T72" s="17"/>
-      <c r="U72" s="17"/>
-    </row>
-    <row r="73" spans="1:22" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A73" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D73" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>94</v>
+      <c r="V72" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G73" s="21"/>
+      <c r="H73" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J73" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K73" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="L73" s="21"/>
+      <c r="M73" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="N73" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="O73" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="P73" s="17" t="s">
+        <v>247</v>
+      </c>
       <c r="Q73" s="21"/>
-      <c r="V73" s="8" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="74" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A74" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D74" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>16</v>
+      <c r="R73" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="S73" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="T73" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="U73" s="17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G74" s="21"/>
       <c r="L74" s="21"/>
+      <c r="M74" s="17"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
       <c r="Q74" s="21"/>
-      <c r="V74" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="75" spans="1:22" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A75" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>98</v>
+      <c r="R74" s="17"/>
+      <c r="S74" s="17"/>
+      <c r="T74" s="17"/>
+      <c r="U74" s="17"/>
+    </row>
+    <row r="75" spans="1:22" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A75" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D75" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G75" s="21"/>
       <c r="L75" s="21"/>
-      <c r="M75" s="17"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="17"/>
       <c r="Q75" s="21"/>
-      <c r="R75" s="17"/>
-      <c r="S75" s="17"/>
-      <c r="T75" s="17"/>
-      <c r="U75" s="17"/>
-    </row>
-    <row r="76" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>1</v>
+      <c r="V75" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A76" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D76" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G76" s="21"/>
-      <c r="H76" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L76" s="21"/>
-      <c r="M76" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N76" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O76" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P76" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="Q76" s="21"/>
-      <c r="R76" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="S76" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="T76" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="U76" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="V76" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>157</v>
+        <v>99</v>
       </c>
       <c r="D77" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="G77" s="21"/>
       <c r="L77" s="21"/>
@@ -4119,78 +4130,68 @@
       <c r="S77" s="17"/>
       <c r="T77" s="17"/>
       <c r="U77" s="17"/>
-      <c r="V77" s="8" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="78" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="78" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
       <c r="D78" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E78" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78" s="21"/>
-      <c r="H78" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I78" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J78" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K78" s="17" t="s">
-        <v>25</v>
+      <c r="H78" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K78" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="L78" s="21"/>
       <c r="M78" s="17" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="N78" s="17" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="O78" s="17" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="P78" s="17" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="Q78" s="21"/>
-      <c r="R78" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="S78" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="T78" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="U78" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="V78" s="8" t="s">
-        <v>235</v>
+      <c r="R78" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S78" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="T78" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="U78" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>208</v>
+        <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>209</v>
+        <v>157</v>
       </c>
       <c r="D79" s="2" t="b">
         <v>0</v>
@@ -4198,8 +4199,8 @@
       <c r="E79" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F79" s="12" t="s">
-        <v>295</v>
+      <c r="F79" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G79" s="21"/>
       <c r="L79" s="21"/>
@@ -4212,108 +4213,118 @@
       <c r="S79" s="17"/>
       <c r="T79" s="17"/>
       <c r="U79" s="17"/>
-    </row>
-    <row r="80" spans="1:22" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="14" t="s">
+      <c r="V79" s="8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G80" s="21"/>
+      <c r="H80" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I80" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J80" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K80" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="L80" s="21"/>
+      <c r="M80" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N80" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O80" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P80" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q80" s="21"/>
+      <c r="R80" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="S80" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="T80" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="U80" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="V80" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="G81" s="21"/>
+      <c r="L81" s="21"/>
+      <c r="M81" s="17"/>
+      <c r="N81" s="17"/>
+      <c r="O81" s="17"/>
+      <c r="P81" s="17"/>
+      <c r="Q81" s="21"/>
+      <c r="R81" s="17"/>
+      <c r="S81" s="17"/>
+      <c r="T81" s="17"/>
+      <c r="U81" s="17"/>
+    </row>
+    <row r="82" spans="1:22" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B82" s="14" t="s">
         <v>292</v>
       </c>
-      <c r="C80" s="14" t="s">
+      <c r="C82" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="D80" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E80" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="6" t="s">
+      <c r="D82" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="6" t="s">
         <v>294</v>
-      </c>
-      <c r="G80" s="21"/>
-      <c r="L80" s="21"/>
-      <c r="M80" s="17"/>
-      <c r="N80" s="17"/>
-      <c r="O80" s="17"/>
-      <c r="P80" s="17"/>
-      <c r="Q80" s="21"/>
-      <c r="R80" s="17"/>
-      <c r="S80" s="17"/>
-      <c r="T80" s="17"/>
-      <c r="U80" s="17"/>
-    </row>
-    <row r="81" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G81" s="21"/>
-      <c r="H81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="L81" s="21"/>
-      <c r="M81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="N81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="O81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="P81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q81" s="21"/>
-      <c r="R81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="S81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="T81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="U81" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G82" s="21"/>
       <c r="L82" s="21"/>
@@ -4327,49 +4338,67 @@
       <c r="T82" s="17"/>
       <c r="U82" s="17"/>
     </row>
-    <row r="83" spans="1:22" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>105</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
       <c r="D83" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F83" s="6" t="s">
-        <v>245</v>
-      </c>
       <c r="G83" s="21"/>
+      <c r="H83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K83" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="L83" s="21"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
+      <c r="M83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P83" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="Q83" s="21"/>
-      <c r="R83" s="17"/>
-      <c r="S83" s="17"/>
-      <c r="T83" s="17"/>
-      <c r="U83" s="17"/>
-      <c r="V83" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="84" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="R83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="S83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="T83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="U83" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D84" s="2" t="b">
         <v>0</v>
@@ -4392,21 +4421,24 @@
       <c r="T84" s="17"/>
       <c r="U84" s="17"/>
     </row>
-    <row r="85" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:22" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>210</v>
+        <v>104</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="D85" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E85" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>245</v>
       </c>
       <c r="G85" s="21"/>
       <c r="L85" s="21"/>
@@ -4419,28 +4451,28 @@
       <c r="S85" s="17"/>
       <c r="T85" s="17"/>
       <c r="U85" s="17"/>
-      <c r="V85" s="8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="86" spans="1:22" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="V85" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D86" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>109</v>
+        <v>16</v>
       </c>
       <c r="G86" s="21"/>
       <c r="L86" s="21"/>
@@ -4453,268 +4485,218 @@
       <c r="S86" s="17"/>
       <c r="T86" s="17"/>
       <c r="U86" s="17"/>
-      <c r="V86" s="8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="87" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="87" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>113</v>
+        <v>211</v>
       </c>
       <c r="D87" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87" s="21"/>
-      <c r="H87" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I87" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J87" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K87" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="L87" s="21"/>
-      <c r="M87" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="N87" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="O87" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="P87" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
       <c r="Q87" s="21"/>
-      <c r="R87" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="S87" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="T87" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="U87" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="V87" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="88" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A88" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D88" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" s="7" t="s">
-        <v>254</v>
+      <c r="R87" s="17"/>
+      <c r="S87" s="17"/>
+      <c r="T87" s="17"/>
+      <c r="U87" s="17"/>
+      <c r="V87" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="G88" s="21"/>
       <c r="L88" s="21"/>
+      <c r="M88" s="17"/>
+      <c r="N88" s="17"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="17"/>
       <c r="Q88" s="21"/>
-      <c r="V88" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="89" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D89" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" s="7" t="s">
+      <c r="R88" s="17"/>
+      <c r="S88" s="17"/>
+      <c r="T88" s="17"/>
+      <c r="U88" s="17"/>
+      <c r="V88" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" s="21"/>
+      <c r="H89" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I89" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J89" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K89" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="L89" s="21"/>
+      <c r="M89" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N89" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O89" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P89" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q89" s="21"/>
+      <c r="R89" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="S89" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="T89" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="U89" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="V89" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A90" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="G89" s="21"/>
-      <c r="L89" s="21"/>
-      <c r="Q89" s="21"/>
-      <c r="V89" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="90" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="G90" s="21"/>
       <c r="L90" s="21"/>
       <c r="Q90" s="21"/>
       <c r="V90" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D91" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="G91" s="21"/>
+      <c r="L91" s="21"/>
+      <c r="Q91" s="21"/>
+      <c r="V91" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D92" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="21"/>
+      <c r="L92" s="21"/>
+      <c r="Q92" s="21"/>
+      <c r="V92" s="7" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="91" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G91" s="21"/>
-      <c r="H91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L91" s="21"/>
-      <c r="M91" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N91" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O91" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P91" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q91" s="21"/>
-      <c r="R91" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="S91" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="T91" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="U91" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G92" s="21"/>
-      <c r="H92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L92" s="21"/>
-      <c r="M92" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N92" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O92" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P92" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q92" s="21"/>
-      <c r="R92" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="S92" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="T92" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="U92" s="17" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D93" s="2" t="b">
         <v>0</v>
@@ -4724,7 +4706,7 @@
       </c>
       <c r="G93" s="21"/>
       <c r="H93" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>4</v>
@@ -4737,7 +4719,7 @@
       </c>
       <c r="L93" s="21"/>
       <c r="M93" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N93" s="17" t="s">
         <v>4</v>
@@ -4750,7 +4732,7 @@
       </c>
       <c r="Q93" s="21"/>
       <c r="R93" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="S93" s="17" t="s">
         <v>4</v>
@@ -4762,28 +4744,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="D94" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E94" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G94" s="21"/>
       <c r="H94" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>4</v>
@@ -4793,10 +4775,10 @@
       </c>
       <c r="L94" s="21"/>
       <c r="M94" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N94" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O94" s="17" t="s">
         <v>4</v>
@@ -4806,10 +4788,10 @@
       </c>
       <c r="Q94" s="21"/>
       <c r="R94" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="S94" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="T94" s="17" t="s">
         <v>4</v>
@@ -4818,44 +4800,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A95" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D95" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>16</v>
+    <row r="95" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G95" s="21"/>
+      <c r="H95" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K95" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L95" s="21"/>
+      <c r="M95" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N95" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O95" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P95" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q95" s="21"/>
-      <c r="V95" s="7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="96" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R95" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S95" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="T95" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="U95" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
         <v>1</v>
@@ -4865,7 +4877,7 @@
         <v>16</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J96" s="2" t="s">
         <v>4</v>
@@ -4878,7 +4890,7 @@
         <v>16</v>
       </c>
       <c r="N96" s="17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O96" s="17" t="s">
         <v>4</v>
@@ -4891,7 +4903,7 @@
         <v>16</v>
       </c>
       <c r="S96" s="17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="T96" s="17" t="s">
         <v>4</v>
@@ -4899,147 +4911,166 @@
       <c r="U96" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="V96" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="97" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>1</v>
+    </row>
+    <row r="97" spans="1:22" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D97" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G97" s="21"/>
-      <c r="H97" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J97" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K97" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L97" s="21"/>
-      <c r="M97" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P97" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="Q97" s="21"/>
-      <c r="R97" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="S97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="T97" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="U97" s="17" t="s">
-        <v>4</v>
+      <c r="V97" s="7" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="98" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" s="21"/>
+      <c r="H98" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L98" s="21"/>
+      <c r="M98" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q98" s="21"/>
+      <c r="R98" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="T98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="U98" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="V98" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G99" s="21"/>
+      <c r="H99" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L99" s="21"/>
+      <c r="M99" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q99" s="21"/>
+      <c r="R99" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="T99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="U99" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F98" s="2" t="s">
+      <c r="D100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G98" s="21"/>
-      <c r="L98" s="21"/>
-      <c r="M98" s="17"/>
-      <c r="N98" s="17"/>
-      <c r="O98" s="17"/>
-      <c r="P98" s="17"/>
-      <c r="Q98" s="21"/>
-      <c r="R98" s="17"/>
-      <c r="S98" s="17"/>
-      <c r="T98" s="17"/>
-      <c r="U98" s="17"/>
-    </row>
-    <row r="99" spans="1:22" s="27" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A99" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="B99" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C99" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="D99" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="28" t="s">
-        <v>319</v>
-      </c>
-      <c r="G99" s="29"/>
-      <c r="H99" s="28"/>
-      <c r="I99" s="28"/>
-      <c r="J99" s="28"/>
-      <c r="K99" s="28"/>
-      <c r="L99" s="29"/>
-      <c r="M99" s="28"/>
-      <c r="N99" s="28"/>
-      <c r="O99" s="28"/>
-      <c r="P99" s="28"/>
-      <c r="Q99" s="29"/>
-      <c r="R99" s="28"/>
-    </row>
-    <row r="100" spans="1:22" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="G100" s="21"/>
       <c r="L100" s="21"/>
@@ -5052,15 +5083,72 @@
       <c r="S100" s="17"/>
       <c r="T100" s="17"/>
       <c r="U100" s="17"/>
-      <c r="V100" s="2" t="s">
+    </row>
+    <row r="101" spans="1:22" s="27" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A101" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C101" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="D101" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="G101" s="29"/>
+      <c r="H101" s="28"/>
+      <c r="I101" s="28"/>
+      <c r="J101" s="28"/>
+      <c r="K101" s="28"/>
+      <c r="L101" s="29"/>
+      <c r="M101" s="28"/>
+      <c r="N101" s="28"/>
+      <c r="O101" s="28"/>
+      <c r="P101" s="28"/>
+      <c r="Q101" s="29"/>
+      <c r="R101" s="28"/>
+    </row>
+    <row r="102" spans="1:22" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G102" s="21"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="17"/>
+      <c r="N102" s="17"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="17"/>
+      <c r="Q102" s="21"/>
+      <c r="R102" s="17"/>
+      <c r="S102" s="17"/>
+      <c r="T102" s="17"/>
+      <c r="U102" s="17"/>
+      <c r="V102" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="V101"/>
-    </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="V102"/>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.4">
       <c r="V103"/>
@@ -5121,6 +5209,12 @@
     </row>
     <row r="122" spans="22:22" x14ac:dyDescent="0.4">
       <c r="V122"/>
+    </row>
+    <row r="123" spans="22:22" x14ac:dyDescent="0.4">
+      <c r="V123"/>
+    </row>
+    <row r="124" spans="22:22" x14ac:dyDescent="0.4">
+      <c r="V124"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5128,10 +5222,10 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F21" r:id="rId1"/>

</xml_diff>

<commit_message>
Kadaster: createjson NO voor andere dan NEN3610 modellen
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -1126,7 +1126,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1201,6 +1201,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1499,11 +1502,11 @@
   </sheetPr>
   <dimension ref="A1:V124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F58" sqref="F58"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1780,16 +1783,16 @@
       <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="31" t="b">
+      <c r="D8" s="32" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
@@ -1811,10 +1814,10 @@
       </c>
     </row>
     <row r="9" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
       <c r="G9" s="21"/>
       <c r="L9" s="21"/>
       <c r="M9" s="17"/>
@@ -2596,27 +2599,27 @@
       <c r="H30" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J30" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="30" t="s">
-        <v>4</v>
+      <c r="I30" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="31" t="s">
+        <v>16</v>
       </c>
       <c r="L30" s="29"/>
-      <c r="M30" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="O30" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="P30" s="30" t="s">
-        <v>4</v>
+      <c r="M30" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="P30" s="31" t="s">
+        <v>16</v>
       </c>
       <c r="Q30" s="29"/>
       <c r="R30" s="30" t="s">
@@ -3005,16 +3008,16 @@
       </c>
     </row>
     <row r="41" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="C41" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="31" t="b">
+      <c r="D41" s="32" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="2" t="b">
@@ -3036,10 +3039,10 @@
       <c r="U41" s="17"/>
     </row>
     <row r="42" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
       <c r="G42" s="21"/>
       <c r="L42" s="21"/>
       <c r="M42" s="17"/>

</xml_diff>

<commit_message>
first step create*variant cli-parameter
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -1509,10 +1509,10 @@
   <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I82" sqref="I82"/>
+      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
create*schemavariant must have a name (Kadaster, ISO19139 or the like)
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="324">
   <si>
     <t>Name</t>
   </si>
@@ -987,19 +987,16 @@
     <t>createxmlschemavariant</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>createjsonschemavariant</t>
   </si>
   <si>
-    <t>The name of the variant of the JSON schema generated. When none specified, use the organisation name</t>
-  </si>
-  <si>
-    <t>The name of the variant of the XML schema generated. When none specified, use the organisation name</t>
-  </si>
-  <si>
     <t xml:space="preserve">KadasterNEN3610 is nog even een tijdelijke naam. </t>
+  </si>
+  <si>
+    <t>The name of the variant of the JSON schema generated.</t>
+  </si>
+  <si>
+    <t>The name of the variant of the XML schema generated.</t>
   </si>
 </sst>
 </file>
@@ -1509,10 +1506,10 @@
   <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2433,9 +2430,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B31" s="32" t="s">
         <v>10</v>
@@ -2448,6 +2445,9 @@
       </c>
       <c r="E31" s="32" t="b">
         <v>1</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>25</v>
       </c>
       <c r="G31" s="29"/>
       <c r="L31" s="29"/>
@@ -2682,7 +2682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:17" s="32" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="32" t="s">
         <v>319</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>320</v>
+        <v>25</v>
       </c>
       <c r="G39" s="29"/>
       <c r="L39" s="29"/>
@@ -3874,7 +3874,7 @@
         <v>296</v>
       </c>
       <c r="Q82" s="8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="83" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
allow-scalar-in-union is now a metamodel feature
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="325">
   <si>
     <t>Name</t>
   </si>
@@ -928,15 +928,6 @@
   </si>
   <si>
     <t>since 1.47</t>
-  </si>
-  <si>
-    <t>allowscalarinunion</t>
-  </si>
-  <si>
-    <t>Yes if scalar values may occur in unions</t>
-  </si>
-  <si>
-    <t>let op, voor ISO19136 misschien anders?</t>
   </si>
   <si>
     <t>xsdfilename</t>
@@ -1138,7 +1129,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1200,9 +1191,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1521,13 +1509,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q126"/>
+  <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M48" sqref="M48:P48"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1603,29 +1591,29 @@
       <c r="F2" s="3"/>
       <c r="G2" s="20"/>
       <c r="H2" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="L2" s="20"/>
       <c r="M2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>318</v>
       </c>
       <c r="Q2" s="5"/>
     </row>
@@ -1710,176 +1698,180 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="26" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A6" s="26" t="s">
-        <v>301</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="D6" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>16</v>
+    <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G6" s="21"/>
       <c r="L6" s="21"/>
-      <c r="Q6" s="8" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="b">
+    </row>
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="21"/>
       <c r="L7" s="21"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="2" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
-      <c r="Q8" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
+    </row>
+    <row r="9" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="G9" s="21"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-    </row>
-    <row r="10" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>16</v>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G10" s="21"/>
       <c r="L10" s="21"/>
-    </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A11" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>4</v>
+      <c r="C11" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G11" s="21"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B12" s="7" t="s">
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="b">
-        <v>1</v>
+      <c r="C12" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G12" s="21"/>
       <c r="L12" s="21"/>
-    </row>
-    <row r="13" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>4</v>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>289</v>
       </c>
       <c r="G13" s="21"/>
       <c r="L13" s="21"/>
@@ -1887,28 +1879,26 @@
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="D14" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>289</v>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G14" s="21"/>
       <c r="L14" s="21"/>
@@ -1916,17 +1906,19 @@
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
-      <c r="Q14"/>
-    </row>
-    <row r="15" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="Q14" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
@@ -1934,83 +1926,80 @@
       <c r="E15" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G15" s="21"/>
+      <c r="H15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>217</v>
+      </c>
       <c r="L15" s="21"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="M15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="P15" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G16" s="21"/>
-      <c r="H16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="L16" s="21"/>
-      <c r="M16" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="P16" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>270</v>
-      </c>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
     </row>
     <row r="17" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>256</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>266</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>265</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>10</v>
+        <v>257</v>
       </c>
       <c r="G17" s="21"/>
       <c r="L17" s="21"/>
@@ -2019,16 +2008,12 @@
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
     </row>
-    <row r="18" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>265</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="2" t="b">
         <v>1</v>
       </c>
@@ -2036,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>257</v>
+        <v>25</v>
       </c>
       <c r="G18" s="21"/>
       <c r="L18" s="21"/>
@@ -2045,20 +2030,21 @@
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
     </row>
-    <row r="19" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+        <v>170</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="D19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="G19" s="21"/>
       <c r="L19" s="21"/>
@@ -2069,19 +2055,22 @@
     </row>
     <row r="20" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="G20" s="21"/>
       <c r="L20" s="21"/>
@@ -2092,13 +2081,13 @@
     </row>
     <row r="21" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
@@ -2107,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G21" s="21"/>
       <c r="L21" s="21"/>
@@ -2116,15 +2105,15 @@
       <c r="O21" s="17"/>
       <c r="P21" s="17"/>
     </row>
-    <row r="22" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>144</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
@@ -2132,90 +2121,87 @@
       <c r="E22" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="G22" s="21"/>
+      <c r="H22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L22" s="21"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-    </row>
-    <row r="23" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="M22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2" t="b">
-        <v>1</v>
+      <c r="C23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G23" s="21"/>
-      <c r="H23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L23" s="21"/>
-      <c r="M23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N23" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O23" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P23" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="7" t="s">
+    </row>
+    <row r="24" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>16</v>
+      <c r="C24" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G24" s="21"/>
       <c r="L24" s="21"/>
-    </row>
-    <row r="25" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+    </row>
+    <row r="25" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>172</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>173</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2" t="b">
         <v>0</v>
@@ -2224,21 +2210,41 @@
         <v>1</v>
       </c>
       <c r="G25" s="21"/>
+      <c r="H25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L25" s="21"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-    </row>
-    <row r="26" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="M25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D26" s="2" t="b">
         <v>0</v>
@@ -2251,7 +2257,7 @@
         <v>16</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>4</v>
@@ -2264,7 +2270,7 @@
         <v>16</v>
       </c>
       <c r="N26" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O26" s="17" t="s">
         <v>4</v>
@@ -2273,18 +2279,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D27" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2" t="b">
         <v>1</v>
@@ -2294,7 +2300,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>4</v>
@@ -2307,7 +2313,7 @@
         <v>16</v>
       </c>
       <c r="N27" s="17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O27" s="17" t="s">
         <v>4</v>
@@ -2315,19 +2321,22 @@
       <c r="P27" s="17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Q27" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="D28" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="2" t="b">
         <v>1</v>
@@ -2337,7 +2346,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>4</v>
@@ -2350,7 +2359,7 @@
         <v>16</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O28" s="17" t="s">
         <v>4</v>
@@ -2358,160 +2367,140 @@
       <c r="P28" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q28" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    </row>
+    <row r="29" spans="1:17" s="29" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="B29" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D29" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="21"/>
-      <c r="H29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="21"/>
-      <c r="M29" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O29" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="30" t="s">
-        <v>307</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="D30" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="29"/>
-      <c r="H30" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="K30" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="L30" s="29"/>
-      <c r="M30" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="O30" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="P30" s="30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A31" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="B31" s="32" t="s">
+      <c r="C29" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="D29" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="28"/>
+      <c r="H29" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="28"/>
+      <c r="M29" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="O29" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" s="29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A30" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="B30" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="D31" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="29"/>
-      <c r="H31" s="33" t="s">
+      <c r="C30" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="D30" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="28"/>
+      <c r="H30" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="34" t="s">
+      <c r="I30" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="J31" s="34" t="s">
+      <c r="J30" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="K31" s="34" t="s">
+      <c r="K30" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="L31" s="29"/>
-      <c r="M31" s="34" t="s">
+      <c r="L30" s="28"/>
+      <c r="M30" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="N31" s="34" t="s">
+      <c r="N30" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="O31" s="34" t="s">
+      <c r="O30" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="P31" s="34" t="s">
+      <c r="P30" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="Q31" s="32" t="s">
-        <v>327</v>
+      <c r="Q30" s="31" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="2" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>175</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>37</v>
+        <v>176</v>
       </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="G32" s="21"/>
       <c r="L32" s="21"/>
@@ -2519,19 +2508,16 @@
       <c r="N32" s="17"/>
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
-      <c r="Q32" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
@@ -2548,13 +2534,13 @@
     </row>
     <row r="34" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>177</v>
+        <v>38</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>178</v>
+        <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>179</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2" t="b">
         <v>0</v>
@@ -2563,21 +2549,41 @@
         <v>1</v>
       </c>
       <c r="G34" s="21"/>
+      <c r="H34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L34" s="21"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-    </row>
-    <row r="35" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="M34" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N34" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O34" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P34" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
@@ -2612,199 +2618,181 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D36" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G36" s="21"/>
-      <c r="H36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L36" s="21"/>
-      <c r="M36" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P36" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+    </row>
+    <row r="37" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D37" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G37" s="21"/>
+      <c r="H37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L37" s="21"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-    </row>
-    <row r="38" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="M37" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P37" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A38" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="28"/>
+      <c r="H38" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J38" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K38" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="L38" s="28"/>
+      <c r="M38" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="N38" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="O38" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="P38" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q38" s="31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" s="21"/>
-      <c r="H38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L38" s="21"/>
-      <c r="M38" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O38" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P38" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A39" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="D39" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="29"/>
-      <c r="H39" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="I39" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="J39" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="K39" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="L39" s="29"/>
-      <c r="M39" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="N39" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="O39" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="P39" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="Q39" s="32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B40" s="2" t="s">
+      <c r="C39" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+    </row>
+    <row r="40" spans="1:17" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A40" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D40" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="C40" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G40" s="21"/>
       <c r="L40" s="21"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
-      <c r="O40" s="17"/>
-      <c r="P40" s="17"/>
-    </row>
-    <row r="41" spans="1:17" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="Q40" s="7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D41" s="7" t="b">
         <v>1</v>
@@ -2813,58 +2801,45 @@
         <v>0</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>16</v>
+        <v>253</v>
       </c>
       <c r="G41" s="21"/>
       <c r="L41" s="21"/>
       <c r="Q41" s="7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>253</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G42" s="21"/>
       <c r="L42" s="21"/>
-      <c r="Q42" s="7" t="s">
-        <v>271</v>
-      </c>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
     </row>
     <row r="43" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
       <c r="G43" s="21"/>
       <c r="L43" s="21"/>
       <c r="M43" s="17"/>
@@ -2872,11 +2847,22 @@
       <c r="O43" s="17"/>
       <c r="P43" s="17"/>
     </row>
-    <row r="44" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
+    <row r="44" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="G44" s="21"/>
       <c r="L44" s="21"/>
       <c r="M44" s="17"/>
@@ -2884,21 +2870,21 @@
       <c r="O44" s="17"/>
       <c r="P44" s="17"/>
     </row>
-    <row r="45" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
-        <v>182</v>
+        <v>53</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>183</v>
+        <v>5</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>184</v>
+        <v>54</v>
       </c>
       <c r="D45" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="21"/>
       <c r="L45" s="21"/>
@@ -2907,15 +2893,15 @@
       <c r="O45" s="17"/>
       <c r="P45" s="17"/>
     </row>
-    <row r="46" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D46" s="2" t="b">
         <v>0</v>
@@ -2923,90 +2909,92 @@
       <c r="E46" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="G46" s="21"/>
-      <c r="L46" s="21"/>
+      <c r="F46" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="G46" s="22"/>
+      <c r="L46" s="22"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17"/>
       <c r="P46" s="17"/>
-    </row>
-    <row r="47" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Q46" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>57</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>221</v>
+        <v>0</v>
       </c>
       <c r="G47" s="22"/>
+      <c r="H47" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="L47" s="22"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="17"/>
-      <c r="Q47" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G48" s="22"/>
-      <c r="H48" s="6" t="s">
+      <c r="M47" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I48" s="6" t="s">
+      <c r="N47" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J48" s="6" t="s">
+      <c r="O47" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K48" s="6" t="s">
+      <c r="P47" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L48" s="22"/>
-      <c r="M48" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N48" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O48" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P48" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="48" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="Q48" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>5</v>
+        <v>188</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D49" s="7" t="b">
         <v>0</v>
@@ -3015,45 +3003,46 @@
         <v>1</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="G49" s="21"/>
       <c r="L49" s="21"/>
-      <c r="Q49" s="8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>241</v>
+    </row>
+    <row r="50" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G50" s="21"/>
       <c r="L50" s="21"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
     </row>
     <row r="51" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D51" s="2" t="b">
         <v>0</v>
@@ -3071,245 +3060,248 @@
       <c r="O51" s="17"/>
       <c r="P51" s="17"/>
     </row>
-    <row r="52" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" s="2" t="s">
+    <row r="52" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A52" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D52" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
+      <c r="C52" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G52" s="21"/>
       <c r="L52" s="21"/>
-      <c r="M52" s="17"/>
-      <c r="N52" s="17"/>
-      <c r="O52" s="17"/>
-      <c r="P52" s="17"/>
-    </row>
-    <row r="53" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A53" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="7" t="s">
+      <c r="Q52" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D53" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F53" s="7" t="s">
+      <c r="C53" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G53" s="21"/>
       <c r="L53" s="21"/>
-      <c r="Q53" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D54" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>16</v>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+    </row>
+    <row r="54" spans="1:17" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A54" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D54" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="G54" s="21"/>
       <c r="L54" s="21"/>
-      <c r="M54" s="17"/>
-      <c r="N54" s="17"/>
-      <c r="O54" s="17"/>
-      <c r="P54" s="17"/>
-    </row>
-    <row r="55" spans="1:17" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A55" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D55" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G55" s="21"/>
-      <c r="L55" s="21"/>
-      <c r="Q55" s="7" t="s">
+      <c r="Q54" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A56" s="16" t="s">
+    <row r="55" spans="1:17" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A55" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B55" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C55" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="D56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="16" t="s">
+      <c r="D55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="G56" s="23"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="23"/>
-      <c r="M56" s="16"/>
-      <c r="N56" s="16"/>
-      <c r="O56" s="16"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="16" t="s">
+      <c r="G55" s="23"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="23"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="57" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
+    <row r="56" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A56" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B56" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="D56" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" s="7" t="s">
         <v>19</v>
+      </c>
+      <c r="G56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="Q56" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="G57" s="21"/>
       <c r="L57" s="21"/>
-      <c r="Q57" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>225</v>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>253</v>
       </c>
       <c r="G58" s="21"/>
       <c r="L58" s="21"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="17"/>
-      <c r="Q58" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="G59" s="21"/>
-      <c r="L59" s="21"/>
-      <c r="Q59" s="7" t="s">
+      <c r="Q58" s="7" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
-        <v>309</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="59" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>306</v>
+      </c>
+      <c r="B59" t="s">
         <v>82</v>
       </c>
-      <c r="C60" t="s">
-        <v>310</v>
-      </c>
-      <c r="D60" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="C59" t="s">
+        <v>307</v>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
         <v>263</v>
       </c>
-      <c r="G60" s="29"/>
-      <c r="L60" s="29"/>
-    </row>
-    <row r="61" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="G59" s="28"/>
+      <c r="L59" s="28"/>
+    </row>
+    <row r="60" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G60" s="21"/>
+      <c r="L60" s="21"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="17"/>
+      <c r="P60" s="17"/>
+      <c r="Q60" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>151</v>
+        <v>72</v>
       </c>
       <c r="D61" s="2" t="b">
         <v>0</v>
@@ -3318,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>242</v>
+        <v>152</v>
       </c>
       <c r="G61" s="21"/>
       <c r="L61" s="21"/>
@@ -3327,27 +3319,27 @@
       <c r="O61" s="17"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>10</v>
+        <v>198</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>72</v>
+        <v>199</v>
       </c>
       <c r="D62" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E62" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>152</v>
+        <v>229</v>
       </c>
       <c r="G62" s="21"/>
       <c r="L62" s="21"/>
@@ -3355,173 +3347,170 @@
       <c r="N62" s="17"/>
       <c r="O62" s="17"/>
       <c r="P62" s="17"/>
-      <c r="Q62" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D63" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>229</v>
+    </row>
+    <row r="63" spans="1:17" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="D63" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="25" t="s">
+        <v>298</v>
       </c>
       <c r="G63" s="21"/>
       <c r="L63" s="21"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="17"/>
-    </row>
-    <row r="64" spans="1:17" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="25" t="s">
-        <v>297</v>
-      </c>
-      <c r="B64" s="25" t="s">
+      <c r="Q63" s="25" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" s="21"/>
+      <c r="H64" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I64" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J64" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K64" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="L64" s="21"/>
+      <c r="M64" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="N64" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="O64" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="P64" s="18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C64" s="25" t="s">
-        <v>299</v>
-      </c>
-      <c r="D64" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="G64" s="21"/>
-      <c r="L64" s="21"/>
-      <c r="Q64" s="25" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C65" s="2" t="s">
-        <v>74</v>
+        <v>201</v>
       </c>
       <c r="D65" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F65" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G65" s="21"/>
-      <c r="H65" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I65" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="J65" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="K65" s="32" t="s">
-        <v>25</v>
-      </c>
       <c r="L65" s="21"/>
-      <c r="M65" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="N65" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="O65" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="P65" s="18" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B66" s="2" t="s">
+      <c r="M65" s="17"/>
+      <c r="N65" s="17"/>
+      <c r="O65" s="17"/>
+      <c r="P65" s="17"/>
+    </row>
+    <row r="66" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
+      <c r="C66" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G66" s="21"/>
       <c r="L66" s="21"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="17"/>
-    </row>
-    <row r="67" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B67" s="7" t="s">
+      <c r="Q66" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D67" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="7" t="s">
+      <c r="C67" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D67" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G67" s="21"/>
       <c r="L67" s="21"/>
-      <c r="Q67" s="7" t="s">
-        <v>230</v>
-      </c>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
     </row>
     <row r="68" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>252</v>
+        <v>77</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>267</v>
+        <v>78</v>
       </c>
       <c r="D68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G68" s="21"/>
       <c r="L68" s="21"/>
@@ -3530,433 +3519,433 @@
       <c r="O68" s="17"/>
       <c r="P68" s="17"/>
     </row>
-    <row r="69" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D69" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="G69" s="21"/>
+      <c r="H69" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I69" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J69" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K69" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="L69" s="21"/>
-      <c r="M69" s="17"/>
-      <c r="N69" s="17"/>
-      <c r="O69" s="17"/>
-      <c r="P69" s="17"/>
-    </row>
-    <row r="70" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="M69" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="N69" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="O69" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="P69" s="18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G70" s="21"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="17"/>
+      <c r="N70" s="17"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="17"/>
+    </row>
+    <row r="71" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D70" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G70" s="21"/>
-      <c r="H70" s="17" t="s">
+      <c r="C71" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D71" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="I70" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J70" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K70" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="L70" s="21"/>
-      <c r="M70" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="N70" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="O70" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="P70" s="18" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="G71" s="21"/>
       <c r="L71" s="21"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-    </row>
-    <row r="72" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D72" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>25</v>
+      <c r="Q71" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G72" s="21"/>
       <c r="L72" s="21"/>
-      <c r="Q72" s="7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>19</v>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
+    </row>
+    <row r="73" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A73" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D73" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="G73" s="21"/>
       <c r="L73" s="21"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
-    </row>
-    <row r="74" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A74" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D74" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>243</v>
+      <c r="Q73" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D74" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G74" s="21"/>
+      <c r="H74" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J74" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K74" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="L74" s="21"/>
-      <c r="Q74" s="8" t="s">
-        <v>231</v>
+      <c r="M74" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="N74" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="O74" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="P74" s="17" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E75" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="G75" s="21"/>
-      <c r="H75" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J75" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="K75" s="17" t="s">
-        <v>87</v>
-      </c>
       <c r="L75" s="21"/>
-      <c r="M75" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="N75" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="O75" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="P75" s="17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>90</v>
+      <c r="M75" s="17"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
+    </row>
+    <row r="76" spans="1:17" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A76" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D76" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="G76" s="21"/>
       <c r="L76" s="21"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
-    </row>
-    <row r="77" spans="1:17" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="Q76" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A77" s="7" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="D77" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E77" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="G77" s="21"/>
       <c r="L77" s="21"/>
-      <c r="Q77" s="8" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A78" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D78" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>16</v>
+      <c r="Q77" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A78" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D78" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="G78" s="21"/>
       <c r="L78" s="21"/>
-      <c r="Q78" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
+    </row>
+    <row r="79" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>99</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
       <c r="D79" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>98</v>
+        <v>1</v>
       </c>
       <c r="G79" s="21"/>
+      <c r="H79" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L79" s="21"/>
-      <c r="M79" s="17"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
-    </row>
-    <row r="80" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="M79" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N79" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O79" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P79" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
+        <v>156</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="D80" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F80" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G80" s="21"/>
-      <c r="H80" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J80" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L80" s="21"/>
-      <c r="M80" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N80" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O80" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P80" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G81" s="21"/>
-      <c r="L81" s="21"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
+      <c r="Q80" s="8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D81" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="G81" s="28"/>
+      <c r="L81" s="28"/>
       <c r="Q81" s="8" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" s="33" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A82" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="B82" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D82" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="33" t="s">
-        <v>324</v>
-      </c>
-      <c r="G82" s="29"/>
-      <c r="L82" s="29"/>
-      <c r="Q82" s="8" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="12" t="s">
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="12" t="s">
         <v>294</v>
+      </c>
+      <c r="G82" s="21"/>
+      <c r="L82" s="21"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
+    </row>
+    <row r="83" spans="1:17" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A83" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="D83" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>293</v>
       </c>
       <c r="G83" s="21"/>
       <c r="L83" s="21"/>
@@ -3965,80 +3954,80 @@
       <c r="O83" s="17"/>
       <c r="P83" s="17"/>
     </row>
-    <row r="84" spans="1:17" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A84" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="D84" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>293</v>
+    <row r="84" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G84" s="21"/>
+      <c r="H84" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I84" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J84" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K84" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="L84" s="21"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
-    </row>
-    <row r="85" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="M84" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N84" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O84" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P84" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="D85" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F85" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G85" s="21"/>
-      <c r="H85" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I85" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J85" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K85" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="L85" s="21"/>
-      <c r="M85" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="N85" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="O85" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="P85" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
+    </row>
+    <row r="86" spans="1:17" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D86" s="2" t="b">
         <v>0</v>
@@ -4046,8 +4035,8 @@
       <c r="E86" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>16</v>
+      <c r="F86" s="6" t="s">
+        <v>244</v>
       </c>
       <c r="G86" s="21"/>
       <c r="L86" s="21"/>
@@ -4055,16 +4044,19 @@
       <c r="N86" s="17"/>
       <c r="O86" s="17"/>
       <c r="P86" s="17"/>
-    </row>
-    <row r="87" spans="1:17" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="Q86" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D87" s="2" t="b">
         <v>0</v>
@@ -4072,8 +4064,8 @@
       <c r="E87" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F87" s="6" t="s">
-        <v>244</v>
+      <c r="F87" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G87" s="21"/>
       <c r="L87" s="21"/>
@@ -4081,28 +4073,22 @@
       <c r="N87" s="17"/>
       <c r="O87" s="17"/>
       <c r="P87" s="17"/>
-      <c r="Q87" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="88" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>107</v>
+        <v>211</v>
       </c>
       <c r="D88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E88" s="2" t="b">
         <v>1</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G88" s="21"/>
       <c r="L88" s="21"/>
@@ -4110,22 +4096,28 @@
       <c r="N88" s="17"/>
       <c r="O88" s="17"/>
       <c r="P88" s="17"/>
-    </row>
-    <row r="89" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Q88" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
-        <v>210</v>
+        <v>108</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>211</v>
+        <v>111</v>
       </c>
       <c r="D89" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E89" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="G89" s="21"/>
       <c r="L89" s="21"/>
@@ -4134,18 +4126,18 @@
       <c r="O89" s="17"/>
       <c r="P89" s="17"/>
       <c r="Q89" s="8" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D90" s="2" t="b">
         <v>1</v>
@@ -4153,74 +4145,70 @@
       <c r="E90" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F90" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G90" s="21"/>
+      <c r="H90" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I90" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J90" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K90" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="L90" s="21"/>
-      <c r="M90" s="17"/>
-      <c r="N90" s="17"/>
-      <c r="O90" s="17"/>
-      <c r="P90" s="17"/>
-      <c r="Q90" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>0</v>
+      <c r="M90" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="N90" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="O90" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="P90" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q90" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A91" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D91" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>253</v>
       </c>
       <c r="G91" s="21"/>
-      <c r="H91" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I91" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J91" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K91" s="17" t="s">
-        <v>25</v>
-      </c>
       <c r="L91" s="21"/>
-      <c r="M91" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="N91" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="O91" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="P91" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="Q91" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="Q91" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A92" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D92" s="7" t="b">
         <v>1</v>
@@ -4234,71 +4222,89 @@
       <c r="G92" s="21"/>
       <c r="L92" s="21"/>
       <c r="Q92" s="7" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A93" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D93" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E93" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>253</v>
+        <v>16</v>
       </c>
       <c r="G93" s="21"/>
       <c r="L93" s="21"/>
       <c r="Q93" s="7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B94" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C94" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D94" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>16</v>
+      <c r="C94" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D94" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G94" s="21"/>
+      <c r="H94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L94" s="21"/>
-      <c r="Q94" s="7" t="s">
-        <v>238</v>
+      <c r="M94" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N94" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O94" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P94" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D95" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
@@ -4332,23 +4338,23 @@
     </row>
     <row r="96" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G96" s="21"/>
       <c r="H96" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>4</v>
@@ -4361,7 +4367,7 @@
       </c>
       <c r="L96" s="21"/>
       <c r="M96" s="17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="N96" s="17" t="s">
         <v>4</v>
@@ -4373,15 +4379,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="D97" s="2" t="b">
         <v>0</v>
@@ -4394,7 +4400,7 @@
         <v>16</v>
       </c>
       <c r="I97" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J97" s="2" t="s">
         <v>4</v>
@@ -4407,7 +4413,7 @@
         <v>16</v>
       </c>
       <c r="N97" s="17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O97" s="17" t="s">
         <v>4</v>
@@ -4416,83 +4422,86 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B98" s="2" t="s">
+    <row r="98" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D98" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" s="21"/>
+      <c r="L98" s="21"/>
+      <c r="Q98" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D98" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G98" s="21"/>
-      <c r="H98" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K98" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L98" s="21"/>
-      <c r="M98" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N98" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O98" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P98" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A99" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D99" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>16</v>
+      <c r="C99" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G99" s="21"/>
+      <c r="H99" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K99" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L99" s="21"/>
-      <c r="Q99" s="7" t="s">
-        <v>245</v>
+      <c r="M99" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P99" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q99" s="2" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="100" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>129</v>
+        <v>280</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D100" s="2" t="b">
         <v>1</v>
@@ -4526,134 +4535,91 @@
       <c r="P100" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q100" s="2" t="s">
-        <v>214</v>
-      </c>
     </row>
     <row r="101" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>280</v>
+        <v>132</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D101" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E101" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="G101" s="21"/>
-      <c r="H101" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="L101" s="21"/>
-      <c r="M101" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P101" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G102" s="21"/>
-      <c r="L102" s="21"/>
-      <c r="M102" s="17"/>
-      <c r="N102" s="17"/>
-      <c r="O102" s="17"/>
-      <c r="P102" s="17"/>
-    </row>
-    <row r="103" spans="1:17" s="27" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A103" s="28" t="s">
-        <v>304</v>
-      </c>
-      <c r="B103" s="28" t="s">
+      <c r="M101" s="17"/>
+      <c r="N101" s="17"/>
+      <c r="O101" s="17"/>
+      <c r="P101" s="17"/>
+    </row>
+    <row r="102" spans="1:17" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A102" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="B102" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C103" s="28" t="s">
-        <v>305</v>
-      </c>
-      <c r="D103" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F103" s="28" t="s">
-        <v>306</v>
-      </c>
-      <c r="G103" s="29"/>
-      <c r="H103" s="28"/>
-      <c r="I103" s="28"/>
-      <c r="J103" s="28"/>
-      <c r="K103" s="28"/>
-      <c r="L103" s="29"/>
-      <c r="M103" s="28"/>
-    </row>
-    <row r="104" spans="1:17" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A104" s="2" t="s">
+      <c r="C102" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="D102" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" s="27" t="s">
+        <v>303</v>
+      </c>
+      <c r="G102" s="28"/>
+      <c r="H102" s="27"/>
+      <c r="I102" s="27"/>
+      <c r="J102" s="27"/>
+      <c r="K102" s="27"/>
+      <c r="L102" s="28"/>
+      <c r="M102" s="27"/>
+    </row>
+    <row r="103" spans="1:17" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" s="2" t="s">
+      <c r="D103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="G104" s="21"/>
-      <c r="L104" s="21"/>
-      <c r="M104" s="17"/>
-      <c r="N104" s="17"/>
-      <c r="O104" s="17"/>
-      <c r="P104" s="17"/>
-      <c r="Q104" s="2" t="s">
+      <c r="G103" s="21"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="17"/>
+      <c r="N103" s="17"/>
+      <c r="O103" s="17"/>
+      <c r="P103" s="17"/>
+      <c r="Q103" s="2" t="s">
         <v>261</v>
       </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="Q104"/>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.4">
       <c r="Q105"/>
@@ -4718,23 +4684,20 @@
     <row r="125" spans="17:17" x14ac:dyDescent="0.4">
       <c r="Q125"/>
     </row>
-    <row r="126" spans="17:17" x14ac:dyDescent="0.4">
-      <c r="Q126"/>
-    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F21" r:id="rId1"/>
-    <hyperlink ref="F22" r:id="rId2"/>
+    <hyperlink ref="F20" r:id="rId1"/>
+    <hyperlink ref="F21" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId3"/>

</xml_diff>

<commit_message>
Kadaster corrections on Respec
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="330">
   <si>
     <t>Name</t>
   </si>
@@ -1012,6 +1012,9 @@
   </si>
   <si>
     <t>respec msword</t>
+  </si>
+  <si>
+    <t>Kadaster-compact</t>
   </si>
 </sst>
 </file>
@@ -1527,10 +1530,10 @@
   <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34:XFD34"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2959,7 +2962,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:17" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>254</v>
       </c>
@@ -2973,16 +2976,16 @@
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="6" t="s">
-        <v>25</v>
+        <v>329</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>25</v>
+        <v>329</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>25</v>
+        <v>329</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>25</v>
+        <v>329</v>
       </c>
       <c r="L48" s="22"/>
       <c r="M48" s="6" t="s">

</xml_diff>

<commit_message>
Kadaster: toegevoegd Uitleg/Explanation en documentatie report aangepast.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="347">
   <si>
     <t>Name</t>
   </si>
@@ -1308,10 +1308,10 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1606,10 +1606,10 @@
   <dimension ref="A1:S132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomRight" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1819,16 +1819,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="37" t="b">
+      <c r="D7" s="38" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1846,10 +1846,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -2993,16 +2993,16 @@
       </c>
     </row>
     <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="37" t="b">
+      <c r="D44" s="38" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
@@ -3020,10 +3020,10 @@
       <c r="Q44" s="28"/>
     </row>
     <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
+      <c r="A45" s="38"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
       <c r="G45" s="21"/>
       <c r="L45" s="21"/>
       <c r="M45" s="17"/>
@@ -3071,6 +3071,9 @@
       </c>
       <c r="E47" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="G47" s="21"/>
       <c r="L47" s="21"/>
@@ -3377,19 +3380,19 @@
       <c r="E58" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F58" s="38" t="s">
+      <c r="F58" s="37" t="s">
         <v>345</v>
       </c>
       <c r="G58" s="28"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="38"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
       <c r="L58" s="28"/>
-      <c r="M58" s="38"/>
-      <c r="N58" s="38"/>
-      <c r="O58" s="38"/>
-      <c r="P58" s="38"/>
+      <c r="M58" s="37"/>
+      <c r="N58" s="37"/>
+      <c r="O58" s="37"/>
+      <c r="P58" s="37"/>
       <c r="Q58" s="28"/>
     </row>
     <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Kadaster: GML 3.2.2 vervangt 3.2.1, plus voorbereiding op kadaster profiel
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="349">
   <si>
     <t>Name</t>
   </si>
@@ -483,9 +483,6 @@
     <t>Language of the metamodel and model. Specify metamodel:model, like "en:nl", or single code for both.</t>
   </si>
   <si>
-    <t>NEN3610_GML321_ENV</t>
-  </si>
-  <si>
     <t>[project-name]-[application-name]-[phase]-[release].office</t>
   </si>
   <si>
@@ -873,9 +870,6 @@
     <t>The GML version to be used for ISO19136 schemas. Example: "3.3".</t>
   </si>
   <si>
-    <t>3.2.1</t>
-  </si>
-  <si>
     <t>Standaard op 3.2.1 gezet.</t>
   </si>
   <si>
@@ -1072,6 +1066,12 @@
   </si>
   <si>
     <t>Generate schemas with IDs with domains. This parameter applies to Kadaster schemas.</t>
+  </si>
+  <si>
+    <t>NEN3610_GML322_ENV</t>
+  </si>
+  <si>
+    <t>3.2.2</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1216,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1315,6 +1315,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1618,10 +1621,10 @@
   <dimension ref="A1:S133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C63" sqref="C63"/>
+      <selection pane="bottomRight" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1656,85 +1659,85 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>247</v>
       </c>
       <c r="G1" s="19"/>
       <c r="H1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L1" s="19"/>
       <c r="M1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="Q1" s="19"/>
       <c r="R1" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="3"/>
       <c r="G2" s="20"/>
       <c r="H2" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="L2" s="20"/>
       <c r="M2" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1777,7 +1780,7 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="28"/>
       <c r="R4" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -1807,18 +1810,18 @@
       <c r="P5" s="17"/>
       <c r="Q5" s="28"/>
       <c r="R5" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="D6" s="7" t="b">
         <v>0</v>
@@ -1831,16 +1834,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="40" t="b">
+      <c r="D7" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1854,14 +1857,14 @@
       <c r="P7" s="17"/>
       <c r="Q7" s="28"/>
       <c r="R7" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -1872,13 +1875,13 @@
     </row>
     <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D9" s="7" t="b">
         <v>0</v>
@@ -1920,18 +1923,18 @@
       <c r="P10" s="17"/>
       <c r="Q10" s="28"/>
       <c r="R10" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>0</v>
@@ -1970,27 +1973,27 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="28"/>
       <c r="R12" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="D13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>285</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="D13" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>287</v>
       </c>
       <c r="G13" s="21"/>
       <c r="L13" s="21"/>
@@ -2028,7 +2031,7 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="28"/>
       <c r="R14" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -2055,10 +2058,10 @@
         <v>19</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="17" t="s">
@@ -2068,14 +2071,14 @@
         <v>19</v>
       </c>
       <c r="O15" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P15" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q15" s="28"/>
       <c r="R15" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2107,22 +2110,22 @@
     </row>
     <row r="17" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="G17" s="21"/>
       <c r="L17" s="21"/>
@@ -2134,7 +2137,7 @@
     </row>
     <row r="18" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2157,13 +2160,13 @@
     </row>
     <row r="19" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
@@ -2302,13 +2305,13 @@
     </row>
     <row r="24" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>
@@ -2456,7 +2459,7 @@
       </c>
       <c r="Q27" s="28"/>
       <c r="R27" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -2505,13 +2508,13 @@
     </row>
     <row r="29" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="29" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D29" s="29" t="b">
         <v>0</v>
@@ -2549,13 +2552,13 @@
     </row>
     <row r="30" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A30" s="31" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D30" s="31" t="b">
         <v>0</v>
@@ -2591,7 +2594,7 @@
       </c>
       <c r="Q30" s="28"/>
       <c r="R30" s="31" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2621,18 +2624,18 @@
       <c r="P31" s="17"/>
       <c r="Q31" s="28"/>
       <c r="R31" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
@@ -2650,13 +2653,13 @@
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
@@ -2674,22 +2677,22 @@
     </row>
     <row r="34" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="C34" s="34" t="s">
         <v>323</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="D34" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" s="34" t="s">
         <v>324</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>325</v>
-      </c>
-      <c r="D34" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>326</v>
       </c>
       <c r="G34" s="28"/>
       <c r="L34" s="28"/>
@@ -2741,13 +2744,13 @@
     </row>
     <row r="36" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="35" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B36" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D36" s="35" t="b">
         <v>0</v>
@@ -2880,13 +2883,13 @@
     </row>
     <row r="40" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A40" s="31" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B40" s="31" t="s">
         <v>10</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D40" s="31" t="b">
         <v>0</v>
@@ -2909,31 +2912,31 @@
       </c>
       <c r="L40" s="28"/>
       <c r="M40" s="31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="N40" s="32" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O40" s="32" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P40" s="32" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="Q40" s="28"/>
       <c r="R40" s="31" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D41" s="2" t="b">
         <v>0</v>
@@ -2975,7 +2978,7 @@
       <c r="L42" s="21"/>
       <c r="Q42" s="28"/>
       <c r="R42" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2995,26 +2998,26 @@
         <v>0</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G43" s="21"/>
       <c r="L43" s="21"/>
       <c r="Q43" s="28"/>
       <c r="R43" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="40" t="s">
+      <c r="C44" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="40" t="b">
+      <c r="D44" s="41" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="2" t="b">
@@ -3032,10 +3035,10 @@
       <c r="Q44" s="28"/>
     </row>
     <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
       <c r="G45" s="21"/>
       <c r="L45" s="21"/>
       <c r="M45" s="17"/>
@@ -3046,13 +3049,13 @@
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="D46" s="2" t="b">
         <v>0</v>
@@ -3112,7 +3115,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G48" s="22"/>
       <c r="L48" s="22"/>
@@ -3122,12 +3125,12 @@
       <c r="P48" s="17"/>
       <c r="Q48" s="28"/>
       <c r="R48" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -3139,16 +3142,16 @@
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L49" s="22"/>
       <c r="M49" s="6" t="s">
@@ -3167,13 +3170,13 @@
     </row>
     <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D50" s="7" t="b">
         <v>0</v>
@@ -3188,19 +3191,19 @@
       <c r="L50" s="21"/>
       <c r="Q50" s="28"/>
       <c r="R50" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>189</v>
-      </c>
       <c r="D51" s="7" t="b">
         <v>0</v>
       </c>
@@ -3208,7 +3211,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G51" s="21"/>
       <c r="L51" s="21"/>
@@ -3291,18 +3294,18 @@
       <c r="L54" s="21"/>
       <c r="Q54" s="28"/>
       <c r="R54" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D55" s="2" t="b">
         <v>0</v>
@@ -3323,13 +3326,13 @@
     </row>
     <row r="56" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A56" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B56" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D56" s="16" t="b">
         <v>0</v>
@@ -3338,7 +3341,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G56" s="23"/>
       <c r="H56" s="16"/>
@@ -3355,22 +3358,22 @@
     </row>
     <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="D57" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="7" t="s">
         <v>339</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>341</v>
       </c>
       <c r="G57" s="28"/>
       <c r="L57" s="28"/>
@@ -3378,13 +3381,13 @@
     </row>
     <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D58" s="7" t="b">
         <v>0</v>
@@ -3393,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="37" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G58" s="28"/>
       <c r="H58" s="37"/>
@@ -3409,14 +3412,14 @@
     </row>
     <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>193</v>
-      </c>
       <c r="D59" s="7" t="b">
         <v>0</v>
       </c>
@@ -3424,7 +3427,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G59" s="28"/>
       <c r="L59" s="28"/>
@@ -3432,14 +3435,14 @@
     </row>
     <row r="60" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="C60" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="C60" s="15" t="s">
-        <v>281</v>
-      </c>
       <c r="D60" s="16" t="b">
         <v>0</v>
       </c>
@@ -3447,7 +3450,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>282</v>
+        <v>348</v>
       </c>
       <c r="G60" s="23"/>
       <c r="H60" s="16"/>
@@ -3461,18 +3464,18 @@
       <c r="P60" s="16"/>
       <c r="Q60" s="23"/>
       <c r="R60" s="16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="D61" s="7" t="b">
         <v>0</v>
@@ -3487,7 +3490,7 @@
       <c r="L61" s="21"/>
       <c r="Q61" s="28"/>
       <c r="R61" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -3507,7 +3510,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G62" s="21"/>
       <c r="L62" s="21"/>
@@ -3517,18 +3520,18 @@
       <c r="P62" s="17"/>
       <c r="Q62" s="28"/>
       <c r="R62" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:18" s="39" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B63" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D63" s="39" t="b">
         <v>0</v>
@@ -3536,33 +3539,11 @@
       <c r="E63" t="b">
         <v>1</v>
       </c>
-      <c r="F63"/>
+      <c r="F63" s="40" t="s">
+        <v>4</v>
+      </c>
       <c r="G63" s="28"/>
-      <c r="H63" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="I63" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="J63" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="K63" s="39" t="s">
-        <v>16</v>
-      </c>
       <c r="L63" s="28"/>
-      <c r="M63" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="N63" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="O63" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="P63" s="39" t="s">
-        <v>4</v>
-      </c>
       <c r="Q63" s="28"/>
     </row>
     <row r="64" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3582,24 +3563,24 @@
         <v>0</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G64" s="21"/>
       <c r="L64" s="21"/>
       <c r="Q64" s="28"/>
       <c r="R64" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B65" t="s">
         <v>82</v>
       </c>
       <c r="C65" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -3608,7 +3589,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G65" s="28"/>
       <c r="L65" s="28"/>
@@ -3631,7 +3612,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G66" s="21"/>
       <c r="L66" s="21"/>
@@ -3641,7 +3622,7 @@
       <c r="P66" s="17"/>
       <c r="Q66" s="28"/>
       <c r="R66" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -3661,7 +3642,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>152</v>
+        <v>347</v>
       </c>
       <c r="G67" s="21"/>
       <c r="L67" s="21"/>
@@ -3671,19 +3652,19 @@
       <c r="P67" s="17"/>
       <c r="Q67" s="28"/>
       <c r="R67" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
       </c>
@@ -3691,7 +3672,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G68" s="21"/>
       <c r="L68" s="21"/>
@@ -3703,13 +3684,13 @@
     </row>
     <row r="69" spans="1:18" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" s="25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B69" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D69" s="25" t="b">
         <v>0</v>
@@ -3718,13 +3699,13 @@
         <v>1</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G69" s="21"/>
       <c r="L69" s="21"/>
       <c r="Q69" s="28"/>
       <c r="R69" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="70" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -3758,28 +3739,28 @@
       </c>
       <c r="L70" s="21"/>
       <c r="M70" s="17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N70" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="O70" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="P70" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q70" s="28"/>
     </row>
     <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" s="38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B71" s="38" t="s">
         <v>10</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D71" s="38" t="b">
         <v>0</v>
@@ -3819,18 +3800,18 @@
       <c r="L72" s="21"/>
       <c r="Q72" s="28"/>
       <c r="R72" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>1</v>
@@ -3907,16 +3888,16 @@
       </c>
       <c r="L75" s="21"/>
       <c r="M75" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N75" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="O75" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="P75" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q75" s="28"/>
     </row>
@@ -3937,7 +3918,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G76" s="21"/>
       <c r="L76" s="21"/>
@@ -3970,18 +3951,18 @@
       <c r="L77" s="21"/>
       <c r="Q77" s="28"/>
       <c r="R77" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
@@ -4002,14 +3983,14 @@
     </row>
     <row r="79" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A79" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B79" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>205</v>
-      </c>
       <c r="D79" s="7" t="b">
         <v>0</v>
       </c>
@@ -4017,13 +3998,13 @@
         <v>1</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G79" s="21"/>
       <c r="L79" s="21"/>
       <c r="Q79" s="28"/>
       <c r="R79" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -4057,16 +4038,16 @@
       </c>
       <c r="L80" s="21"/>
       <c r="M80" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N80" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O80" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P80" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q80" s="28"/>
     </row>
@@ -4120,18 +4101,18 @@
       <c r="L82" s="21"/>
       <c r="Q82" s="28"/>
       <c r="R82" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="83" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D83" s="7" t="b">
         <v>0</v>
@@ -4146,7 +4127,7 @@
       <c r="L83" s="21"/>
       <c r="Q83" s="28"/>
       <c r="R83" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
@@ -4178,7 +4159,7 @@
     </row>
     <row r="85" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
@@ -4218,13 +4199,13 @@
     </row>
     <row r="86" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D86" s="2" t="b">
         <v>0</v>
@@ -4243,7 +4224,7 @@
       <c r="P86" s="17"/>
       <c r="Q86" s="28"/>
       <c r="R86" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:19" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4263,25 +4244,25 @@
         <v>0</v>
       </c>
       <c r="F87" s="32" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G87" s="28"/>
       <c r="L87" s="28"/>
       <c r="Q87" s="28"/>
       <c r="R87" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="88" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="D88" s="2" t="b">
         <v>0</v>
       </c>
@@ -4289,7 +4270,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G88" s="21"/>
       <c r="L88" s="21"/>
@@ -4301,22 +4282,22 @@
     </row>
     <row r="89" spans="1:19" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C89" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="D89" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="6" t="s">
         <v>289</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="D89" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>291</v>
       </c>
       <c r="G89" s="21"/>
       <c r="L89" s="21"/>
@@ -4328,13 +4309,13 @@
     </row>
     <row r="90" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B90" t="s">
         <v>10</v>
       </c>
       <c r="C90" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D90" s="2" t="b">
         <v>1</v>
@@ -4359,13 +4340,13 @@
     </row>
     <row r="91" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
       </c>
       <c r="C91" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D91" t="b">
         <v>1</v>
@@ -4426,7 +4407,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G93" s="21"/>
       <c r="L93" s="21"/>
@@ -4436,7 +4417,7 @@
       <c r="P93" s="17"/>
       <c r="Q93" s="28"/>
       <c r="R93" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4468,13 +4449,13 @@
     </row>
     <row r="95" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
@@ -4490,7 +4471,7 @@
       <c r="P95" s="17"/>
       <c r="Q95" s="28"/>
       <c r="R95" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="96" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
@@ -4520,7 +4501,7 @@
       <c r="P96" s="17"/>
       <c r="Q96" s="28"/>
       <c r="R96" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="97" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4554,20 +4535,20 @@
       </c>
       <c r="L97" s="21"/>
       <c r="M97" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="N97" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="O97" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="P97" s="18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q97" s="28"/>
       <c r="R97" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="98" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -4587,13 +4568,13 @@
         <v>0</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G98" s="21"/>
       <c r="L98" s="21"/>
       <c r="Q98" s="28"/>
       <c r="R98" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -4613,13 +4594,13 @@
         <v>0</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G99" s="21"/>
       <c r="L99" s="21"/>
       <c r="Q99" s="28"/>
       <c r="R99" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="100" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -4645,7 +4626,7 @@
       <c r="L100" s="21"/>
       <c r="Q100" s="28"/>
       <c r="R100" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="101" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -4782,13 +4763,13 @@
     </row>
     <row r="104" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D104" s="2" t="b">
         <v>0</v>
@@ -4809,13 +4790,13 @@
     </row>
     <row r="105" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B105" t="s">
         <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D105" t="b">
         <v>0</v>
@@ -4863,7 +4844,7 @@
       <c r="L106" s="21"/>
       <c r="Q106" s="28"/>
       <c r="R106" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -4910,12 +4891,12 @@
       </c>
       <c r="Q107" s="28"/>
       <c r="R107" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
@@ -4986,13 +4967,13 @@
     </row>
     <row r="110" spans="1:19" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A110" s="27" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B110" s="27" t="s">
         <v>82</v>
       </c>
       <c r="C110" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D110" s="27" t="b">
         <v>1</v>
@@ -5001,7 +4982,7 @@
         <v>1</v>
       </c>
       <c r="F110" s="27" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G110" s="28"/>
       <c r="H110" s="27"/>
@@ -5029,7 +5010,7 @@
         <v>0</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G111" s="21"/>
       <c r="L111" s="21"/>
@@ -5039,7 +5020,7 @@
       <c r="P111" s="17"/>
       <c r="Q111" s="28"/>
       <c r="R111" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.4">
@@ -5145,48 +5126,48 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Kadaster: Default cli parameter Creategmlprofile gezet (no)
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="351">
   <si>
     <t>Name</t>
   </si>
@@ -1068,10 +1068,16 @@
     <t>Generate schemas with IDs with domains. This parameter applies to Kadaster schemas.</t>
   </si>
   <si>
-    <t>NEN3610_GML322_ENV</t>
-  </si>
-  <si>
     <t>3.2.2</t>
+  </si>
+  <si>
+    <t>NEN3610_GML322PROFILE_ENV</t>
+  </si>
+  <si>
+    <t>creategmlprofile</t>
+  </si>
+  <si>
+    <t>Generate a GML profile for the model from XSD files configured. Only avaiable for GML 3.2.2.</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1222,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1315,6 +1321,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1618,13 +1627,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S133"/>
+  <dimension ref="A1:S134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1834,16 +1843,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="41" t="b">
+      <c r="D7" s="42" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1861,10 +1870,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -2415,65 +2424,41 @@
       </c>
       <c r="Q26" s="28"/>
     </row>
-    <row r="27" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:18" s="41" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A27" s="41" t="s">
+        <v>349</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>350</v>
+      </c>
+      <c r="D27" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="Q27" s="28"/>
+    </row>
+    <row r="28" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" s="21"/>
-      <c r="H27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L27" s="21"/>
-      <c r="M27" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P27" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="8" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="D28" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="b">
         <v>1</v>
@@ -2483,7 +2468,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>4</v>
@@ -2496,7 +2481,7 @@
         <v>16</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O28" s="17" t="s">
         <v>4</v>
@@ -2505,143 +2490,163 @@
         <v>4</v>
       </c>
       <c r="Q28" s="28"/>
-    </row>
-    <row r="29" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="29" t="s">
+      <c r="R28" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="21"/>
+      <c r="H29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="21"/>
+      <c r="M29" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="28"/>
+    </row>
+    <row r="30" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B30" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C30" s="29" t="s">
         <v>301</v>
       </c>
-      <c r="D29" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="K29" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="L29" s="28"/>
-      <c r="M29" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="O29" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q29" s="28"/>
-    </row>
-    <row r="30" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A30" s="31" t="s">
+      <c r="D30" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="28"/>
+      <c r="H30" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" s="28"/>
+      <c r="M30" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="O30" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="28"/>
+    </row>
+    <row r="31" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A31" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B31" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C31" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="D30" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="32" t="s">
+      <c r="D31" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="28"/>
+      <c r="H31" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="I30" s="33" t="s">
+      <c r="I31" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="J30" s="33" t="s">
+      <c r="J31" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="33" t="s">
+      <c r="K31" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="L30" s="28"/>
-      <c r="M30" s="33" t="s">
+      <c r="L31" s="28"/>
+      <c r="M31" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="N30" s="33" t="s">
+      <c r="N31" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="O30" s="33" t="s">
+      <c r="O31" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="P30" s="33" t="s">
+      <c r="P31" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="31" t="s">
+      <c r="Q31" s="28"/>
+      <c r="R31" s="31" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>173</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>174</v>
+        <v>36</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>175</v>
+        <v>37</v>
       </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="G32" s="21"/>
       <c r="L32" s="21"/>
@@ -2650,16 +2655,19 @@
       <c r="O32" s="17"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="28"/>
-    </row>
-    <row r="33" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R32" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
@@ -2675,321 +2683,319 @@
       <c r="P33" s="17"/>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="34" t="s">
+    <row r="34" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="28"/>
+    </row>
+    <row r="35" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A35" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B35" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C35" s="34" t="s">
         <v>323</v>
       </c>
-      <c r="D34" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="34" t="s">
+      <c r="D35" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="34" t="s">
         <v>324</v>
       </c>
-      <c r="G34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="Q34" s="28"/>
-    </row>
-    <row r="35" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="2" t="s">
+      <c r="G35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="Q35" s="28"/>
+    </row>
+    <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" s="21"/>
-      <c r="H35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L35" s="21"/>
-      <c r="M35" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N35" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O35" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P35" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q35" s="28"/>
-    </row>
-    <row r="36" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="35" t="s">
+      <c r="D36" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="21"/>
+      <c r="H36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L36" s="21"/>
+      <c r="M36" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N36" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O36" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P36" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q36" s="28"/>
+    </row>
+    <row r="37" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B37" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C37" s="35" t="s">
         <v>327</v>
       </c>
-      <c r="D36" s="35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="Q36" s="28"/>
-      <c r="R36"/>
-    </row>
-    <row r="37" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
+      <c r="D37" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="36"/>
+      <c r="L37" s="36"/>
+      <c r="Q37" s="28"/>
+      <c r="R37"/>
+    </row>
+    <row r="38" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" s="21"/>
-      <c r="H37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L37" s="21"/>
-      <c r="M37" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N37" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O37" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P37" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q37" s="28"/>
-    </row>
-    <row r="38" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D38" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G38" s="21"/>
+      <c r="H38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L38" s="21"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17"/>
+      <c r="M38" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P38" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q38" s="28"/>
     </row>
-    <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="28"/>
+    </row>
+    <row r="40" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="21"/>
-      <c r="H39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L39" s="21"/>
-      <c r="M39" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P39" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q39" s="28"/>
-    </row>
-    <row r="40" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A40" s="31" t="s">
+      <c r="D40" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="21"/>
+      <c r="H40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L40" s="21"/>
+      <c r="M40" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O40" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P40" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q40" s="28"/>
+    </row>
+    <row r="41" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A41" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B41" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C41" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="D40" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="28"/>
-      <c r="H40" s="31" t="s">
+      <c r="D41" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="28"/>
+      <c r="H41" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="I40" s="33" t="s">
+      <c r="I41" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="33" t="s">
+      <c r="J41" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="K40" s="33" t="s">
+      <c r="K41" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="L40" s="28"/>
-      <c r="M40" s="31" t="s">
+      <c r="L41" s="28"/>
+      <c r="M41" s="31" t="s">
         <v>316</v>
       </c>
-      <c r="N40" s="32" t="s">
+      <c r="N41" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="O40" s="32" t="s">
+      <c r="O41" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="P40" s="32" t="s">
+      <c r="P41" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="31" t="s">
+      <c r="Q41" s="28"/>
+      <c r="R41" s="31" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="41" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D41" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="28"/>
-    </row>
-    <row r="42" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A42" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="7" t="s">
+      <c r="D42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G42" s="21"/>
       <c r="L42" s="21"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
       <c r="Q42" s="28"/>
-      <c r="R42" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="43" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A43" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D43" s="7" t="b">
         <v>1</v>
@@ -2998,47 +3004,60 @@
         <v>0</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>250</v>
+        <v>16</v>
       </c>
       <c r="G43" s="21"/>
       <c r="L43" s="21"/>
       <c r="Q43" s="28"/>
       <c r="R43" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D44" s="41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>16</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A44" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="G44" s="21"/>
       <c r="L44" s="21"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="17"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="17"/>
       <c r="Q44" s="28"/>
+      <c r="R44" s="7" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
+      <c r="A45" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G45" s="21"/>
       <c r="L45" s="21"/>
       <c r="M45" s="17"/>
@@ -3047,22 +3066,11 @@
       <c r="P45" s="17"/>
       <c r="Q45" s="28"/>
     </row>
-    <row r="46" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A46" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
       <c r="G46" s="21"/>
       <c r="L46" s="21"/>
       <c r="M46" s="17"/>
@@ -3071,24 +3079,21 @@
       <c r="P46" s="17"/>
       <c r="Q46" s="28"/>
     </row>
-    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G47" s="21"/>
       <c r="L47" s="21"/>
@@ -3098,15 +3103,15 @@
       <c r="P47" s="17"/>
       <c r="Q47" s="28"/>
     </row>
-    <row r="48" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D48" s="2" t="b">
         <v>0</v>
@@ -3114,96 +3119,97 @@
       <c r="E48" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G48" s="22"/>
-      <c r="L48" s="22"/>
+      <c r="F48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="21"/>
+      <c r="L48" s="21"/>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
       <c r="O48" s="17"/>
       <c r="P48" s="17"/>
       <c r="Q48" s="28"/>
-      <c r="R48" s="2" t="s">
+    </row>
+    <row r="49" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G49" s="22"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="28"/>
+      <c r="R49" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G49" s="22"/>
-      <c r="H49" s="6" t="s">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="22"/>
+      <c r="H50" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="I49" s="6" t="s">
+      <c r="I50" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="J49" s="6" t="s">
+      <c r="J50" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="K49" s="6" t="s">
+      <c r="K50" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="L49" s="22"/>
-      <c r="M49" s="6" t="s">
+      <c r="L50" s="22"/>
+      <c r="M50" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="N49" s="6" t="s">
+      <c r="N50" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O49" s="6" t="s">
+      <c r="O50" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P49" s="6" t="s">
+      <c r="P50" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Q49" s="22"/>
-    </row>
-    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="7" t="s">
+      <c r="Q50" s="22"/>
+    </row>
+    <row r="51" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B51" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D50" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="Q50" s="28"/>
-      <c r="R50" s="8" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A51" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="D51" s="7" t="b">
         <v>0</v>
       </c>
@@ -3211,48 +3217,47 @@
         <v>1</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>238</v>
+        <v>4</v>
       </c>
       <c r="G51" s="21"/>
       <c r="L51" s="21"/>
       <c r="Q51" s="28"/>
-    </row>
-    <row r="52" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D52" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>16</v>
+      <c r="R51" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A52" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D52" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="G52" s="21"/>
       <c r="L52" s="21"/>
-      <c r="M52" s="17"/>
-      <c r="N52" s="17"/>
-      <c r="O52" s="17"/>
-      <c r="P52" s="17"/>
       <c r="Q52" s="28"/>
     </row>
     <row r="53" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D53" s="2" t="b">
         <v>0</v>
@@ -3271,378 +3276,375 @@
       <c r="P53" s="17"/>
       <c r="Q53" s="28"/>
     </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A54" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B54" s="7" t="s">
+    <row r="54" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F54" s="7" t="s">
+      <c r="C54" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G54" s="21"/>
       <c r="L54" s="21"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="17"/>
       <c r="Q54" s="28"/>
-      <c r="R54" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B55" s="2" t="s">
+    </row>
+    <row r="55" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="C55" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="21"/>
       <c r="L55" s="21"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="17"/>
       <c r="Q55" s="28"/>
-    </row>
-    <row r="56" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A56" s="16" t="s">
+      <c r="R55" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D56" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="28"/>
+    </row>
+    <row r="57" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A57" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B57" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="C57" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="D56" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="16" t="s">
+      <c r="D57" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="G56" s="23"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="23"/>
-      <c r="M56" s="16"/>
-      <c r="N56" s="16"/>
-      <c r="O56" s="16"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="23"/>
-      <c r="R56" s="16"/>
-    </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
+      <c r="G57" s="23"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="23"/>
+      <c r="R57" s="16"/>
+    </row>
+    <row r="58" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C58" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="G57" s="28"/>
-      <c r="L57" s="28"/>
-      <c r="Q57" s="28"/>
-    </row>
-    <row r="58" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A58" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="D58" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="37" t="s">
-        <v>342</v>
-      </c>
       <c r="G58" s="28"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="37"/>
       <c r="L58" s="28"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="37"/>
-      <c r="O58" s="37"/>
-      <c r="P58" s="37"/>
       <c r="Q58" s="28"/>
     </row>
     <row r="59" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="37" t="s">
+        <v>342</v>
+      </c>
+      <c r="G59" s="28"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="37"/>
+      <c r="O59" s="37"/>
+      <c r="P59" s="37"/>
+      <c r="Q59" s="28"/>
+    </row>
+    <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="G59" s="28"/>
-      <c r="L59" s="28"/>
-      <c r="Q59"/>
-    </row>
-    <row r="60" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="16" t="s">
+      <c r="G60" s="28"/>
+      <c r="L60" s="28"/>
+      <c r="Q60"/>
+    </row>
+    <row r="61" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B61" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C61" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="D60" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>348</v>
-      </c>
-      <c r="G60" s="23"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="16"/>
-      <c r="K60" s="16"/>
-      <c r="L60" s="23"/>
-      <c r="M60" s="16"/>
-      <c r="N60" s="16"/>
-      <c r="O60" s="16"/>
-      <c r="P60" s="16"/>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="16" t="s">
+      <c r="D61" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="G61" s="23"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="16" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
+    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="D62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G61" s="21"/>
-      <c r="L61" s="21"/>
-      <c r="Q61" s="28"/>
-      <c r="R61" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D62" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="G62" s="21"/>
       <c r="L62" s="21"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="17"/>
       <c r="Q62" s="28"/>
-      <c r="R62" s="2" t="s">
+      <c r="R62" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G63" s="21"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="28"/>
+      <c r="R63" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:18" s="39" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
+    <row r="64" spans="1:18" s="39" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
         <v>345</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C64" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="D63" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="G63" s="28"/>
-      <c r="L63" s="28"/>
-      <c r="Q63" s="28"/>
-    </row>
-    <row r="64" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="7" t="s">
+      <c r="D64" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="Q64" s="28"/>
+    </row>
+    <row r="65" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B65" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C65" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="7" t="s">
+      <c r="D65" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="G64" s="21"/>
-      <c r="L64" s="21"/>
-      <c r="Q64" s="28"/>
-      <c r="R64" s="7" t="s">
+      <c r="G65" s="21"/>
+      <c r="L65" s="21"/>
+      <c r="Q65" s="28"/>
+      <c r="R65" s="7" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="65" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
+    <row r="66" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
         <v>302</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>82</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>303</v>
       </c>
-      <c r="D65" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
         <v>260</v>
       </c>
-      <c r="G65" s="28"/>
-      <c r="L65" s="28"/>
-      <c r="Q65" s="28"/>
-    </row>
-    <row r="66" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
+      <c r="G66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="Q66" s="28"/>
+    </row>
+    <row r="67" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" s="2" t="s">
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="G66" s="21"/>
-      <c r="L66" s="21"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="17"/>
-      <c r="Q66" s="28"/>
-      <c r="R66" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A67" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="G67" s="21"/>
       <c r="L67" s="21"/>
@@ -3652,27 +3654,27 @@
       <c r="P67" s="17"/>
       <c r="Q67" s="28"/>
       <c r="R67" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>197</v>
+        <v>10</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>198</v>
+        <v>72</v>
       </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E68" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>226</v>
+        <v>348</v>
       </c>
       <c r="G68" s="21"/>
       <c r="L68" s="21"/>
@@ -3681,173 +3683,176 @@
       <c r="O68" s="17"/>
       <c r="P68" s="17"/>
       <c r="Q68" s="28"/>
-    </row>
-    <row r="69" spans="1:18" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="25" t="s">
-        <v>293</v>
-      </c>
-      <c r="B69" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="D69" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="25" t="s">
-        <v>294</v>
+      <c r="R68" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="G69" s="21"/>
       <c r="L69" s="21"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
       <c r="Q69" s="28"/>
-      <c r="R69" s="25" t="s">
+    </row>
+    <row r="70" spans="1:18" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>295</v>
+      </c>
+      <c r="D70" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="G70" s="21"/>
+      <c r="L70" s="21"/>
+      <c r="Q70" s="28"/>
+      <c r="R70" s="25" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="70" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D70" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G70" s="21"/>
-      <c r="H70" s="2" t="s">
+      <c r="D71" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" s="21"/>
+      <c r="H71" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I70" s="31" t="s">
+      <c r="I71" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J70" s="31" t="s">
+      <c r="J71" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="K70" s="31" t="s">
+      <c r="K71" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="L70" s="21"/>
-      <c r="M70" s="17" t="s">
+      <c r="L71" s="21"/>
+      <c r="M71" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="N70" s="18" t="s">
+      <c r="N71" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="O70" s="18" t="s">
+      <c r="O71" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="P70" s="18" t="s">
+      <c r="P71" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="Q70" s="28"/>
-    </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A71" s="38" t="s">
+      <c r="Q71" s="28"/>
+    </row>
+    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B71" s="38" t="s">
+      <c r="B72" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C71" s="38" t="s">
+      <c r="C72" s="38" t="s">
         <v>344</v>
       </c>
-      <c r="D71" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="38"/>
-      <c r="G71" s="21"/>
-      <c r="L71" s="21"/>
-      <c r="M71" s="17"/>
-      <c r="N71" s="17"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="17"/>
-      <c r="Q71" s="28"/>
-    </row>
-    <row r="72" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D72" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="D72" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="38"/>
       <c r="G72" s="21"/>
       <c r="L72" s="21"/>
+      <c r="M72" s="17"/>
+      <c r="N72" s="17"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="17"/>
       <c r="Q72" s="28"/>
-      <c r="R72" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B73" s="2" t="s">
+    </row>
+    <row r="73" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
+      <c r="C73" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G73" s="21"/>
       <c r="L73" s="21"/>
-      <c r="M73" s="17"/>
-      <c r="N73" s="17"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="17"/>
       <c r="Q73" s="28"/>
+      <c r="R73" s="7" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="D74" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G74" s="21"/>
       <c r="L74" s="21"/>
@@ -3857,447 +3862,447 @@
       <c r="P74" s="17"/>
       <c r="Q74" s="28"/>
     </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="21"/>
+      <c r="L75" s="21"/>
+      <c r="M75" s="17"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
+      <c r="Q75" s="28"/>
+    </row>
+    <row r="76" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D75" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G75" s="21"/>
-      <c r="H75" s="17" t="s">
+      <c r="D76" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" s="21"/>
+      <c r="H76" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I75" s="17" t="s">
+      <c r="I76" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J75" s="17" t="s">
+      <c r="J76" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K75" s="17" t="s">
+      <c r="K76" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L75" s="21"/>
-      <c r="M75" s="18" t="s">
+      <c r="L76" s="21"/>
+      <c r="M76" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="N75" s="18" t="s">
+      <c r="N76" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="O75" s="18" t="s">
+      <c r="O76" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="P75" s="18" t="s">
+      <c r="P76" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="Q75" s="28"/>
-    </row>
-    <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
+      <c r="Q76" s="28"/>
+    </row>
+    <row r="77" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="2" t="s">
+      <c r="D77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="G76" s="21"/>
-      <c r="L76" s="21"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
-      <c r="Q76" s="28"/>
-    </row>
-    <row r="77" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D77" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="G77" s="21"/>
       <c r="L77" s="21"/>
+      <c r="M77" s="17"/>
+      <c r="N77" s="17"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="17"/>
       <c r="Q77" s="28"/>
-      <c r="R77" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>19</v>
+    </row>
+    <row r="78" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D78" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G78" s="21"/>
       <c r="L78" s="21"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="17"/>
       <c r="Q78" s="28"/>
-    </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>240</v>
+      <c r="R78" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G79" s="21"/>
       <c r="L79" s="21"/>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="17"/>
       <c r="Q79" s="28"/>
-      <c r="R79" s="8" t="s">
+    </row>
+    <row r="80" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A80" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="Q80" s="28"/>
+      <c r="R80" s="8" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G80" s="21"/>
-      <c r="H80" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J80" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="K80" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="L80" s="21"/>
-      <c r="M80" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="N80" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="O80" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="P80" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q80" s="28"/>
     </row>
     <row r="81" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" s="21"/>
+      <c r="H81" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J81" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K81" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L81" s="21"/>
+      <c r="M81" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="N81" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="O81" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="P81" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q81" s="28"/>
+    </row>
+    <row r="82" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="D82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="G81" s="21"/>
-      <c r="L81" s="21"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
-      <c r="Q81" s="28"/>
-    </row>
-    <row r="82" spans="1:19" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D82" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="G82" s="21"/>
       <c r="L82" s="21"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
       <c r="Q82" s="28"/>
-      <c r="R82" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="83" spans="1:19" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D83" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E83" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="G83" s="21"/>
       <c r="L83" s="21"/>
       <c r="Q83" s="28"/>
-      <c r="R83" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>98</v>
+      <c r="R83" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A84" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G84" s="21"/>
       <c r="L84" s="21"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
       <c r="Q84" s="28"/>
-    </row>
-    <row r="85" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R84" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G85" s="21"/>
+      <c r="L85" s="21"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
+      <c r="Q85" s="28"/>
+    </row>
+    <row r="86" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G85" s="21"/>
-      <c r="H85" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L85" s="21"/>
-      <c r="M85" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N85" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O85" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P85" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q85" s="28"/>
-    </row>
-    <row r="86" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" s="21"/>
+      <c r="H86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L86" s="21"/>
+      <c r="M86" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N86" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O86" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P86" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q86" s="28"/>
+    </row>
+    <row r="87" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G86" s="21"/>
-      <c r="L86" s="21"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="28"/>
-      <c r="R86" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B87" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C87" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D87" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="G87" s="28"/>
-      <c r="L87" s="28"/>
+      <c r="D87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G87" s="21"/>
+      <c r="L87" s="21"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
       <c r="Q87" s="28"/>
       <c r="R87" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B88" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D88" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="G88" s="28"/>
+      <c r="L88" s="28"/>
+      <c r="Q88" s="28"/>
+      <c r="R88" s="8" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="88" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="12" t="s">
+      <c r="D89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="12" t="s">
         <v>290</v>
-      </c>
-      <c r="G88" s="21"/>
-      <c r="L88" s="21"/>
-      <c r="M88" s="17"/>
-      <c r="N88" s="17"/>
-      <c r="O88" s="17"/>
-      <c r="P88" s="17"/>
-      <c r="Q88" s="28"/>
-    </row>
-    <row r="89" spans="1:19" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D89" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="G89" s="21"/>
       <c r="L89" s="21"/>
@@ -4307,30 +4312,26 @@
       <c r="P89" s="17"/>
       <c r="Q89" s="28"/>
     </row>
-    <row r="90" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B90" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" t="s">
-        <v>330</v>
-      </c>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>25</v>
+    <row r="90" spans="1:19" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D90" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="G90" s="21"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="17"/>
       <c r="L90" s="21"/>
       <c r="M90" s="17"/>
       <c r="N90" s="17"/>
@@ -4338,76 +4339,80 @@
       <c r="P90" s="17"/>
       <c r="Q90" s="28"/>
     </row>
-    <row r="91" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A91" t="s">
-        <v>328</v>
+    <row r="91" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="B91" t="s">
         <v>10</v>
       </c>
       <c r="C91" t="s">
+        <v>330</v>
+      </c>
+      <c r="D91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G91" s="21"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
+      <c r="J91" s="17"/>
+      <c r="K91" s="17"/>
+      <c r="L91" s="21"/>
+      <c r="M91" s="17"/>
+      <c r="N91" s="17"/>
+      <c r="O91" s="17"/>
+      <c r="P91" s="17"/>
+      <c r="Q91" s="28"/>
+    </row>
+    <row r="92" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>328</v>
+      </c>
+      <c r="B92" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" t="s">
         <v>329</v>
       </c>
-      <c r="D91" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="D92" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" t="s">
         <v>25</v>
       </c>
-      <c r="G91" s="28"/>
-      <c r="L91" s="28"/>
-      <c r="Q91" s="28"/>
-      <c r="R91"/>
-      <c r="S91"/>
-    </row>
-    <row r="92" spans="1:19" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
+      <c r="G92" s="28"/>
+      <c r="L92" s="28"/>
+      <c r="Q92" s="28"/>
+      <c r="R92"/>
+      <c r="S92"/>
+    </row>
+    <row r="93" spans="1:19" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D92" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="21"/>
-      <c r="L92" s="21"/>
-      <c r="M92" s="17"/>
-      <c r="N92" s="17"/>
-      <c r="O92" s="17"/>
-      <c r="P92" s="17"/>
-      <c r="Q92" s="28"/>
-    </row>
-    <row r="93" spans="1:19" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D93" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E93" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F93" s="6" t="s">
-        <v>241</v>
+      <c r="F93" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G93" s="21"/>
       <c r="L93" s="21"/>
@@ -4416,19 +4421,16 @@
       <c r="O93" s="17"/>
       <c r="P93" s="17"/>
       <c r="Q93" s="28"/>
-      <c r="R93" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="94" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="94" spans="1:19" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D94" s="2" t="b">
         <v>0</v>
@@ -4436,8 +4438,8 @@
       <c r="E94" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F94" s="2" t="s">
-        <v>16</v>
+      <c r="F94" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="G94" s="21"/>
       <c r="L94" s="21"/>
@@ -4446,22 +4448,28 @@
       <c r="O94" s="17"/>
       <c r="P94" s="17"/>
       <c r="Q94" s="28"/>
-    </row>
-    <row r="95" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R94" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E95" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G95" s="21"/>
       <c r="L95" s="21"/>
@@ -4470,28 +4478,22 @@
       <c r="O95" s="17"/>
       <c r="P95" s="17"/>
       <c r="Q95" s="28"/>
-      <c r="R95" s="8" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="96" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="96" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="D96" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="G96" s="21"/>
       <c r="L96" s="21"/>
@@ -4501,91 +4503,95 @@
       <c r="P96" s="17"/>
       <c r="Q96" s="28"/>
       <c r="R96" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G97" s="21"/>
+      <c r="L97" s="21"/>
+      <c r="M97" s="17"/>
+      <c r="N97" s="17"/>
+      <c r="O97" s="17"/>
+      <c r="P97" s="17"/>
+      <c r="Q97" s="28"/>
+      <c r="R97" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="97" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G97" s="21"/>
-      <c r="H97" s="17" t="s">
+      <c r="D98" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G98" s="21"/>
+      <c r="H98" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I97" s="17" t="s">
+      <c r="I98" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J97" s="17" t="s">
+      <c r="J98" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K97" s="17" t="s">
+      <c r="K98" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L97" s="21"/>
-      <c r="M97" s="18" t="s">
+      <c r="L98" s="21"/>
+      <c r="M98" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="N97" s="18" t="s">
+      <c r="N98" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="O97" s="18" t="s">
+      <c r="O98" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="P97" s="18" t="s">
+      <c r="P98" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="Q97" s="28"/>
-      <c r="R97" s="2" t="s">
+      <c r="Q98" s="28"/>
+      <c r="R98" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="98" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A98" s="7" t="s">
+    <row r="99" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A99" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B99" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C99" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D98" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G98" s="21"/>
-      <c r="L98" s="21"/>
-      <c r="Q98" s="28"/>
-      <c r="R98" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="99" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="D99" s="7" t="b">
         <v>1</v>
@@ -4600,91 +4606,73 @@
       <c r="L99" s="21"/>
       <c r="Q99" s="28"/>
       <c r="R99" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="100" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D100" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E100" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="G100" s="21"/>
       <c r="L100" s="21"/>
       <c r="Q100" s="28"/>
       <c r="R100" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101" s="21"/>
+      <c r="L101" s="21"/>
+      <c r="Q101" s="28"/>
+      <c r="R101" s="7" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="101" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G101" s="21"/>
-      <c r="H101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L101" s="21"/>
-      <c r="M101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P101" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q101" s="28"/>
     </row>
     <row r="102" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D102" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="2" t="b">
         <v>1</v>
@@ -4719,23 +4707,23 @@
     </row>
     <row r="103" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D103" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G103" s="21"/>
       <c r="H103" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I103" s="2" t="s">
         <v>4</v>
@@ -4748,7 +4736,7 @@
       </c>
       <c r="L103" s="21"/>
       <c r="M103" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N103" s="17" t="s">
         <v>4</v>
@@ -4761,148 +4749,145 @@
       </c>
       <c r="Q103" s="28"/>
     </row>
-    <row r="104" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D104" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G104" s="21"/>
+      <c r="H104" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L104" s="21"/>
+      <c r="M104" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P104" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q104" s="28"/>
+    </row>
+    <row r="105" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D104" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G104" s="21"/>
-      <c r="L104" s="21"/>
-      <c r="M104" s="17"/>
-      <c r="N104" s="17"/>
-      <c r="O104" s="17"/>
-      <c r="P104" s="17"/>
-      <c r="Q104" s="28"/>
-    </row>
-    <row r="105" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
+      <c r="D105" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G105" s="21"/>
+      <c r="L105" s="21"/>
+      <c r="M105" s="17"/>
+      <c r="N105" s="17"/>
+      <c r="O105" s="17"/>
+      <c r="P105" s="17"/>
+      <c r="Q105" s="28"/>
+    </row>
+    <row r="106" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
         <v>331</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>5</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>332</v>
       </c>
-      <c r="D105" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" t="b">
-        <v>1</v>
-      </c>
-      <c r="F105" t="s">
-        <v>4</v>
-      </c>
-      <c r="G105" s="28"/>
-      <c r="H105"/>
-      <c r="I105"/>
-      <c r="J105"/>
-      <c r="K105"/>
-      <c r="L105" s="28"/>
-      <c r="M105"/>
-      <c r="N105"/>
-      <c r="O105"/>
-      <c r="P105"/>
-      <c r="Q105" s="24"/>
-      <c r="R105"/>
-      <c r="S105"/>
-    </row>
-    <row r="106" spans="1:19" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A106" s="7" t="s">
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>4</v>
+      </c>
+      <c r="G106" s="28"/>
+      <c r="H106"/>
+      <c r="I106"/>
+      <c r="J106"/>
+      <c r="K106"/>
+      <c r="L106" s="28"/>
+      <c r="M106"/>
+      <c r="N106"/>
+      <c r="O106"/>
+      <c r="P106"/>
+      <c r="Q106" s="24"/>
+      <c r="R106"/>
+      <c r="S106"/>
+    </row>
+    <row r="107" spans="1:19" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A107" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B107" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C107" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D106" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G106" s="21"/>
-      <c r="L106" s="21"/>
-      <c r="Q106" s="28"/>
-      <c r="R106" s="7" t="s">
+      <c r="D107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G107" s="21"/>
+      <c r="L107" s="21"/>
+      <c r="Q107" s="28"/>
+      <c r="R107" s="7" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="107" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G107" s="21"/>
-      <c r="H107" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L107" s="21"/>
-      <c r="M107" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q107" s="28"/>
-      <c r="R107" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>277</v>
+        <v>129</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D108" s="2" t="b">
         <v>1</v>
@@ -4937,94 +4922,138 @@
         <v>4</v>
       </c>
       <c r="Q108" s="28"/>
+      <c r="R108" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="109" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" s="21"/>
+      <c r="H109" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L109" s="21"/>
+      <c r="M109" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="28"/>
+    </row>
+    <row r="110" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F109" s="2" t="s">
+      <c r="D110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G109" s="21"/>
-      <c r="L109" s="21"/>
-      <c r="M109" s="17"/>
-      <c r="N109" s="17"/>
-      <c r="O109" s="17"/>
-      <c r="P109" s="17"/>
-      <c r="Q109" s="28"/>
-    </row>
-    <row r="110" spans="1:19" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A110" s="27" t="s">
+      <c r="G110" s="21"/>
+      <c r="L110" s="21"/>
+      <c r="M110" s="17"/>
+      <c r="N110" s="17"/>
+      <c r="O110" s="17"/>
+      <c r="P110" s="17"/>
+      <c r="Q110" s="28"/>
+    </row>
+    <row r="111" spans="1:19" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A111" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="B110" s="27" t="s">
+      <c r="B111" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C110" s="27" t="s">
+      <c r="C111" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="D110" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="27" t="s">
+      <c r="D111" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="G110" s="28"/>
-      <c r="H110" s="27"/>
-      <c r="I110" s="27"/>
-      <c r="J110" s="27"/>
-      <c r="K110" s="27"/>
-      <c r="L110" s="28"/>
-      <c r="M110" s="27"/>
-      <c r="Q110" s="28"/>
-    </row>
-    <row r="111" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A111" s="2" t="s">
+      <c r="G111" s="28"/>
+      <c r="H111" s="27"/>
+      <c r="I111" s="27"/>
+      <c r="J111" s="27"/>
+      <c r="K111" s="27"/>
+      <c r="L111" s="28"/>
+      <c r="M111" s="27"/>
+      <c r="Q111" s="28"/>
+    </row>
+    <row r="112" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A112" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D111" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111" s="2" t="s">
+      <c r="D112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="G111" s="21"/>
-      <c r="L111" s="21"/>
-      <c r="M111" s="17"/>
-      <c r="N111" s="17"/>
-      <c r="O111" s="17"/>
-      <c r="P111" s="17"/>
-      <c r="Q111" s="28"/>
-      <c r="R111" s="2" t="s">
+      <c r="G112" s="21"/>
+      <c r="L112" s="21"/>
+      <c r="M112" s="17"/>
+      <c r="N112" s="17"/>
+      <c r="O112" s="17"/>
+      <c r="P112" s="17"/>
+      <c r="Q112" s="28"/>
+      <c r="R112" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="R112"/>
     </row>
     <row r="113" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R113"/>
@@ -5088,6 +5117,9 @@
     </row>
     <row r="133" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R133"/>
+    </row>
+    <row r="134" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R134"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5095,15 +5127,15 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1"/>
     <hyperlink ref="F21" r:id="rId2"/>
-    <hyperlink ref="F58" r:id="rId3"/>
+    <hyperlink ref="F59" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
Introductie van nativescalars tbv. #139; Schema generatoren aangepast.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="360">
   <si>
     <t>Name</t>
   </si>
@@ -1096,6 +1096,15 @@
   </si>
   <si>
     <t>1.0.0.-3.2.2</t>
+  </si>
+  <si>
+    <t>nativescalars</t>
+  </si>
+  <si>
+    <t>yes/no</t>
+  </si>
+  <si>
+    <t>Yes if scalar types may be entered without reference to a UML datatype</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1249,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1339,6 +1348,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1645,13 +1657,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S136"/>
+  <dimension ref="A1:S137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A59" sqref="A59"/>
+      <selection pane="bottomRight" activeCell="A76" sqref="A76:XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1861,16 +1873,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="42" t="b">
+      <c r="D7" s="43" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1888,10 +1900,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -3058,16 +3070,16 @@
       </c>
     </row>
     <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="42" t="b">
+      <c r="D45" s="43" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="2" t="b">
@@ -3085,10 +3097,10 @@
       <c r="Q45" s="28"/>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="42"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
       <c r="G46" s="21"/>
       <c r="L46" s="21"/>
       <c r="M46" s="17"/>
@@ -3899,51 +3911,63 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G76" s="21"/>
-      <c r="L76" s="21"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17"/>
+    <row r="76" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="42" t="s">
+        <v>357</v>
+      </c>
+      <c r="B76" s="42" t="s">
+        <v>358</v>
+      </c>
+      <c r="C76" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D76" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="28"/>
+      <c r="H76" s="42"/>
+      <c r="I76" s="42"/>
+      <c r="J76" s="42"/>
+      <c r="K76" s="42"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="N76" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="O76" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="P76" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="Q76" s="28"/>
     </row>
     <row r="77" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="D77" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G77" s="21"/>
       <c r="L77" s="21"/>
@@ -3953,447 +3977,447 @@
       <c r="P77" s="17"/>
       <c r="Q77" s="28"/>
     </row>
-    <row r="78" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="21"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
+      <c r="Q78" s="28"/>
+    </row>
+    <row r="79" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G78" s="21"/>
-      <c r="H78" s="17" t="s">
+      <c r="D79" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" s="21"/>
+      <c r="H79" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I78" s="17" t="s">
+      <c r="I79" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J78" s="17" t="s">
+      <c r="J79" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K78" s="17" t="s">
+      <c r="K79" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L78" s="21"/>
-      <c r="M78" s="18" t="s">
+      <c r="L79" s="21"/>
+      <c r="M79" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="N78" s="18" t="s">
+      <c r="N79" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="O78" s="18" t="s">
+      <c r="O79" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="P78" s="18" t="s">
+      <c r="P79" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="Q78" s="28"/>
-    </row>
-    <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A79" s="2" t="s">
+      <c r="Q79" s="28"/>
+    </row>
+    <row r="80" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="2" t="s">
+      <c r="D80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="G79" s="21"/>
-      <c r="L79" s="21"/>
-      <c r="M79" s="17"/>
-      <c r="N79" s="17"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="17"/>
-      <c r="Q79" s="28"/>
-    </row>
-    <row r="80" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D80" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="G80" s="21"/>
       <c r="L80" s="21"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
       <c r="Q80" s="28"/>
-      <c r="R80" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="81" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>19</v>
+    </row>
+    <row r="81" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D81" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G81" s="21"/>
       <c r="L81" s="21"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
       <c r="Q81" s="28"/>
-    </row>
-    <row r="82" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D82" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>240</v>
+      <c r="R81" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G82" s="21"/>
       <c r="L82" s="21"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
       <c r="Q82" s="28"/>
-      <c r="R82" s="8" t="s">
+    </row>
+    <row r="83" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A83" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D83" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G83" s="21"/>
+      <c r="L83" s="21"/>
+      <c r="Q83" s="28"/>
+      <c r="R83" s="8" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G83" s="21"/>
-      <c r="H83" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J83" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="K83" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="L83" s="21"/>
-      <c r="M83" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="N83" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="O83" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="P83" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q83" s="28"/>
     </row>
     <row r="84" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" s="21"/>
+      <c r="H84" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J84" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K84" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L84" s="21"/>
+      <c r="M84" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="N84" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="O84" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="P84" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q84" s="28"/>
+    </row>
+    <row r="85" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="2" t="s">
+      <c r="D85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="G84" s="21"/>
-      <c r="L84" s="21"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
-      <c r="Q84" s="28"/>
-    </row>
-    <row r="85" spans="1:19" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="G85" s="21"/>
       <c r="L85" s="21"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
       <c r="Q85" s="28"/>
-      <c r="R85" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="86" spans="1:19" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A86" s="7" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D86" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E86" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="G86" s="21"/>
       <c r="L86" s="21"/>
       <c r="Q86" s="28"/>
-      <c r="R86" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A87" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D87" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>98</v>
+      <c r="R86" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A87" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D87" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G87" s="21"/>
       <c r="L87" s="21"/>
-      <c r="M87" s="17"/>
-      <c r="N87" s="17"/>
-      <c r="O87" s="17"/>
-      <c r="P87" s="17"/>
       <c r="Q87" s="28"/>
-    </row>
-    <row r="88" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R87" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G88" s="21"/>
+      <c r="L88" s="21"/>
+      <c r="M88" s="17"/>
+      <c r="N88" s="17"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="17"/>
+      <c r="Q88" s="28"/>
+    </row>
+    <row r="89" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G88" s="21"/>
-      <c r="H88" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L88" s="21"/>
-      <c r="M88" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N88" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O88" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P88" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q88" s="28"/>
-    </row>
-    <row r="89" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G89" s="21"/>
+      <c r="H89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L89" s="21"/>
+      <c r="M89" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N89" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O89" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P89" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q89" s="28"/>
+    </row>
+    <row r="90" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G89" s="21"/>
-      <c r="L89" s="21"/>
-      <c r="M89" s="17"/>
-      <c r="N89" s="17"/>
-      <c r="O89" s="17"/>
-      <c r="P89" s="17"/>
-      <c r="Q89" s="28"/>
-      <c r="R89" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="90" spans="1:19" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B90" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D90" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F90" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="G90" s="28"/>
-      <c r="L90" s="28"/>
+      <c r="D90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G90" s="21"/>
+      <c r="L90" s="21"/>
+      <c r="M90" s="17"/>
+      <c r="N90" s="17"/>
+      <c r="O90" s="17"/>
+      <c r="P90" s="17"/>
       <c r="Q90" s="28"/>
       <c r="R90" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A91" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D91" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="G91" s="28"/>
+      <c r="L91" s="28"/>
+      <c r="Q91" s="28"/>
+      <c r="R91" s="8" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="91" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="12" t="s">
+      <c r="D92" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="12" t="s">
         <v>290</v>
-      </c>
-      <c r="G91" s="21"/>
-      <c r="L91" s="21"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
-      <c r="Q91" s="28"/>
-    </row>
-    <row r="92" spans="1:19" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D92" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="G92" s="21"/>
       <c r="L92" s="21"/>
@@ -4403,30 +4427,26 @@
       <c r="P92" s="17"/>
       <c r="Q92" s="28"/>
     </row>
-    <row r="93" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B93" t="s">
-        <v>10</v>
-      </c>
-      <c r="C93" t="s">
-        <v>330</v>
-      </c>
-      <c r="D93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>25</v>
+    <row r="93" spans="1:19" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D93" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="G93" s="21"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="17"/>
-      <c r="J93" s="17"/>
-      <c r="K93" s="17"/>
       <c r="L93" s="21"/>
       <c r="M93" s="17"/>
       <c r="N93" s="17"/>
@@ -4434,76 +4454,80 @@
       <c r="P93" s="17"/>
       <c r="Q93" s="28"/>
     </row>
-    <row r="94" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
-        <v>328</v>
+    <row r="94" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
       </c>
       <c r="C94" t="s">
+        <v>330</v>
+      </c>
+      <c r="D94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" s="21"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
+      <c r="J94" s="17"/>
+      <c r="K94" s="17"/>
+      <c r="L94" s="21"/>
+      <c r="M94" s="17"/>
+      <c r="N94" s="17"/>
+      <c r="O94" s="17"/>
+      <c r="P94" s="17"/>
+      <c r="Q94" s="28"/>
+    </row>
+    <row r="95" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>328</v>
+      </c>
+      <c r="B95" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" t="s">
         <v>329</v>
       </c>
-      <c r="D94" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="D95" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" t="s">
         <v>25</v>
       </c>
-      <c r="G94" s="28"/>
-      <c r="L94" s="28"/>
-      <c r="Q94" s="28"/>
-      <c r="R94"/>
-      <c r="S94"/>
-    </row>
-    <row r="95" spans="1:19" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
+      <c r="G95" s="28"/>
+      <c r="L95" s="28"/>
+      <c r="Q95" s="28"/>
+      <c r="R95"/>
+      <c r="S95"/>
+    </row>
+    <row r="96" spans="1:19" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D95" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G95" s="21"/>
-      <c r="L95" s="21"/>
-      <c r="M95" s="17"/>
-      <c r="N95" s="17"/>
-      <c r="O95" s="17"/>
-      <c r="P95" s="17"/>
-      <c r="Q95" s="28"/>
-    </row>
-    <row r="96" spans="1:19" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A96" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D96" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E96" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F96" s="6" t="s">
-        <v>241</v>
+      <c r="F96" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G96" s="21"/>
       <c r="L96" s="21"/>
@@ -4512,19 +4536,16 @@
       <c r="O96" s="17"/>
       <c r="P96" s="17"/>
       <c r="Q96" s="28"/>
-      <c r="R96" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="97" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="97" spans="1:19" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D97" s="2" t="b">
         <v>0</v>
@@ -4532,8 +4553,8 @@
       <c r="E97" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F97" s="2" t="s">
-        <v>16</v>
+      <c r="F97" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="G97" s="21"/>
       <c r="L97" s="21"/>
@@ -4542,22 +4563,28 @@
       <c r="O97" s="17"/>
       <c r="P97" s="17"/>
       <c r="Q97" s="28"/>
-    </row>
-    <row r="98" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R97" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D98" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E98" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G98" s="21"/>
       <c r="L98" s="21"/>
@@ -4566,28 +4593,22 @@
       <c r="O98" s="17"/>
       <c r="P98" s="17"/>
       <c r="Q98" s="28"/>
-      <c r="R98" s="8" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="99" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="99" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="D99" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="G99" s="21"/>
       <c r="L99" s="21"/>
@@ -4597,91 +4618,95 @@
       <c r="P99" s="17"/>
       <c r="Q99" s="28"/>
       <c r="R99" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A100" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D100" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G100" s="21"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="17"/>
+      <c r="N100" s="17"/>
+      <c r="O100" s="17"/>
+      <c r="P100" s="17"/>
+      <c r="Q100" s="28"/>
+      <c r="R100" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="100" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G100" s="21"/>
-      <c r="H100" s="17" t="s">
+      <c r="D101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101" s="21"/>
+      <c r="H101" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I100" s="17" t="s">
+      <c r="I101" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J100" s="17" t="s">
+      <c r="J101" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K100" s="17" t="s">
+      <c r="K101" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L100" s="21"/>
-      <c r="M100" s="18" t="s">
+      <c r="L101" s="21"/>
+      <c r="M101" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="N100" s="18" t="s">
+      <c r="N101" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="O100" s="18" t="s">
+      <c r="O101" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="P100" s="18" t="s">
+      <c r="P101" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="Q100" s="28"/>
-      <c r="R100" s="2" t="s">
+      <c r="Q101" s="28"/>
+      <c r="R101" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="101" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A101" s="7" t="s">
+    <row r="102" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A102" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B102" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="C102" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D101" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G101" s="21"/>
-      <c r="L101" s="21"/>
-      <c r="Q101" s="28"/>
-      <c r="R101" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="102" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="D102" s="7" t="b">
         <v>1</v>
@@ -4696,91 +4721,73 @@
       <c r="L102" s="21"/>
       <c r="Q102" s="28"/>
       <c r="R102" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D103" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E103" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103" s="7" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="G103" s="21"/>
       <c r="L103" s="21"/>
       <c r="Q103" s="28"/>
       <c r="R103" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D104" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E104" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" s="21"/>
+      <c r="L104" s="21"/>
+      <c r="Q104" s="28"/>
+      <c r="R104" s="7" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="104" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D104" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E104" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G104" s="21"/>
-      <c r="H104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L104" s="21"/>
-      <c r="M104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P104" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q104" s="28"/>
     </row>
     <row r="105" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D105" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105" s="2" t="b">
         <v>1</v>
@@ -4815,23 +4822,23 @@
     </row>
     <row r="106" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D106" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G106" s="21"/>
       <c r="H106" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>4</v>
@@ -4844,7 +4851,7 @@
       </c>
       <c r="L106" s="21"/>
       <c r="M106" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N106" s="17" t="s">
         <v>4</v>
@@ -4857,148 +4864,145 @@
       </c>
       <c r="Q106" s="28"/>
     </row>
-    <row r="107" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C107" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D107" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G107" s="21"/>
+      <c r="H107" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L107" s="21"/>
+      <c r="M107" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P107" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q107" s="28"/>
+    </row>
+    <row r="108" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A108" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D107" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G107" s="21"/>
-      <c r="L107" s="21"/>
-      <c r="M107" s="17"/>
-      <c r="N107" s="17"/>
-      <c r="O107" s="17"/>
-      <c r="P107" s="17"/>
-      <c r="Q107" s="28"/>
-    </row>
-    <row r="108" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A108" t="s">
+      <c r="D108" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G108" s="21"/>
+      <c r="L108" s="21"/>
+      <c r="M108" s="17"/>
+      <c r="N108" s="17"/>
+      <c r="O108" s="17"/>
+      <c r="P108" s="17"/>
+      <c r="Q108" s="28"/>
+    </row>
+    <row r="109" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
         <v>331</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>5</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C109" t="s">
         <v>332</v>
       </c>
-      <c r="D108" t="b">
-        <v>0</v>
-      </c>
-      <c r="E108" t="b">
-        <v>1</v>
-      </c>
-      <c r="F108" t="s">
-        <v>4</v>
-      </c>
-      <c r="G108" s="28"/>
-      <c r="H108"/>
-      <c r="I108"/>
-      <c r="J108"/>
-      <c r="K108"/>
-      <c r="L108" s="28"/>
-      <c r="M108"/>
-      <c r="N108"/>
-      <c r="O108"/>
-      <c r="P108"/>
-      <c r="Q108" s="24"/>
-      <c r="R108"/>
-      <c r="S108"/>
-    </row>
-    <row r="109" spans="1:19" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A109" s="7" t="s">
+      <c r="D109" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" t="s">
+        <v>4</v>
+      </c>
+      <c r="G109" s="28"/>
+      <c r="H109"/>
+      <c r="I109"/>
+      <c r="J109"/>
+      <c r="K109"/>
+      <c r="L109" s="28"/>
+      <c r="M109"/>
+      <c r="N109"/>
+      <c r="O109"/>
+      <c r="P109"/>
+      <c r="Q109" s="24"/>
+      <c r="R109"/>
+      <c r="S109"/>
+    </row>
+    <row r="110" spans="1:19" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A110" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="B110" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C109" s="7" t="s">
+      <c r="C110" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D109" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F109" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G109" s="21"/>
-      <c r="L109" s="21"/>
-      <c r="Q109" s="28"/>
-      <c r="R109" s="7" t="s">
+      <c r="D110" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" s="21"/>
+      <c r="L110" s="21"/>
+      <c r="Q110" s="28"/>
+      <c r="R110" s="7" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="110" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D110" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G110" s="21"/>
-      <c r="H110" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K110" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L110" s="21"/>
-      <c r="M110" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N110" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O110" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P110" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q110" s="28"/>
-      <c r="R110" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="111" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
-        <v>277</v>
+        <v>129</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D111" s="2" t="b">
         <v>1</v>
@@ -5033,94 +5037,138 @@
         <v>4</v>
       </c>
       <c r="Q111" s="28"/>
+      <c r="R111" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="112" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G112" s="21"/>
+      <c r="H112" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L112" s="21"/>
+      <c r="M112" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q112" s="28"/>
+    </row>
+    <row r="113" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112" s="2" t="s">
+      <c r="D113" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G112" s="21"/>
-      <c r="L112" s="21"/>
-      <c r="M112" s="17"/>
-      <c r="N112" s="17"/>
-      <c r="O112" s="17"/>
-      <c r="P112" s="17"/>
-      <c r="Q112" s="28"/>
-    </row>
-    <row r="113" spans="1:18" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A113" s="27" t="s">
+      <c r="G113" s="21"/>
+      <c r="L113" s="21"/>
+      <c r="M113" s="17"/>
+      <c r="N113" s="17"/>
+      <c r="O113" s="17"/>
+      <c r="P113" s="17"/>
+      <c r="Q113" s="28"/>
+    </row>
+    <row r="114" spans="1:18" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A114" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="B113" s="27" t="s">
+      <c r="B114" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C113" s="27" t="s">
+      <c r="C114" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="D113" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F113" s="27" t="s">
+      <c r="D114" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="G113" s="28"/>
-      <c r="H113" s="27"/>
-      <c r="I113" s="27"/>
-      <c r="J113" s="27"/>
-      <c r="K113" s="27"/>
-      <c r="L113" s="28"/>
-      <c r="M113" s="27"/>
-      <c r="Q113" s="28"/>
-    </row>
-    <row r="114" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A114" s="2" t="s">
+      <c r="G114" s="28"/>
+      <c r="H114" s="27"/>
+      <c r="I114" s="27"/>
+      <c r="J114" s="27"/>
+      <c r="K114" s="27"/>
+      <c r="L114" s="28"/>
+      <c r="M114" s="27"/>
+      <c r="Q114" s="28"/>
+    </row>
+    <row r="115" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A115" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F114" s="2" t="s">
+      <c r="D115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="G114" s="21"/>
-      <c r="L114" s="21"/>
-      <c r="M114" s="17"/>
-      <c r="N114" s="17"/>
-      <c r="O114" s="17"/>
-      <c r="P114" s="17"/>
-      <c r="Q114" s="28"/>
-      <c r="R114" s="2" t="s">
+      <c r="G115" s="21"/>
+      <c r="L115" s="21"/>
+      <c r="M115" s="17"/>
+      <c r="N115" s="17"/>
+      <c r="O115" s="17"/>
+      <c r="P115" s="17"/>
+      <c r="Q115" s="28"/>
+      <c r="R115" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R115"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R116"/>
@@ -5184,6 +5232,9 @@
     </row>
     <row r="136" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R136"/>
+    </row>
+    <row r="137" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R137"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
[kadaster] Naamgeving Profile files GML aangepast
https://github.com/Imvertor/Imvertor-Maven/issues/132
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -1089,9 +1089,6 @@
     <t>Name of the GML profile XSD file. You may use [...] parameters. Defaults to "GmlProfile".</t>
   </si>
   <si>
-    <t>GmlProfile</t>
-  </si>
-  <si>
     <t>Version of the GML profile XSD file. You may use [...] parameters. Defaults to "1.0.0-3.2.2".</t>
   </si>
   <si>
@@ -1105,6 +1102,9 @@
   </si>
   <si>
     <t>Yes if scalar types may be entered without reference to a UML datatype</t>
+  </si>
+  <si>
+    <t>[appinfo/application-name]</t>
   </si>
 </sst>
 </file>
@@ -1660,10 +1660,10 @@
   <dimension ref="A1:S137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A76" sqref="A76:XFD76"/>
+      <selection pane="bottomRight" activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3512,7 +3512,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="G61" s="28"/>
       <c r="L61" s="28"/>
@@ -3526,16 +3526,16 @@
         <v>82</v>
       </c>
       <c r="C62" t="s">
+        <v>354</v>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
         <v>355</v>
-      </c>
-      <c r="D62" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" t="s">
-        <v>356</v>
       </c>
       <c r="G62" s="28"/>
       <c r="L62" s="28"/>
@@ -3913,13 +3913,13 @@
     </row>
     <row r="76" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="42" t="s">
+        <v>356</v>
+      </c>
+      <c r="B76" s="42" t="s">
         <v>357</v>
       </c>
-      <c r="B76" s="42" t="s">
+      <c r="C76" s="42" t="s">
         <v>358</v>
-      </c>
-      <c r="C76" s="42" t="s">
-        <v>359</v>
       </c>
       <c r="D76" s="42" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
[kadaster] IMKAD gebaseerd op MIM1.1
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -903,9 +903,6 @@
     <t>Config</t>
   </si>
   <si>
-    <t>KadasterNEN3610</t>
-  </si>
-  <si>
     <t>messagecollapsekeys</t>
   </si>
   <si>
@@ -1117,6 +1114,9 @@
   </si>
   <si>
     <t>Should an EA toolbox be generated?</t>
+  </si>
+  <si>
+    <t>KadasterMIM11</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1261,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1360,6 +1360,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1678,10 +1681,10 @@
   <dimension ref="A1:S139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1759,29 +1762,29 @@
       <c r="F2" s="3"/>
       <c r="G2" s="20"/>
       <c r="H2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="L2" s="20"/>
       <c r="M2" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>311</v>
       </c>
       <c r="Q2" s="20"/>
       <c r="R2" s="5"/>
@@ -1891,16 +1894,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="45" t="b">
+      <c r="D7" s="46" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1918,10 +1921,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -2474,13 +2477,13 @@
     </row>
     <row r="27" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="44" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B27" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D27" s="44" t="b">
         <v>0</v>
@@ -2518,13 +2521,13 @@
     </row>
     <row r="28" spans="1:18" s="41" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D28" s="41" t="b">
         <v>0</v>
@@ -2632,13 +2635,13 @@
     </row>
     <row r="31" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D31" s="29" t="b">
         <v>0</v>
@@ -2676,13 +2679,13 @@
     </row>
     <row r="32" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A32" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D32" s="31" t="b">
         <v>0</v>
@@ -2718,7 +2721,7 @@
       </c>
       <c r="Q32" s="28"/>
       <c r="R32" s="31" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2801,22 +2804,22 @@
     </row>
     <row r="36" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="B36" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="C36" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="D36" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="34" t="s">
         <v>323</v>
-      </c>
-      <c r="D36" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="34" t="s">
-        <v>324</v>
       </c>
       <c r="G36" s="28"/>
       <c r="L36" s="28"/>
@@ -2868,13 +2871,13 @@
     </row>
     <row r="38" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="35" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B38" s="35" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D38" s="35" t="b">
         <v>0</v>
@@ -3007,13 +3010,13 @@
     </row>
     <row r="42" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A42" s="31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B42" s="31" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D42" s="31" t="b">
         <v>0</v>
@@ -3036,20 +3039,20 @@
       </c>
       <c r="L42" s="28"/>
       <c r="M42" s="31" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N42" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O42" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P42" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q42" s="28"/>
       <c r="R42" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -3132,16 +3135,16 @@
       </c>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="45" t="b">
+      <c r="D46" s="46" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
@@ -3159,10 +3162,10 @@
       <c r="Q46" s="28"/>
     </row>
     <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
       <c r="G47" s="21"/>
       <c r="L47" s="21"/>
       <c r="M47" s="17"/>
@@ -3266,16 +3269,16 @@
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L51" s="22"/>
       <c r="M51" s="6" t="s">
@@ -3450,22 +3453,22 @@
     </row>
     <row r="58" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A58" s="16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B58" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C58" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="D58" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="16" t="s">
         <v>334</v>
-      </c>
-      <c r="D58" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>335</v>
       </c>
       <c r="G58" s="23"/>
       <c r="H58" s="16"/>
@@ -3482,22 +3485,22 @@
     </row>
     <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="D59" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="7" t="s">
         <v>338</v>
-      </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>339</v>
       </c>
       <c r="G59" s="28"/>
       <c r="L59" s="28"/>
@@ -3505,22 +3508,22 @@
     </row>
     <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C60" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="37" t="s">
         <v>341</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="37" t="s">
-        <v>342</v>
       </c>
       <c r="G60" s="28"/>
       <c r="H60" s="37"/>
@@ -3551,7 +3554,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G61" s="28"/>
       <c r="L61" s="28"/>
@@ -3559,13 +3562,13 @@
     </row>
     <row r="62" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B62" t="s">
         <v>82</v>
       </c>
       <c r="C62" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -3574,7 +3577,7 @@
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G62" s="28"/>
       <c r="L62" s="28"/>
@@ -3582,22 +3585,22 @@
     </row>
     <row r="63" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B63" t="s">
         <v>82</v>
       </c>
       <c r="C63" t="s">
+        <v>353</v>
+      </c>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
         <v>354</v>
-      </c>
-      <c r="D63" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" t="s">
-        <v>355</v>
       </c>
       <c r="G63" s="28"/>
       <c r="L63" s="28"/>
@@ -3620,7 +3623,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G64" s="23"/>
       <c r="H64" s="16"/>
@@ -3695,13 +3698,13 @@
     </row>
     <row r="67" spans="1:18" s="39" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D67" s="39" t="b">
         <v>0</v>
@@ -3744,13 +3747,13 @@
     </row>
     <row r="69" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B69" t="s">
         <v>82</v>
       </c>
       <c r="C69" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -3812,7 +3815,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G71" s="21"/>
       <c r="L71" s="21"/>
@@ -3854,13 +3857,13 @@
     </row>
     <row r="73" spans="1:18" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A73" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B73" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D73" s="25" t="b">
         <v>0</v>
@@ -3869,13 +3872,13 @@
         <v>1</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G73" s="21"/>
       <c r="L73" s="21"/>
       <c r="Q73" s="28"/>
       <c r="R73" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="74" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -3908,17 +3911,17 @@
         <v>25</v>
       </c>
       <c r="L74" s="21"/>
-      <c r="M74" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="N74" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="O74" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="P74" s="18" t="s">
-        <v>292</v>
+      <c r="M74" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="N74" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="O74" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="P74" s="45" t="s">
+        <v>363</v>
       </c>
       <c r="Q74" s="28"/>
     </row>
@@ -3930,7 +3933,7 @@
         <v>10</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D75" s="38" t="b">
         <v>0</v>
@@ -3975,13 +3978,13 @@
     </row>
     <row r="77" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="42" t="s">
+        <v>355</v>
+      </c>
+      <c r="B77" s="42" t="s">
         <v>356</v>
       </c>
-      <c r="B77" s="42" t="s">
+      <c r="C77" s="42" t="s">
         <v>357</v>
-      </c>
-      <c r="C77" s="42" t="s">
-        <v>358</v>
       </c>
       <c r="D77" s="42" t="b">
         <v>1</v>
@@ -4096,17 +4099,17 @@
         <v>25</v>
       </c>
       <c r="L80" s="21"/>
-      <c r="M80" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="N80" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="O80" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="P80" s="18" t="s">
-        <v>292</v>
+      <c r="M80" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="N80" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="O80" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="P80" s="45" t="s">
+        <v>363</v>
       </c>
       <c r="Q80" s="28"/>
     </row>
@@ -4453,13 +4456,13 @@
         <v>0</v>
       </c>
       <c r="F92" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G92" s="28"/>
       <c r="L92" s="28"/>
       <c r="Q92" s="28"/>
       <c r="R92" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="93" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4524,7 +4527,7 @@
         <v>10</v>
       </c>
       <c r="C95" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D95" s="2" t="b">
         <v>1</v>
@@ -4549,13 +4552,13 @@
     </row>
     <row r="96" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B96" t="s">
         <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D96" t="b">
         <v>1</v>
@@ -4744,16 +4747,16 @@
       </c>
       <c r="L102" s="21"/>
       <c r="M102" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="N102" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="O102" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="P102" s="18" t="s">
-        <v>292</v>
+        <v>363</v>
+      </c>
+      <c r="N102" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="O102" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="P102" s="45" t="s">
+        <v>363</v>
       </c>
       <c r="Q102" s="28"/>
       <c r="R102" s="2" t="s">
@@ -4999,13 +5002,13 @@
     </row>
     <row r="110" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B110" t="s">
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D110" t="b">
         <v>0</v>
@@ -5176,13 +5179,13 @@
     </row>
     <row r="115" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="43" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B115" s="43" t="s">
         <v>10</v>
       </c>
       <c r="C115" s="43" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D115" s="43" t="b">
         <v>1</v>
@@ -5204,38 +5207,38 @@
         <v>25</v>
       </c>
       <c r="L115" s="28"/>
-      <c r="M115" s="43" t="s">
-        <v>292</v>
-      </c>
-      <c r="N115" s="43" t="s">
-        <v>292</v>
-      </c>
-      <c r="O115" s="43" t="s">
-        <v>292</v>
-      </c>
-      <c r="P115" s="43" t="s">
-        <v>292</v>
+      <c r="M115" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="N115" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="O115" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="P115" s="45" t="s">
+        <v>363</v>
       </c>
       <c r="Q115" s="28"/>
     </row>
     <row r="116" spans="1:18" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A116" s="27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B116" s="27" t="s">
         <v>82</v>
       </c>
       <c r="C116" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="D116" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" s="27" t="s">
         <v>298</v>
-      </c>
-      <c r="D116" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" s="27" t="s">
-        <v>299</v>
       </c>
       <c r="G116" s="28"/>
       <c r="H116" s="27"/>

</xml_diff>

<commit_message>
[Kadaster] Opleveren respec met en zonder wrapper Respec document
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="366">
   <si>
     <t>Name</t>
   </si>
@@ -1117,6 +1117,12 @@
   </si>
   <si>
     <t>KadasterMIM11</t>
+  </si>
+  <si>
+    <t>fullrespec</t>
+  </si>
+  <si>
+    <t>Should a full respec version be generated along with the catalog?</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1267,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1360,6 +1366,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1678,13 +1687,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S139"/>
+  <dimension ref="A1:S140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1894,16 +1903,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="46" t="b">
+      <c r="D7" s="47" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1921,10 +1930,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -3135,16 +3144,16 @@
       </c>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="46" t="s">
+      <c r="A46" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="46" t="b">
+      <c r="D46" s="47" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
@@ -3162,10 +3171,10 @@
       <c r="Q46" s="28"/>
     </row>
     <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="46"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
+      <c r="A47" s="47"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
       <c r="G47" s="21"/>
       <c r="L47" s="21"/>
       <c r="M47" s="17"/>
@@ -3451,133 +3460,151 @@
       <c r="P57" s="17"/>
       <c r="Q57" s="28"/>
     </row>
-    <row r="58" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A58" s="16" t="s">
+    <row r="58" spans="1:18" s="46" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="B58" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="D58" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="28"/>
+      <c r="I58" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="J58" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K58" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="L58" s="28"/>
+      <c r="N58" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="O58" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="P58" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q58" s="28"/>
+    </row>
+    <row r="59" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A59" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B59" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C59" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="D58" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="16" t="s">
+      <c r="D59" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="G58" s="23"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="23"/>
-      <c r="M58" s="16"/>
-      <c r="N58" s="16"/>
-      <c r="O58" s="16"/>
-      <c r="P58" s="16"/>
-      <c r="Q58" s="23"/>
-      <c r="R58" s="16"/>
-    </row>
-    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="7" t="s">
+      <c r="G59" s="23"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="23"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="16"/>
+      <c r="P59" s="16"/>
+      <c r="Q59" s="23"/>
+      <c r="R59" s="16"/>
+    </row>
+    <row r="60" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="D59" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="7" t="s">
+      <c r="D60" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="G59" s="28"/>
-      <c r="L59" s="28"/>
-      <c r="Q59" s="28"/>
-    </row>
-    <row r="60" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="D60" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="37" t="s">
-        <v>341</v>
-      </c>
       <c r="G60" s="28"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="37"/>
       <c r="L60" s="28"/>
-      <c r="M60" s="37"/>
-      <c r="N60" s="37"/>
-      <c r="O60" s="37"/>
-      <c r="P60" s="37"/>
       <c r="Q60" s="28"/>
     </row>
     <row r="61" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D61" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="37" t="s">
+        <v>341</v>
+      </c>
+      <c r="G61" s="28"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="28"/>
+      <c r="M61" s="37"/>
+      <c r="N61" s="37"/>
+      <c r="O61" s="37"/>
+      <c r="P61" s="37"/>
+      <c r="Q61" s="28"/>
+    </row>
+    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="D62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>342</v>
-      </c>
-      <c r="G61" s="28"/>
-      <c r="L61" s="28"/>
-      <c r="Q61" s="28"/>
-    </row>
-    <row r="62" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>350</v>
-      </c>
-      <c r="B62" t="s">
-        <v>82</v>
-      </c>
-      <c r="C62" t="s">
-        <v>352</v>
-      </c>
-      <c r="D62" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" t="s">
-        <v>358</v>
       </c>
       <c r="G62" s="28"/>
       <c r="L62" s="28"/>
@@ -3585,13 +3612,13 @@
     </row>
     <row r="63" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B63" t="s">
         <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -3600,222 +3627,215 @@
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="G63" s="28"/>
       <c r="L63" s="28"/>
       <c r="Q63" s="28"/>
     </row>
-    <row r="64" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="16" t="s">
+    <row r="64" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>351</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" t="s">
+        <v>353</v>
+      </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>354</v>
+      </c>
+      <c r="G64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="Q64" s="28"/>
+    </row>
+    <row r="65" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B65" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C65" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="D64" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="16" t="s">
+      <c r="D65" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="G64" s="23"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="23"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="16"/>
-      <c r="O64" s="16"/>
-      <c r="P64" s="16"/>
-      <c r="Q64" s="23"/>
-      <c r="R64" s="16" t="s">
+      <c r="G65" s="23"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="23"/>
+      <c r="M65" s="16"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="16"/>
+      <c r="P65" s="16"/>
+      <c r="Q65" s="23"/>
+      <c r="R65" s="16" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="65" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="7" t="s">
+    <row r="66" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B66" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C66" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D65" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="7" t="s">
+      <c r="D66" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G65" s="21"/>
-      <c r="L65" s="21"/>
-      <c r="Q65" s="28"/>
-      <c r="R65" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D66" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="G66" s="21"/>
       <c r="L66" s="21"/>
-      <c r="M66" s="17"/>
-      <c r="N66" s="17"/>
-      <c r="O66" s="17"/>
-      <c r="P66" s="17"/>
       <c r="Q66" s="28"/>
-      <c r="R66" s="2" t="s">
+      <c r="R66" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G67" s="21"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="17"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="17"/>
+      <c r="Q67" s="28"/>
+      <c r="R67" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="67" spans="1:18" s="39" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
+    <row r="68" spans="1:18" s="39" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
         <v>344</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C68" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="D67" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="G67" s="28"/>
-      <c r="L67" s="28"/>
-      <c r="Q67" s="28"/>
-    </row>
-    <row r="68" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="7" t="s">
+      <c r="D68" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="28"/>
+      <c r="L68" s="28"/>
+      <c r="Q68" s="28"/>
+    </row>
+    <row r="69" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C69" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D68" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="7" t="s">
+      <c r="D69" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E69" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="G68" s="21"/>
-      <c r="L68" s="21"/>
-      <c r="Q68" s="28"/>
-      <c r="R68" s="7" t="s">
+      <c r="G69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="Q69" s="28"/>
+      <c r="R69" s="7" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="69" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
+    <row r="70" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
         <v>301</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>82</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>302</v>
       </c>
-      <c r="D69" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
         <v>260</v>
       </c>
-      <c r="G69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="Q69" s="28"/>
-    </row>
-    <row r="70" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="2" t="s">
+      <c r="G70" s="28"/>
+      <c r="L70" s="28"/>
+      <c r="Q70" s="28"/>
+    </row>
+    <row r="71" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="2" t="s">
+      <c r="D71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="G70" s="21"/>
-      <c r="L70" s="21"/>
-      <c r="M70" s="17"/>
-      <c r="N70" s="17"/>
-      <c r="O70" s="17"/>
-      <c r="P70" s="17"/>
-      <c r="Q70" s="28"/>
-      <c r="R70" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A71" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="G71" s="21"/>
       <c r="L71" s="21"/>
@@ -3825,27 +3845,27 @@
       <c r="P71" s="17"/>
       <c r="Q71" s="28"/>
       <c r="R71" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>197</v>
+        <v>10</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>198</v>
+        <v>72</v>
       </c>
       <c r="D72" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E72" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>226</v>
+        <v>347</v>
       </c>
       <c r="G72" s="21"/>
       <c r="L72" s="21"/>
@@ -3854,212 +3874,215 @@
       <c r="O72" s="17"/>
       <c r="P72" s="17"/>
       <c r="Q72" s="28"/>
-    </row>
-    <row r="73" spans="1:18" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="25" t="s">
-        <v>292</v>
-      </c>
-      <c r="B73" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="D73" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="25" t="s">
-        <v>293</v>
+      <c r="R72" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="G73" s="21"/>
       <c r="L73" s="21"/>
+      <c r="M73" s="17"/>
+      <c r="N73" s="17"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="17"/>
       <c r="Q73" s="28"/>
-      <c r="R73" s="25" t="s">
+    </row>
+    <row r="74" spans="1:18" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A74" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="D74" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="G74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="Q74" s="28"/>
+      <c r="R74" s="25" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="74" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G74" s="21"/>
-      <c r="H74" s="2" t="s">
+      <c r="D75" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" s="21"/>
+      <c r="H75" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I74" s="31" t="s">
+      <c r="I75" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J74" s="31" t="s">
+      <c r="J75" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="K74" s="31" t="s">
+      <c r="K75" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="L74" s="21"/>
-      <c r="M74" s="45" t="s">
+      <c r="L75" s="21"/>
+      <c r="M75" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="N74" s="45" t="s">
+      <c r="N75" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="O74" s="45" t="s">
+      <c r="O75" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="P74" s="45" t="s">
+      <c r="P75" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="Q74" s="28"/>
-    </row>
-    <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A75" s="38" t="s">
+      <c r="Q75" s="28"/>
+    </row>
+    <row r="76" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B75" s="38" t="s">
+      <c r="B76" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="38" t="s">
+      <c r="C76" s="38" t="s">
         <v>343</v>
       </c>
-      <c r="D75" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="38"/>
-      <c r="G75" s="21"/>
-      <c r="L75" s="21"/>
-      <c r="M75" s="17"/>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="17"/>
-      <c r="Q75" s="28"/>
-    </row>
-    <row r="76" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D76" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="D76" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="38"/>
       <c r="G76" s="21"/>
       <c r="L76" s="21"/>
+      <c r="M76" s="17"/>
+      <c r="N76" s="17"/>
+      <c r="O76" s="17"/>
+      <c r="P76" s="17"/>
       <c r="Q76" s="28"/>
-      <c r="R76" s="7" t="s">
+    </row>
+    <row r="77" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D77" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" s="21"/>
+      <c r="L77" s="21"/>
+      <c r="Q77" s="28"/>
+      <c r="R77" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="42" t="s">
+    <row r="78" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A78" s="42" t="s">
         <v>355</v>
       </c>
-      <c r="B77" s="42" t="s">
+      <c r="B78" s="42" t="s">
         <v>356</v>
       </c>
-      <c r="C77" s="42" t="s">
+      <c r="C78" s="42" t="s">
         <v>357</v>
       </c>
-      <c r="D77" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="G77" s="28"/>
-      <c r="H77" s="42"/>
-      <c r="I77" s="42"/>
-      <c r="J77" s="42"/>
-      <c r="K77" s="42"/>
-      <c r="L77" s="28"/>
-      <c r="M77" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="N77" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="O77" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="P77" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q77" s="28"/>
-    </row>
-    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A78" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D78" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G78" s="21"/>
-      <c r="L78" s="21"/>
-      <c r="M78" s="17"/>
-      <c r="N78" s="17"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="17"/>
+      <c r="D78" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="28"/>
+      <c r="H78" s="42"/>
+      <c r="I78" s="42"/>
+      <c r="J78" s="42"/>
+      <c r="K78" s="42"/>
+      <c r="L78" s="28"/>
+      <c r="M78" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="N78" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="O78" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="P78" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="Q78" s="28"/>
     </row>
     <row r="79" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="D79" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G79" s="21"/>
       <c r="L79" s="21"/>
@@ -4069,447 +4092,447 @@
       <c r="P79" s="17"/>
       <c r="Q79" s="28"/>
     </row>
-    <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+      <c r="P80" s="17"/>
+      <c r="Q80" s="28"/>
+    </row>
+    <row r="81" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D80" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G80" s="21"/>
-      <c r="H80" s="17" t="s">
+      <c r="D81" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G81" s="21"/>
+      <c r="H81" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I80" s="17" t="s">
+      <c r="I81" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J80" s="17" t="s">
+      <c r="J81" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K80" s="17" t="s">
+      <c r="K81" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L80" s="21"/>
-      <c r="M80" s="45" t="s">
+      <c r="L81" s="21"/>
+      <c r="M81" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="N80" s="45" t="s">
+      <c r="N81" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="O80" s="45" t="s">
+      <c r="O81" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="P80" s="45" t="s">
+      <c r="P81" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="Q80" s="28"/>
-    </row>
-    <row r="81" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
+      <c r="Q81" s="28"/>
+    </row>
+    <row r="82" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="G81" s="21"/>
-      <c r="L81" s="21"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
-      <c r="Q81" s="28"/>
-    </row>
-    <row r="82" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D82" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="G82" s="21"/>
       <c r="L82" s="21"/>
+      <c r="M82" s="17"/>
+      <c r="N82" s="17"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="17"/>
       <c r="Q82" s="28"/>
-      <c r="R82" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A83" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>19</v>
+    </row>
+    <row r="83" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D83" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G83" s="21"/>
       <c r="L83" s="21"/>
-      <c r="M83" s="17"/>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
       <c r="Q83" s="28"/>
-    </row>
-    <row r="84" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A84" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D84" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>240</v>
+      <c r="R83" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G84" s="21"/>
       <c r="L84" s="21"/>
+      <c r="M84" s="17"/>
+      <c r="N84" s="17"/>
+      <c r="O84" s="17"/>
+      <c r="P84" s="17"/>
       <c r="Q84" s="28"/>
-      <c r="R84" s="8" t="s">
+    </row>
+    <row r="85" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A85" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D85" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G85" s="21"/>
+      <c r="L85" s="21"/>
+      <c r="Q85" s="28"/>
+      <c r="R85" s="8" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="85" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D85" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G85" s="21"/>
-      <c r="H85" s="2" t="s">
+      <c r="D86" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G86" s="21"/>
+      <c r="H86" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I86" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J85" s="17" t="s">
+      <c r="J86" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="K85" s="17" t="s">
+      <c r="K86" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="L85" s="21"/>
-      <c r="M85" s="17" t="s">
+      <c r="L86" s="21"/>
+      <c r="M86" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="N85" s="17" t="s">
+      <c r="N86" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="O85" s="17" t="s">
+      <c r="O86" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="P85" s="17" t="s">
+      <c r="P86" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="Q85" s="28"/>
-    </row>
-    <row r="86" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
+      <c r="Q86" s="28"/>
+    </row>
+    <row r="87" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2" t="s">
+      <c r="D87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="G86" s="21"/>
-      <c r="L86" s="21"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
-      <c r="Q86" s="28"/>
-    </row>
-    <row r="87" spans="1:19" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A87" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D87" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="G87" s="21"/>
       <c r="L87" s="21"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
       <c r="Q87" s="28"/>
-      <c r="R87" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="88" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A88" s="7" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D88" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E88" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="G88" s="21"/>
       <c r="L88" s="21"/>
       <c r="Q88" s="28"/>
-      <c r="R88" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>98</v>
+      <c r="R88" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A89" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D89" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G89" s="21"/>
       <c r="L89" s="21"/>
-      <c r="M89" s="17"/>
-      <c r="N89" s="17"/>
-      <c r="O89" s="17"/>
-      <c r="P89" s="17"/>
       <c r="Q89" s="28"/>
-    </row>
-    <row r="90" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R89" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G90" s="21"/>
+      <c r="L90" s="21"/>
+      <c r="M90" s="17"/>
+      <c r="N90" s="17"/>
+      <c r="O90" s="17"/>
+      <c r="P90" s="17"/>
+      <c r="Q90" s="28"/>
+    </row>
+    <row r="91" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G90" s="21"/>
-      <c r="H90" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K90" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L90" s="21"/>
-      <c r="M90" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N90" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O90" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P90" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q90" s="28"/>
-    </row>
-    <row r="91" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A91" s="2" t="s">
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G91" s="21"/>
+      <c r="H91" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L91" s="21"/>
+      <c r="M91" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N91" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O91" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P91" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q91" s="28"/>
+    </row>
+    <row r="92" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D91" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G91" s="21"/>
-      <c r="L91" s="21"/>
-      <c r="M91" s="17"/>
-      <c r="N91" s="17"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="17"/>
-      <c r="Q91" s="28"/>
-      <c r="R91" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="92" spans="1:19" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B92" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C92" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D92" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F92" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="G92" s="28"/>
-      <c r="L92" s="28"/>
+      <c r="D92" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G92" s="21"/>
+      <c r="L92" s="21"/>
+      <c r="M92" s="17"/>
+      <c r="N92" s="17"/>
+      <c r="O92" s="17"/>
+      <c r="P92" s="17"/>
       <c r="Q92" s="28"/>
       <c r="R92" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D93" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="G93" s="28"/>
+      <c r="L93" s="28"/>
+      <c r="Q93" s="28"/>
+      <c r="R93" s="8" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="93" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="2" t="s">
+    <row r="94" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D93" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="12" t="s">
+      <c r="D94" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="12" t="s">
         <v>290</v>
-      </c>
-      <c r="G93" s="21"/>
-      <c r="L93" s="21"/>
-      <c r="M93" s="17"/>
-      <c r="N93" s="17"/>
-      <c r="O93" s="17"/>
-      <c r="P93" s="17"/>
-      <c r="Q93" s="28"/>
-    </row>
-    <row r="94" spans="1:19" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="B94" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="C94" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D94" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="G94" s="21"/>
       <c r="L94" s="21"/>
@@ -4519,30 +4542,26 @@
       <c r="P94" s="17"/>
       <c r="Q94" s="28"/>
     </row>
-    <row r="95" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B95" t="s">
-        <v>10</v>
-      </c>
-      <c r="C95" t="s">
-        <v>329</v>
-      </c>
-      <c r="D95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>25</v>
+    <row r="95" spans="1:18" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D95" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="G95" s="21"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="17"/>
-      <c r="J95" s="17"/>
-      <c r="K95" s="17"/>
       <c r="L95" s="21"/>
       <c r="M95" s="17"/>
       <c r="N95" s="17"/>
@@ -4550,76 +4569,80 @@
       <c r="P95" s="17"/>
       <c r="Q95" s="28"/>
     </row>
-    <row r="96" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A96" t="s">
-        <v>327</v>
+    <row r="96" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="B96" t="s">
         <v>10</v>
       </c>
       <c r="C96" t="s">
+        <v>329</v>
+      </c>
+      <c r="D96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" s="21"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="17"/>
+      <c r="J96" s="17"/>
+      <c r="K96" s="17"/>
+      <c r="L96" s="21"/>
+      <c r="M96" s="17"/>
+      <c r="N96" s="17"/>
+      <c r="O96" s="17"/>
+      <c r="P96" s="17"/>
+      <c r="Q96" s="28"/>
+    </row>
+    <row r="97" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
+        <v>327</v>
+      </c>
+      <c r="B97" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" t="s">
         <v>328</v>
       </c>
-      <c r="D96" t="b">
-        <v>1</v>
-      </c>
-      <c r="E96" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="D97" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
         <v>25</v>
       </c>
-      <c r="G96" s="28"/>
-      <c r="L96" s="28"/>
-      <c r="Q96" s="28"/>
-      <c r="R96"/>
-      <c r="S96"/>
-    </row>
-    <row r="97" spans="1:19" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="2" t="s">
+      <c r="G97" s="28"/>
+      <c r="L97" s="28"/>
+      <c r="Q97" s="28"/>
+      <c r="R97"/>
+      <c r="S97"/>
+    </row>
+    <row r="98" spans="1:19" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B98" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D97" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G97" s="21"/>
-      <c r="L97" s="21"/>
-      <c r="M97" s="17"/>
-      <c r="N97" s="17"/>
-      <c r="O97" s="17"/>
-      <c r="P97" s="17"/>
-      <c r="Q97" s="28"/>
-    </row>
-    <row r="98" spans="1:19" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D98" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E98" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F98" s="6" t="s">
-        <v>241</v>
+      <c r="F98" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G98" s="21"/>
       <c r="L98" s="21"/>
@@ -4628,19 +4651,16 @@
       <c r="O98" s="17"/>
       <c r="P98" s="17"/>
       <c r="Q98" s="28"/>
-      <c r="R98" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="99" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="99" spans="1:19" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D99" s="2" t="b">
         <v>0</v>
@@ -4648,8 +4668,8 @@
       <c r="E99" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F99" s="2" t="s">
-        <v>16</v>
+      <c r="F99" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="G99" s="21"/>
       <c r="L99" s="21"/>
@@ -4658,22 +4678,28 @@
       <c r="O99" s="17"/>
       <c r="P99" s="17"/>
       <c r="Q99" s="28"/>
-    </row>
-    <row r="100" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R99" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D100" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E100" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G100" s="21"/>
       <c r="L100" s="21"/>
@@ -4682,28 +4708,22 @@
       <c r="O100" s="17"/>
       <c r="P100" s="17"/>
       <c r="Q100" s="28"/>
-      <c r="R100" s="8" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="101" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="101" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="D101" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="G101" s="21"/>
       <c r="L101" s="21"/>
@@ -4713,91 +4733,95 @@
       <c r="P101" s="17"/>
       <c r="Q101" s="28"/>
       <c r="R101" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A102" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D102" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G102" s="21"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="17"/>
+      <c r="N102" s="17"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="17"/>
+      <c r="Q102" s="28"/>
+      <c r="R102" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="102" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
+    <row r="103" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G102" s="21"/>
-      <c r="H102" s="17" t="s">
+      <c r="D103" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G103" s="21"/>
+      <c r="H103" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I102" s="17" t="s">
+      <c r="I103" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J102" s="17" t="s">
+      <c r="J103" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K102" s="17" t="s">
+      <c r="K103" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L102" s="21"/>
-      <c r="M102" s="18" t="s">
+      <c r="L103" s="21"/>
+      <c r="M103" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="N102" s="45" t="s">
+      <c r="N103" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="O102" s="45" t="s">
+      <c r="O103" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="P102" s="45" t="s">
+      <c r="P103" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="Q102" s="28"/>
-      <c r="R102" s="2" t="s">
+      <c r="Q103" s="28"/>
+      <c r="R103" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="103" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A103" s="7" t="s">
+    <row r="104" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A104" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B104" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C104" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D103" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G103" s="21"/>
-      <c r="L103" s="21"/>
-      <c r="Q103" s="28"/>
-      <c r="R103" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="104" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B104" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="D104" s="7" t="b">
         <v>1</v>
@@ -4812,91 +4836,73 @@
       <c r="L104" s="21"/>
       <c r="Q104" s="28"/>
       <c r="R104" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="105" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D105" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E105" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="G105" s="21"/>
       <c r="L105" s="21"/>
       <c r="Q105" s="28"/>
       <c r="R105" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D106" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" s="21"/>
+      <c r="L106" s="21"/>
+      <c r="Q106" s="28"/>
+      <c r="R106" s="7" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="106" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D106" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E106" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G106" s="21"/>
-      <c r="H106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K106" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L106" s="21"/>
-      <c r="M106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P106" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q106" s="28"/>
     </row>
     <row r="107" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D107" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107" s="2" t="b">
         <v>1</v>
@@ -4931,23 +4937,23 @@
     </row>
     <row r="108" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D108" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G108" s="21"/>
       <c r="H108" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>4</v>
@@ -4960,7 +4966,7 @@
       </c>
       <c r="L108" s="21"/>
       <c r="M108" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N108" s="17" t="s">
         <v>4</v>
@@ -4973,148 +4979,145 @@
       </c>
       <c r="Q108" s="28"/>
     </row>
-    <row r="109" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C109" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D109" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" s="21"/>
+      <c r="H109" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L109" s="21"/>
+      <c r="M109" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P109" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="28"/>
+    </row>
+    <row r="110" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A110" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D109" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G109" s="21"/>
-      <c r="L109" s="21"/>
-      <c r="M109" s="17"/>
-      <c r="N109" s="17"/>
-      <c r="O109" s="17"/>
-      <c r="P109" s="17"/>
-      <c r="Q109" s="28"/>
-    </row>
-    <row r="110" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A110" t="s">
+      <c r="D110" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G110" s="21"/>
+      <c r="L110" s="21"/>
+      <c r="M110" s="17"/>
+      <c r="N110" s="17"/>
+      <c r="O110" s="17"/>
+      <c r="P110" s="17"/>
+      <c r="Q110" s="28"/>
+    </row>
+    <row r="111" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
         <v>330</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>5</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>331</v>
       </c>
-      <c r="D110" t="b">
-        <v>0</v>
-      </c>
-      <c r="E110" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" t="s">
-        <v>4</v>
-      </c>
-      <c r="G110" s="28"/>
-      <c r="H110"/>
-      <c r="I110"/>
-      <c r="J110"/>
-      <c r="K110"/>
-      <c r="L110" s="28"/>
-      <c r="M110"/>
-      <c r="N110"/>
-      <c r="O110"/>
-      <c r="P110"/>
-      <c r="Q110" s="24"/>
-      <c r="R110"/>
-      <c r="S110"/>
-    </row>
-    <row r="111" spans="1:19" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A111" s="7" t="s">
+      <c r="D111" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" t="s">
+        <v>4</v>
+      </c>
+      <c r="G111" s="28"/>
+      <c r="H111"/>
+      <c r="I111"/>
+      <c r="J111"/>
+      <c r="K111"/>
+      <c r="L111" s="28"/>
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+      <c r="P111"/>
+      <c r="Q111" s="24"/>
+      <c r="R111"/>
+      <c r="S111"/>
+    </row>
+    <row r="112" spans="1:19" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A112" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B112" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C112" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D111" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G111" s="21"/>
-      <c r="L111" s="21"/>
-      <c r="Q111" s="28"/>
-      <c r="R111" s="7" t="s">
+      <c r="D112" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" s="21"/>
+      <c r="L112" s="21"/>
+      <c r="Q112" s="28"/>
+      <c r="R112" s="7" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="112" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G112" s="21"/>
-      <c r="H112" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L112" s="21"/>
-      <c r="M112" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P112" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q112" s="28"/>
-      <c r="R112" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="113" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
-        <v>277</v>
+        <v>129</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D113" s="2" t="b">
         <v>1</v>
@@ -5149,138 +5152,182 @@
         <v>4</v>
       </c>
       <c r="Q113" s="28"/>
+      <c r="R113" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="114" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G114" s="21"/>
+      <c r="H114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L114" s="21"/>
+      <c r="M114" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q114" s="28"/>
+    </row>
+    <row r="115" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F114" s="2" t="s">
+      <c r="D115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G114" s="21"/>
-      <c r="L114" s="21"/>
-      <c r="M114" s="17"/>
-      <c r="N114" s="17"/>
-      <c r="O114" s="17"/>
-      <c r="P114" s="17"/>
-      <c r="Q114" s="28"/>
-    </row>
-    <row r="115" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="43" t="s">
+      <c r="G115" s="21"/>
+      <c r="L115" s="21"/>
+      <c r="M115" s="17"/>
+      <c r="N115" s="17"/>
+      <c r="O115" s="17"/>
+      <c r="P115" s="17"/>
+      <c r="Q115" s="28"/>
+    </row>
+    <row r="116" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="B115" s="43" t="s">
+      <c r="B116" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C115" s="43" t="s">
+      <c r="C116" s="43" t="s">
         <v>360</v>
       </c>
-      <c r="D115" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G115" s="28"/>
-      <c r="H115" s="43" t="s">
+      <c r="D116" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G116" s="28"/>
+      <c r="H116" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I115" s="43" t="s">
+      <c r="I116" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="J115" s="43" t="s">
+      <c r="J116" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="K115" s="43" t="s">
+      <c r="K116" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="L115" s="28"/>
-      <c r="M115" s="45" t="s">
+      <c r="L116" s="28"/>
+      <c r="M116" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="N115" s="45" t="s">
+      <c r="N116" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="O115" s="45" t="s">
+      <c r="O116" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="P115" s="45" t="s">
+      <c r="P116" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="Q115" s="28"/>
-    </row>
-    <row r="116" spans="1:18" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A116" s="27" t="s">
+      <c r="Q116" s="28"/>
+    </row>
+    <row r="117" spans="1:18" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A117" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="B116" s="27" t="s">
+      <c r="B117" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C116" s="27" t="s">
+      <c r="C117" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="D116" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" s="27" t="s">
+      <c r="D117" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="G116" s="28"/>
-      <c r="H116" s="27"/>
-      <c r="I116" s="27"/>
-      <c r="J116" s="27"/>
-      <c r="K116" s="27"/>
-      <c r="L116" s="28"/>
-      <c r="M116" s="27"/>
-      <c r="Q116" s="28"/>
-    </row>
-    <row r="117" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A117" s="2" t="s">
+      <c r="G117" s="28"/>
+      <c r="H117" s="27"/>
+      <c r="I117" s="27"/>
+      <c r="J117" s="27"/>
+      <c r="K117" s="27"/>
+      <c r="L117" s="28"/>
+      <c r="M117" s="27"/>
+      <c r="Q117" s="28"/>
+    </row>
+    <row r="118" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A118" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D117" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F117" s="2" t="s">
+      <c r="D118" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="G117" s="21"/>
-      <c r="L117" s="21"/>
-      <c r="M117" s="17"/>
-      <c r="N117" s="17"/>
-      <c r="O117" s="17"/>
-      <c r="P117" s="17"/>
-      <c r="Q117" s="28"/>
-      <c r="R117" s="2" t="s">
+      <c r="G118" s="21"/>
+      <c r="L118" s="21"/>
+      <c r="M118" s="17"/>
+      <c r="N118" s="17"/>
+      <c r="O118" s="17"/>
+      <c r="P118" s="17"/>
+      <c r="Q118" s="28"/>
+      <c r="R118" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R118"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R119"/>
@@ -5344,6 +5391,9 @@
     </row>
     <row r="139" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R139"/>
+    </row>
+    <row r="140" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R140"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5359,7 +5409,7 @@
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1"/>
     <hyperlink ref="F21" r:id="rId2"/>
-    <hyperlink ref="F60" r:id="rId3"/>
+    <hyperlink ref="F61" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
[kadaster] introductie XLinks profile via xlinkversion=
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="370">
   <si>
     <t>Name</t>
   </si>
@@ -1123,6 +1123,18 @@
   </si>
   <si>
     <t>Should a full respec version be generated along with the catalog?</t>
+  </si>
+  <si>
+    <t>xlinkversion</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Version of the xlinks specification</t>
+  </si>
+  <si>
+    <t>KADPROFILE</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1279,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1366,6 +1378,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1687,13 +1702,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S140"/>
+  <dimension ref="A1:S141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
+      <selection pane="bottomRight" activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1903,16 +1918,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="47" t="b">
+      <c r="D7" s="48" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1930,10 +1945,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -3144,16 +3159,16 @@
       </c>
     </row>
     <row r="46" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="47" t="s">
+      <c r="A46" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="47" t="s">
+      <c r="C46" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="47" t="b">
+      <c r="D46" s="48" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="2" t="b">
@@ -3171,10 +3186,10 @@
       <c r="Q46" s="28"/>
     </row>
     <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="47"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
       <c r="G47" s="21"/>
       <c r="L47" s="21"/>
       <c r="M47" s="17"/>
@@ -5271,66 +5286,86 @@
       </c>
       <c r="Q116" s="28"/>
     </row>
-    <row r="117" spans="1:18" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A117" s="27" t="s">
+    <row r="117" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="47" t="s">
+        <v>366</v>
+      </c>
+      <c r="B117" s="47" t="s">
+        <v>367</v>
+      </c>
+      <c r="C117" s="47" t="s">
+        <v>368</v>
+      </c>
+      <c r="D117" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E117" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117" s="47" t="s">
+        <v>369</v>
+      </c>
+      <c r="G117" s="28"/>
+      <c r="L117" s="28"/>
+      <c r="Q117" s="28"/>
+    </row>
+    <row r="118" spans="1:18" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A118" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="B117" s="27" t="s">
+      <c r="B118" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C117" s="27" t="s">
+      <c r="C118" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="D117" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F117" s="27" t="s">
+      <c r="D118" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F118" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="G117" s="28"/>
-      <c r="H117" s="27"/>
-      <c r="I117" s="27"/>
-      <c r="J117" s="27"/>
-      <c r="K117" s="27"/>
-      <c r="L117" s="28"/>
-      <c r="M117" s="27"/>
-      <c r="Q117" s="28"/>
-    </row>
-    <row r="118" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A118" s="2" t="s">
+      <c r="G118" s="28"/>
+      <c r="H118" s="27"/>
+      <c r="I118" s="27"/>
+      <c r="J118" s="27"/>
+      <c r="K118" s="27"/>
+      <c r="L118" s="28"/>
+      <c r="M118" s="27"/>
+      <c r="Q118" s="28"/>
+    </row>
+    <row r="119" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A119" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D118" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E118" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F118" s="2" t="s">
+      <c r="D119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="G118" s="21"/>
-      <c r="L118" s="21"/>
-      <c r="M118" s="17"/>
-      <c r="N118" s="17"/>
-      <c r="O118" s="17"/>
-      <c r="P118" s="17"/>
-      <c r="Q118" s="28"/>
-      <c r="R118" s="2" t="s">
+      <c r="G119" s="21"/>
+      <c r="L119" s="21"/>
+      <c r="M119" s="17"/>
+      <c r="N119" s="17"/>
+      <c r="O119" s="17"/>
+      <c r="P119" s="17"/>
+      <c r="Q119" s="28"/>
+      <c r="R119" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="R119"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.4">
       <c r="R120"/>
@@ -5394,6 +5429,9 @@
     </row>
     <row r="140" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R140"/>
+    </row>
+    <row r="141" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R141"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
[kadaster] Compacte respec, en nooit een listing sectie
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -1720,10 +1720,10 @@
   <dimension ref="A1:S143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F79" sqref="F79"/>
+      <selection pane="bottomRight" activeCell="M52" sqref="M52:P52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3365,16 +3365,16 @@
       </c>
       <c r="L52" s="22"/>
       <c r="M52" s="6" t="s">
-        <v>25</v>
+        <v>324</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>25</v>
+        <v>324</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>25</v>
+        <v>324</v>
       </c>
       <c r="P52" s="6" t="s">
-        <v>25</v>
+        <v>324</v>
       </c>
       <c r="Q52" s="22"/>
     </row>

</xml_diff>

<commit_message>
[kadaster] createmimformat stanaadrd op "no"
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -1720,10 +1720,10 @@
   <dimension ref="A1:S143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M52" sqref="M52:P52"/>
+      <selection pane="bottomRight" activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2797,13 +2797,13 @@
         <v>16</v>
       </c>
       <c r="N33" s="48" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O33" s="48" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="P33" s="48" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="Q33" s="28"/>
     </row>

</xml_diff>

<commit_message>
[Kadaster] Default settings voor mimformat toegevoegd aan excel
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="377">
   <si>
     <t>Name</t>
   </si>
@@ -1147,6 +1147,15 @@
   </si>
   <si>
     <t>The name of the MIM format file generated</t>
+  </si>
+  <si>
+    <t>createmimformatname</t>
+  </si>
+  <si>
+    <t>xml|rdf-xml|turtle|legacy</t>
+  </si>
+  <si>
+    <t>The type of the MIM format file generated</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1300,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1390,6 +1399,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1717,19 +1729,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S143"/>
+  <dimension ref="A1:S144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P33" sqref="P33"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="23.84375" customWidth="1"/>
-    <col min="2" max="2" width="19.3046875" customWidth="1"/>
+    <col min="2" max="2" width="29.3046875" customWidth="1"/>
     <col min="3" max="3" width="50.69140625" customWidth="1"/>
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
@@ -1933,16 +1945,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="49" t="b">
+      <c r="D7" s="50" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1960,10 +1972,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="49"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -2797,61 +2809,57 @@
         <v>16</v>
       </c>
       <c r="N33" s="48" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O33" s="48" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="P33" s="48" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="Q33" s="28"/>
     </row>
-    <row r="34" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
+    <row r="34" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="49" t="s">
+        <v>374</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>375</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>376</v>
+      </c>
+      <c r="D34" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>358</v>
+      </c>
+      <c r="G34" s="28"/>
+      <c r="L34" s="28"/>
       <c r="Q34" s="28"/>
-      <c r="R34" s="2" t="s">
-        <v>211</v>
-      </c>
     </row>
     <row r="35" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>173</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>174</v>
+        <v>36</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>175</v>
+        <v>37</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="G35" s="21"/>
       <c r="L35" s="21"/>
@@ -2860,16 +2868,19 @@
       <c r="O35" s="17"/>
       <c r="P35" s="17"/>
       <c r="Q35" s="28"/>
-    </row>
-    <row r="36" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R35" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D36" s="2" t="b">
         <v>0</v>
@@ -2885,321 +2896,319 @@
       <c r="P36" s="17"/>
       <c r="Q36" s="28"/>
     </row>
-    <row r="37" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A37" s="34" t="s">
+    <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="28"/>
+    </row>
+    <row r="38" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A38" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B38" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C38" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="D37" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="34" t="s">
+      <c r="D38" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="34" t="s">
         <v>323</v>
       </c>
-      <c r="G37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="Q37" s="28"/>
-    </row>
-    <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="2" t="s">
+      <c r="G38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="Q38" s="28"/>
+    </row>
+    <row r="39" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" s="21"/>
-      <c r="H38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L38" s="21"/>
-      <c r="M38" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P38" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q38" s="28"/>
-    </row>
-    <row r="39" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="35" t="s">
+      <c r="D39" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="21"/>
+      <c r="H39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L39" s="21"/>
+      <c r="M39" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P39" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q39" s="28"/>
+    </row>
+    <row r="40" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="35" t="s">
         <v>325</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B40" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C40" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="D39" s="35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="Q39" s="28"/>
-      <c r="R39"/>
-    </row>
-    <row r="40" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A40" s="2" t="s">
+      <c r="D40" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="Q40" s="28"/>
+      <c r="R40"/>
+    </row>
+    <row r="41" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="21"/>
-      <c r="H40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L40" s="21"/>
-      <c r="M40" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N40" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O40" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P40" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q40" s="28"/>
-    </row>
-    <row r="41" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A41" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G41" s="21"/>
+      <c r="H41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L41" s="21"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
+      <c r="M41" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O41" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P41" s="17" t="s">
+        <v>4</v>
+      </c>
       <c r="Q41" s="28"/>
     </row>
-    <row r="42" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="28"/>
+    </row>
+    <row r="43" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42" s="21"/>
-      <c r="H42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L42" s="21"/>
-      <c r="M42" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N42" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O42" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P42" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q42" s="28"/>
-    </row>
-    <row r="43" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A43" s="31" t="s">
+      <c r="D43" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" s="21"/>
+      <c r="H43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L43" s="21"/>
+      <c r="M43" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O43" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P43" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q43" s="28"/>
+    </row>
+    <row r="44" spans="1:18" s="31" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A44" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B44" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C44" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="D43" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G43" s="28"/>
-      <c r="H43" s="31" t="s">
+      <c r="D44" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="28"/>
+      <c r="H44" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="I43" s="33" t="s">
+      <c r="I44" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="J43" s="33" t="s">
+      <c r="J44" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="K43" s="33" t="s">
+      <c r="K44" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="L43" s="28"/>
-      <c r="M43" s="31" t="s">
+      <c r="L44" s="28"/>
+      <c r="M44" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="N43" s="32" t="s">
+      <c r="N44" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="O43" s="32" t="s">
+      <c r="O44" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="P43" s="32" t="s">
+      <c r="P44" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="Q43" s="28"/>
-      <c r="R43" s="31" t="s">
+      <c r="Q44" s="28"/>
+      <c r="R44" s="31" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D44" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="21"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="17"/>
-      <c r="O44" s="17"/>
-      <c r="P44" s="17"/>
-      <c r="Q44" s="28"/>
-    </row>
-    <row r="45" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A45" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F45" s="7" t="s">
+      <c r="D45" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="21"/>
       <c r="L45" s="21"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
       <c r="Q45" s="28"/>
-      <c r="R45" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="46" spans="1:18" s="7" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A46" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D46" s="7" t="b">
         <v>1</v>
@@ -3208,47 +3217,60 @@
         <v>0</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>250</v>
+        <v>16</v>
       </c>
       <c r="G46" s="21"/>
       <c r="L46" s="21"/>
       <c r="Q46" s="28"/>
       <c r="R46" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>16</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A47" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="G47" s="21"/>
       <c r="L47" s="21"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="17"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="17"/>
       <c r="Q47" s="28"/>
+      <c r="R47" s="7" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="49"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
+      <c r="A48" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G48" s="21"/>
       <c r="L48" s="21"/>
       <c r="M48" s="17"/>
@@ -3257,22 +3279,11 @@
       <c r="P48" s="17"/>
       <c r="Q48" s="28"/>
     </row>
-    <row r="49" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A49" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D49" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="2" t="b">
-        <v>0</v>
-      </c>
+    <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="50"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
       <c r="G49" s="21"/>
       <c r="L49" s="21"/>
       <c r="M49" s="17"/>
@@ -3281,24 +3292,21 @@
       <c r="P49" s="17"/>
       <c r="Q49" s="28"/>
     </row>
-    <row r="50" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D50" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E50" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G50" s="21"/>
       <c r="L50" s="21"/>
@@ -3308,15 +3316,15 @@
       <c r="P50" s="17"/>
       <c r="Q50" s="28"/>
     </row>
-    <row r="51" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D51" s="2" t="b">
         <v>0</v>
@@ -3324,96 +3332,97 @@
       <c r="E51" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G51" s="22"/>
-      <c r="L51" s="22"/>
+      <c r="F51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="21"/>
+      <c r="L51" s="21"/>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
       <c r="O51" s="17"/>
       <c r="P51" s="17"/>
       <c r="Q51" s="28"/>
-      <c r="R51" s="2" t="s">
+    </row>
+    <row r="52" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+      <c r="Q52" s="28"/>
+      <c r="R52" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="52" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A53" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E52" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G52" s="22"/>
-      <c r="H52" s="6" t="s">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="22"/>
+      <c r="H53" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="I52" s="6" t="s">
+      <c r="I53" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="J52" s="6" t="s">
+      <c r="J53" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="K52" s="6" t="s">
+      <c r="K53" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="L52" s="22"/>
-      <c r="M52" s="6" t="s">
+      <c r="L53" s="22"/>
+      <c r="M53" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="N52" s="6" t="s">
+      <c r="N53" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="O52" s="6" t="s">
+      <c r="O53" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="P52" s="6" t="s">
+      <c r="P53" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="Q52" s="22"/>
-    </row>
-    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="7" t="s">
+      <c r="Q53" s="22"/>
+    </row>
+    <row r="54" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B54" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C54" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D53" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G53" s="21"/>
-      <c r="L53" s="21"/>
-      <c r="Q53" s="28"/>
-      <c r="R53" s="8" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A54" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="D54" s="7" t="b">
         <v>0</v>
       </c>
@@ -3421,48 +3430,47 @@
         <v>1</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>238</v>
+        <v>4</v>
       </c>
       <c r="G54" s="21"/>
       <c r="L54" s="21"/>
       <c r="Q54" s="28"/>
-    </row>
-    <row r="55" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D55" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>16</v>
+      <c r="R54" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A55" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D55" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="G55" s="21"/>
       <c r="L55" s="21"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="17"/>
       <c r="Q55" s="28"/>
     </row>
     <row r="56" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D56" s="2" t="b">
         <v>0</v>
@@ -3481,227 +3489,231 @@
       <c r="P56" s="17"/>
       <c r="Q56" s="28"/>
     </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="7" t="s">
+    <row r="57" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="C57" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G57" s="21"/>
       <c r="L57" s="21"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
       <c r="Q57" s="28"/>
-      <c r="R57" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B58" s="2" t="s">
+    </row>
+    <row r="58" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A58" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D58" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="2" t="s">
+      <c r="C58" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G58" s="21"/>
       <c r="L58" s="21"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="17"/>
       <c r="Q58" s="28"/>
-    </row>
-    <row r="59" spans="1:18" s="46" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A59" s="46" t="s">
+      <c r="R58" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="21"/>
+      <c r="L59" s="21"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="28"/>
+    </row>
+    <row r="60" spans="1:18" s="46" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A60" s="46" t="s">
         <v>364</v>
       </c>
-      <c r="B59" s="46" t="s">
+      <c r="B60" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="46" t="s">
+      <c r="C60" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="D59" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="G59" s="28"/>
-      <c r="I59" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J59" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="K59" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="L59" s="28"/>
-      <c r="N59" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="O59" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="P59" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q59" s="28"/>
-    </row>
-    <row r="60" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A60" s="16" t="s">
+      <c r="D60" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="28"/>
+      <c r="I60" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="J60" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K60" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="L60" s="28"/>
+      <c r="N60" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="O60" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="P60" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q60" s="28"/>
+    </row>
+    <row r="61" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A61" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B61" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C61" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="D60" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="16" t="s">
+      <c r="D61" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="G60" s="23"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="16"/>
-      <c r="K60" s="16"/>
-      <c r="L60" s="23"/>
-      <c r="M60" s="16"/>
-      <c r="N60" s="16"/>
-      <c r="O60" s="16"/>
-      <c r="P60" s="16"/>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="16"/>
-    </row>
-    <row r="61" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="7" t="s">
+      <c r="G61" s="23"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="16"/>
+    </row>
+    <row r="62" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="D61" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="7" t="s">
+      <c r="D62" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="G61" s="28"/>
-      <c r="L61" s="28"/>
-      <c r="Q61" s="28"/>
-    </row>
-    <row r="62" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A62" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="D62" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="37" t="s">
-        <v>341</v>
-      </c>
       <c r="G62" s="28"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="37"/>
       <c r="L62" s="28"/>
-      <c r="M62" s="37"/>
-      <c r="N62" s="37"/>
-      <c r="O62" s="37"/>
-      <c r="P62" s="37"/>
       <c r="Q62" s="28"/>
     </row>
     <row r="63" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A63" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D63" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="37" t="s">
+        <v>341</v>
+      </c>
+      <c r="G63" s="28"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="28"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
+      <c r="O63" s="37"/>
+      <c r="P63" s="37"/>
+      <c r="Q63" s="28"/>
+    </row>
+    <row r="64" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A64" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B64" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C64" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D63" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="7" t="s">
+      <c r="D64" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="7" t="s">
         <v>342</v>
-      </c>
-      <c r="G63" s="28"/>
-      <c r="L63" s="28"/>
-      <c r="Q63" s="28"/>
-    </row>
-    <row r="64" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>350</v>
-      </c>
-      <c r="B64" t="s">
-        <v>82</v>
-      </c>
-      <c r="C64" t="s">
-        <v>352</v>
-      </c>
-      <c r="D64" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="s">
-        <v>358</v>
       </c>
       <c r="G64" s="28"/>
       <c r="L64" s="28"/>
@@ -3709,13 +3721,13 @@
     </row>
     <row r="65" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B65" t="s">
         <v>82</v>
       </c>
       <c r="C65" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -3724,222 +3736,215 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="G65" s="28"/>
       <c r="L65" s="28"/>
       <c r="Q65" s="28"/>
     </row>
-    <row r="66" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" s="16" t="s">
+    <row r="66" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>351</v>
+      </c>
+      <c r="B66" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" t="s">
+        <v>353</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>354</v>
+      </c>
+      <c r="G66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="Q66" s="28"/>
+    </row>
+    <row r="67" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B67" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C67" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="D66" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="16" t="s">
+      <c r="D67" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="G66" s="23"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-      <c r="L66" s="23"/>
-      <c r="M66" s="16"/>
-      <c r="N66" s="16"/>
-      <c r="O66" s="16"/>
-      <c r="P66" s="16"/>
-      <c r="Q66" s="23"/>
-      <c r="R66" s="16" t="s">
+      <c r="G67" s="23"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="16"/>
+      <c r="P67" s="16"/>
+      <c r="Q67" s="23"/>
+      <c r="R67" s="16" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="67" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="7" t="s">
+    <row r="68" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A68" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B68" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C68" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D67" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="7" t="s">
+      <c r="D68" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="G67" s="21"/>
-      <c r="L67" s="21"/>
-      <c r="Q67" s="28"/>
-      <c r="R67" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="G68" s="21"/>
       <c r="L68" s="21"/>
-      <c r="M68" s="17"/>
-      <c r="N68" s="17"/>
-      <c r="O68" s="17"/>
-      <c r="P68" s="17"/>
       <c r="Q68" s="28"/>
-      <c r="R68" s="2" t="s">
+      <c r="R68" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="17"/>
+      <c r="N69" s="17"/>
+      <c r="O69" s="17"/>
+      <c r="P69" s="17"/>
+      <c r="Q69" s="28"/>
+      <c r="R69" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="69" spans="1:18" s="39" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
+    <row r="70" spans="1:18" s="39" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
         <v>344</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>5</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C70" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="D69" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="G69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="Q69" s="28"/>
-    </row>
-    <row r="70" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="7" t="s">
+      <c r="D70" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="28"/>
+      <c r="L70" s="28"/>
+      <c r="Q70" s="28"/>
+    </row>
+    <row r="71" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D70" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="7" t="s">
+      <c r="D71" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="G70" s="21"/>
-      <c r="L70" s="21"/>
-      <c r="Q70" s="28"/>
-      <c r="R70" s="7" t="s">
+      <c r="G71" s="21"/>
+      <c r="L71" s="21"/>
+      <c r="Q71" s="28"/>
+      <c r="R71" s="7" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="71" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" t="s">
+    <row r="72" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
         <v>301</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>82</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>302</v>
       </c>
-      <c r="D71" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
         <v>260</v>
       </c>
-      <c r="G71" s="28"/>
-      <c r="L71" s="28"/>
-      <c r="Q71" s="28"/>
-    </row>
-    <row r="72" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="2" t="s">
+      <c r="G72" s="28"/>
+      <c r="L72" s="28"/>
+      <c r="Q72" s="28"/>
+    </row>
+    <row r="73" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="D73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="G72" s="21"/>
-      <c r="L72" s="21"/>
-      <c r="M72" s="17"/>
-      <c r="N72" s="17"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="17"/>
-      <c r="Q72" s="28"/>
-      <c r="R72" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A73" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>347</v>
       </c>
       <c r="G73" s="21"/>
       <c r="L73" s="21"/>
@@ -3949,27 +3954,27 @@
       <c r="P73" s="17"/>
       <c r="Q73" s="28"/>
       <c r="R73" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" s="2" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>196</v>
+        <v>71</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>197</v>
+        <v>10</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>198</v>
+        <v>72</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E74" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>226</v>
+        <v>347</v>
       </c>
       <c r="G74" s="21"/>
       <c r="L74" s="21"/>
@@ -3978,235 +3983,238 @@
       <c r="O74" s="17"/>
       <c r="P74" s="17"/>
       <c r="Q74" s="28"/>
-    </row>
-    <row r="75" spans="1:18" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A75" s="25" t="s">
-        <v>292</v>
-      </c>
-      <c r="B75" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="D75" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="25" t="s">
-        <v>293</v>
+      <c r="R74" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A75" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D75" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="G75" s="21"/>
       <c r="L75" s="21"/>
+      <c r="M75" s="17"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
       <c r="Q75" s="28"/>
-      <c r="R75" s="25" t="s">
+    </row>
+    <row r="76" spans="1:18" s="25" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="25" t="s">
+        <v>292</v>
+      </c>
+      <c r="B76" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="D76" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="G76" s="21"/>
+      <c r="L76" s="21"/>
+      <c r="Q76" s="28"/>
+      <c r="R76" s="25" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="76" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D76" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G76" s="21"/>
-      <c r="H76" s="2" t="s">
+      <c r="D77" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G77" s="21"/>
+      <c r="H77" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I76" s="31" t="s">
+      <c r="I77" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J76" s="31" t="s">
+      <c r="J77" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="K76" s="31" t="s">
+      <c r="K77" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="L76" s="21"/>
-      <c r="M76" s="45" t="s">
+      <c r="L77" s="21"/>
+      <c r="M77" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="N76" s="45" t="s">
+      <c r="N77" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="O76" s="45" t="s">
+      <c r="O77" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="P76" s="45" t="s">
+      <c r="P77" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="Q76" s="28"/>
-    </row>
-    <row r="77" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="38" t="s">
+      <c r="Q77" s="28"/>
+    </row>
+    <row r="78" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A78" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B77" s="38" t="s">
+      <c r="B78" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C77" s="38" t="s">
+      <c r="C78" s="38" t="s">
         <v>343</v>
       </c>
-      <c r="D77" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="38"/>
-      <c r="G77" s="21"/>
-      <c r="L77" s="21"/>
-      <c r="M77" s="17"/>
-      <c r="N77" s="17"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="17"/>
-      <c r="Q77" s="28"/>
-    </row>
-    <row r="78" spans="1:18" s="48" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="48" t="s">
+      <c r="D78" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" s="38"/>
+      <c r="G78" s="21"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="17"/>
+      <c r="N78" s="17"/>
+      <c r="O78" s="17"/>
+      <c r="P78" s="17"/>
+      <c r="Q78" s="28"/>
+    </row>
+    <row r="79" spans="1:18" s="48" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="48" t="s">
         <v>372</v>
       </c>
-      <c r="B78" s="48" t="s">
+      <c r="B79" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="48" t="s">
+      <c r="C79" s="48" t="s">
         <v>373</v>
       </c>
-      <c r="D78" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" s="48" t="s">
+      <c r="D79" s="48" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" s="48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" s="48" t="s">
         <v>260</v>
       </c>
-      <c r="G78" s="28"/>
-      <c r="L78" s="28"/>
-      <c r="Q78" s="28"/>
-    </row>
-    <row r="79" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A79" s="7" t="s">
+      <c r="G79" s="28"/>
+      <c r="L79" s="28"/>
+      <c r="Q79" s="28"/>
+    </row>
+    <row r="80" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A80" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B80" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D79" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G79" s="21"/>
-      <c r="L79" s="21"/>
-      <c r="Q79" s="28"/>
-      <c r="R79" s="7" t="s">
+      <c r="D80" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="Q80" s="28"/>
+      <c r="R80" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="80" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="42" t="s">
+    <row r="81" spans="1:18" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="42" t="s">
         <v>355</v>
       </c>
-      <c r="B80" s="42" t="s">
+      <c r="B81" s="42" t="s">
         <v>356</v>
       </c>
-      <c r="C80" s="42" t="s">
+      <c r="C81" s="42" t="s">
         <v>357</v>
       </c>
-      <c r="D80" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="G80" s="28"/>
-      <c r="H80" s="42"/>
-      <c r="I80" s="42"/>
-      <c r="J80" s="42"/>
-      <c r="K80" s="42"/>
-      <c r="L80" s="28"/>
-      <c r="M80" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="N80" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="O80" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="P80" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q80" s="28"/>
-    </row>
-    <row r="81" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D81" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G81" s="21"/>
-      <c r="L81" s="21"/>
-      <c r="M81" s="17"/>
-      <c r="N81" s="17"/>
-      <c r="O81" s="17"/>
-      <c r="P81" s="17"/>
+      <c r="D81" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="28"/>
+      <c r="H81" s="42"/>
+      <c r="I81" s="42"/>
+      <c r="J81" s="42"/>
+      <c r="K81" s="42"/>
+      <c r="L81" s="28"/>
+      <c r="M81" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="N81" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="O81" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="P81" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="Q81" s="28"/>
     </row>
     <row r="82" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="D82" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G82" s="21"/>
       <c r="L82" s="21"/>
@@ -4216,447 +4224,447 @@
       <c r="P82" s="17"/>
       <c r="Q82" s="28"/>
     </row>
-    <row r="83" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" s="21"/>
+      <c r="L83" s="21"/>
+      <c r="M83" s="17"/>
+      <c r="N83" s="17"/>
+      <c r="O83" s="17"/>
+      <c r="P83" s="17"/>
+      <c r="Q83" s="28"/>
+    </row>
+    <row r="84" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D83" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G83" s="21"/>
-      <c r="H83" s="17" t="s">
+      <c r="D84" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G84" s="21"/>
+      <c r="H84" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I83" s="17" t="s">
+      <c r="I84" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J83" s="17" t="s">
+      <c r="J84" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K83" s="17" t="s">
+      <c r="K84" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L83" s="21"/>
-      <c r="M83" s="45" t="s">
+      <c r="L84" s="21"/>
+      <c r="M84" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="N83" s="45" t="s">
+      <c r="N84" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="O83" s="45" t="s">
+      <c r="O84" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="P83" s="45" t="s">
+      <c r="P84" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="Q83" s="28"/>
-    </row>
-    <row r="84" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A84" s="2" t="s">
+      <c r="Q84" s="28"/>
+    </row>
+    <row r="85" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" s="2" t="s">
+      <c r="D85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="G84" s="21"/>
-      <c r="L84" s="21"/>
-      <c r="M84" s="17"/>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
-      <c r="Q84" s="28"/>
-    </row>
-    <row r="85" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D85" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="G85" s="21"/>
       <c r="L85" s="21"/>
+      <c r="M85" s="17"/>
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17"/>
       <c r="Q85" s="28"/>
-      <c r="R85" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>19</v>
+    </row>
+    <row r="86" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="G86" s="21"/>
       <c r="L86" s="21"/>
-      <c r="M86" s="17"/>
-      <c r="N86" s="17"/>
-      <c r="O86" s="17"/>
-      <c r="P86" s="17"/>
       <c r="Q86" s="28"/>
-    </row>
-    <row r="87" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A87" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D87" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>240</v>
+      <c r="R86" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G87" s="21"/>
       <c r="L87" s="21"/>
+      <c r="M87" s="17"/>
+      <c r="N87" s="17"/>
+      <c r="O87" s="17"/>
+      <c r="P87" s="17"/>
       <c r="Q87" s="28"/>
-      <c r="R87" s="8" t="s">
+    </row>
+    <row r="88" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A88" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D88" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G88" s="21"/>
+      <c r="L88" s="21"/>
+      <c r="Q88" s="28"/>
+      <c r="R88" s="8" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D88" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G88" s="21"/>
-      <c r="H88" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J88" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="K88" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="L88" s="21"/>
-      <c r="M88" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="N88" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="O88" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="P88" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q88" s="28"/>
     </row>
     <row r="89" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D89" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G89" s="21"/>
+      <c r="H89" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J89" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K89" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L89" s="21"/>
+      <c r="M89" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="N89" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="O89" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="P89" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q89" s="28"/>
+    </row>
+    <row r="90" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2" t="s">
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="G89" s="21"/>
-      <c r="L89" s="21"/>
-      <c r="M89" s="17"/>
-      <c r="N89" s="17"/>
-      <c r="O89" s="17"/>
-      <c r="P89" s="17"/>
-      <c r="Q89" s="28"/>
-    </row>
-    <row r="90" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A90" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D90" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="G90" s="21"/>
       <c r="L90" s="21"/>
+      <c r="M90" s="17"/>
+      <c r="N90" s="17"/>
+      <c r="O90" s="17"/>
+      <c r="P90" s="17"/>
       <c r="Q90" s="28"/>
-      <c r="R90" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    </row>
+    <row r="91" spans="1:18" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A91" s="7" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="D91" s="7" t="b">
         <v>0</v>
       </c>
       <c r="E91" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="G91" s="21"/>
       <c r="L91" s="21"/>
       <c r="Q91" s="28"/>
-      <c r="R91" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A92" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D92" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>98</v>
+      <c r="R91" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A92" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="G92" s="21"/>
       <c r="L92" s="21"/>
-      <c r="M92" s="17"/>
-      <c r="N92" s="17"/>
-      <c r="O92" s="17"/>
-      <c r="P92" s="17"/>
       <c r="Q92" s="28"/>
-    </row>
-    <row r="93" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R92" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D93" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G93" s="21"/>
+      <c r="L93" s="21"/>
+      <c r="M93" s="17"/>
+      <c r="N93" s="17"/>
+      <c r="O93" s="17"/>
+      <c r="P93" s="17"/>
+      <c r="Q93" s="28"/>
+    </row>
+    <row r="94" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G93" s="21"/>
-      <c r="H93" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I93" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K93" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L93" s="21"/>
-      <c r="M93" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N93" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O93" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P93" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q93" s="28"/>
-    </row>
-    <row r="94" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G94" s="21"/>
+      <c r="H94" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K94" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L94" s="21"/>
+      <c r="M94" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N94" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O94" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P94" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q94" s="28"/>
+    </row>
+    <row r="95" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G94" s="21"/>
-      <c r="L94" s="21"/>
-      <c r="M94" s="17"/>
-      <c r="N94" s="17"/>
-      <c r="O94" s="17"/>
-      <c r="P94" s="17"/>
-      <c r="Q94" s="28"/>
-      <c r="R94" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A95" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B95" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C95" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D95" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F95" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="G95" s="28"/>
-      <c r="L95" s="28"/>
+      <c r="D95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G95" s="21"/>
+      <c r="L95" s="21"/>
+      <c r="M95" s="17"/>
+      <c r="N95" s="17"/>
+      <c r="O95" s="17"/>
+      <c r="P95" s="17"/>
       <c r="Q95" s="28"/>
       <c r="R95" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A96" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B96" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D96" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="G96" s="28"/>
+      <c r="L96" s="28"/>
+      <c r="Q96" s="28"/>
+      <c r="R96" s="8" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="96" spans="1:18" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A96" s="2" t="s">
+    <row r="97" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="12" t="s">
+      <c r="D97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="12" t="s">
         <v>290</v>
-      </c>
-      <c r="G96" s="21"/>
-      <c r="L96" s="21"/>
-      <c r="M96" s="17"/>
-      <c r="N96" s="17"/>
-      <c r="O96" s="17"/>
-      <c r="P96" s="17"/>
-      <c r="Q96" s="28"/>
-    </row>
-    <row r="97" spans="1:19" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="B97" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="C97" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D97" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="G97" s="21"/>
       <c r="L97" s="21"/>
@@ -4666,30 +4674,26 @@
       <c r="P97" s="17"/>
       <c r="Q97" s="28"/>
     </row>
-    <row r="98" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B98" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" t="s">
-        <v>329</v>
-      </c>
-      <c r="D98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>25</v>
+    <row r="98" spans="1:19" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D98" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="G98" s="21"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="17"/>
-      <c r="K98" s="17"/>
       <c r="L98" s="21"/>
       <c r="M98" s="17"/>
       <c r="N98" s="17"/>
@@ -4697,76 +4701,80 @@
       <c r="P98" s="17"/>
       <c r="Q98" s="28"/>
     </row>
-    <row r="99" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A99" t="s">
-        <v>327</v>
+    <row r="99" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="B99" t="s">
         <v>10</v>
       </c>
       <c r="C99" t="s">
+        <v>329</v>
+      </c>
+      <c r="D99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G99" s="21"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="17"/>
+      <c r="J99" s="17"/>
+      <c r="K99" s="17"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="17"/>
+      <c r="N99" s="17"/>
+      <c r="O99" s="17"/>
+      <c r="P99" s="17"/>
+      <c r="Q99" s="28"/>
+    </row>
+    <row r="100" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
+        <v>327</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" t="s">
         <v>328</v>
       </c>
-      <c r="D99" t="b">
-        <v>1</v>
-      </c>
-      <c r="E99" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="D100" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" t="s">
         <v>25</v>
       </c>
-      <c r="G99" s="28"/>
-      <c r="L99" s="28"/>
-      <c r="Q99" s="28"/>
-      <c r="R99"/>
-      <c r="S99"/>
-    </row>
-    <row r="100" spans="1:19" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
+      <c r="G100" s="28"/>
+      <c r="L100" s="28"/>
+      <c r="Q100" s="28"/>
+      <c r="R100"/>
+      <c r="S100"/>
+    </row>
+    <row r="101" spans="1:19" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D100" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G100" s="21"/>
-      <c r="L100" s="21"/>
-      <c r="M100" s="17"/>
-      <c r="N100" s="17"/>
-      <c r="O100" s="17"/>
-      <c r="P100" s="17"/>
-      <c r="Q100" s="28"/>
-    </row>
-    <row r="101" spans="1:19" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A101" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D101" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E101" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F101" s="6" t="s">
-        <v>241</v>
+      <c r="F101" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G101" s="21"/>
       <c r="L101" s="21"/>
@@ -4775,19 +4783,16 @@
       <c r="O101" s="17"/>
       <c r="P101" s="17"/>
       <c r="Q101" s="28"/>
-      <c r="R101" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="102" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="102" spans="1:19" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D102" s="2" t="b">
         <v>0</v>
@@ -4795,8 +4800,8 @@
       <c r="E102" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F102" s="2" t="s">
-        <v>16</v>
+      <c r="F102" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="G102" s="21"/>
       <c r="L102" s="21"/>
@@ -4805,22 +4810,28 @@
       <c r="O102" s="17"/>
       <c r="P102" s="17"/>
       <c r="Q102" s="28"/>
-    </row>
-    <row r="103" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="R102" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D103" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E103" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G103" s="21"/>
       <c r="L103" s="21"/>
@@ -4829,28 +4840,22 @@
       <c r="O103" s="17"/>
       <c r="P103" s="17"/>
       <c r="Q103" s="28"/>
-      <c r="R103" s="8" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="104" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="104" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="D104" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="G104" s="21"/>
       <c r="L104" s="21"/>
@@ -4860,91 +4865,95 @@
       <c r="P104" s="17"/>
       <c r="Q104" s="28"/>
       <c r="R104" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A105" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D105" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G105" s="21"/>
+      <c r="L105" s="21"/>
+      <c r="M105" s="17"/>
+      <c r="N105" s="17"/>
+      <c r="O105" s="17"/>
+      <c r="P105" s="17"/>
+      <c r="Q105" s="28"/>
+      <c r="R105" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="105" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A105" s="2" t="s">
+    <row r="106" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A106" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D105" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G105" s="21"/>
-      <c r="H105" s="17" t="s">
+      <c r="D106" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E106" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G106" s="21"/>
+      <c r="H106" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I105" s="17" t="s">
+      <c r="I106" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J105" s="17" t="s">
+      <c r="J106" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K105" s="17" t="s">
+      <c r="K106" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="L105" s="21"/>
-      <c r="M105" s="18" t="s">
+      <c r="L106" s="21"/>
+      <c r="M106" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="N105" s="45" t="s">
+      <c r="N106" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="O105" s="45" t="s">
+      <c r="O106" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="P105" s="45" t="s">
+      <c r="P106" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="Q105" s="28"/>
-      <c r="R105" s="2" t="s">
+      <c r="Q106" s="28"/>
+      <c r="R106" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="106" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A106" s="7" t="s">
+    <row r="107" spans="1:19" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A107" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B107" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C107" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D106" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G106" s="21"/>
-      <c r="L106" s="21"/>
-      <c r="Q106" s="28"/>
-      <c r="R106" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="107" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A107" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="D107" s="7" t="b">
         <v>1</v>
@@ -4959,91 +4968,73 @@
       <c r="L107" s="21"/>
       <c r="Q107" s="28"/>
       <c r="R107" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="108" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D108" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E108" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="G108" s="21"/>
       <c r="L108" s="21"/>
       <c r="Q108" s="28"/>
       <c r="R108" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D109" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G109" s="21"/>
+      <c r="L109" s="21"/>
+      <c r="Q109" s="28"/>
+      <c r="R109" s="7" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="109" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D109" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G109" s="21"/>
-      <c r="H109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109" s="21"/>
-      <c r="M109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q109" s="28"/>
     </row>
     <row r="110" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D110" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110" s="2" t="b">
         <v>1</v>
@@ -5078,23 +5069,23 @@
     </row>
     <row r="111" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D111" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G111" s="21"/>
       <c r="H111" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>4</v>
@@ -5107,7 +5098,7 @@
       </c>
       <c r="L111" s="21"/>
       <c r="M111" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N111" s="17" t="s">
         <v>4</v>
@@ -5120,148 +5111,145 @@
       </c>
       <c r="Q111" s="28"/>
     </row>
-    <row r="112" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D112" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G112" s="21"/>
+      <c r="H112" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L112" s="21"/>
+      <c r="M112" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q112" s="28"/>
+    </row>
+    <row r="113" spans="1:19" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A113" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D112" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E112" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G112" s="21"/>
-      <c r="L112" s="21"/>
-      <c r="M112" s="17"/>
-      <c r="N112" s="17"/>
-      <c r="O112" s="17"/>
-      <c r="P112" s="17"/>
-      <c r="Q112" s="28"/>
-    </row>
-    <row r="113" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A113" t="s">
+      <c r="D113" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E113" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G113" s="21"/>
+      <c r="L113" s="21"/>
+      <c r="M113" s="17"/>
+      <c r="N113" s="17"/>
+      <c r="O113" s="17"/>
+      <c r="P113" s="17"/>
+      <c r="Q113" s="28"/>
+    </row>
+    <row r="114" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
         <v>330</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>5</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>331</v>
       </c>
-      <c r="D113" t="b">
-        <v>0</v>
-      </c>
-      <c r="E113" t="b">
-        <v>1</v>
-      </c>
-      <c r="F113" t="s">
-        <v>4</v>
-      </c>
-      <c r="G113" s="28"/>
-      <c r="H113"/>
-      <c r="I113"/>
-      <c r="J113"/>
-      <c r="K113"/>
-      <c r="L113" s="28"/>
-      <c r="M113"/>
-      <c r="N113"/>
-      <c r="O113"/>
-      <c r="P113"/>
-      <c r="Q113" s="24"/>
-      <c r="R113"/>
-      <c r="S113"/>
-    </row>
-    <row r="114" spans="1:19" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A114" s="7" t="s">
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+      <c r="F114" t="s">
+        <v>4</v>
+      </c>
+      <c r="G114" s="28"/>
+      <c r="H114"/>
+      <c r="I114"/>
+      <c r="J114"/>
+      <c r="K114"/>
+      <c r="L114" s="28"/>
+      <c r="M114"/>
+      <c r="N114"/>
+      <c r="O114"/>
+      <c r="P114"/>
+      <c r="Q114" s="24"/>
+      <c r="R114"/>
+      <c r="S114"/>
+    </row>
+    <row r="115" spans="1:19" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A115" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B114" s="7" t="s">
+      <c r="B115" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C114" s="7" t="s">
+      <c r="C115" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D114" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F114" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G114" s="21"/>
-      <c r="L114" s="21"/>
-      <c r="Q114" s="28"/>
-      <c r="R114" s="7" t="s">
+      <c r="D115" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" s="21"/>
+      <c r="L115" s="21"/>
+      <c r="Q115" s="28"/>
+      <c r="R115" s="7" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="115" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D115" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G115" s="21"/>
-      <c r="H115" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L115" s="21"/>
-      <c r="M115" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N115" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O115" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P115" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q115" s="28"/>
-      <c r="R115" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
-        <v>277</v>
+        <v>129</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D116" s="2" t="b">
         <v>1</v>
@@ -5296,161 +5284,205 @@
         <v>4</v>
       </c>
       <c r="Q116" s="28"/>
+      <c r="R116" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="117" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D117" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G117" s="21"/>
+      <c r="H117" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K117" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L117" s="21"/>
+      <c r="M117" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N117" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O117" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P117" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q117" s="28"/>
+    </row>
+    <row r="118" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A118" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D117" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F117" s="2" t="s">
+      <c r="D118" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G117" s="21"/>
-      <c r="L117" s="21"/>
-      <c r="M117" s="17"/>
-      <c r="N117" s="17"/>
-      <c r="O117" s="17"/>
-      <c r="P117" s="17"/>
-      <c r="Q117" s="28"/>
-    </row>
-    <row r="118" spans="1:19" s="43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="43" t="s">
+      <c r="G118" s="21"/>
+      <c r="L118" s="21"/>
+      <c r="M118" s="17"/>
+      <c r="N118" s="17"/>
+      <c r="O118" s="17"/>
+      <c r="P118" s="17"/>
+      <c r="Q118" s="28"/>
+    </row>
+    <row r="119" spans="1:19" s="43" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="B118" s="43" t="s">
+      <c r="B119" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C118" s="43" t="s">
+      <c r="C119" s="43" t="s">
         <v>360</v>
       </c>
-      <c r="D118" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E118" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G118" s="28"/>
-      <c r="H118" s="43" t="s">
+      <c r="D119" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G119" s="28"/>
+      <c r="H119" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I118" s="43" t="s">
+      <c r="I119" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="J118" s="43" t="s">
+      <c r="J119" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="K118" s="43" t="s">
+      <c r="K119" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="L118" s="28"/>
-      <c r="M118" s="45" t="s">
+      <c r="L119" s="28"/>
+      <c r="M119" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="N118" s="45" t="s">
+      <c r="N119" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="O118" s="45" t="s">
+      <c r="O119" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="P118" s="45" t="s">
+      <c r="P119" s="45" t="s">
         <v>363</v>
       </c>
-      <c r="Q118" s="28"/>
-    </row>
-    <row r="119" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="47" t="s">
+      <c r="Q119" s="28"/>
+    </row>
+    <row r="120" spans="1:19" s="47" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="47" t="s">
         <v>366</v>
       </c>
-      <c r="B119" s="47" t="s">
+      <c r="B120" s="47" t="s">
         <v>367</v>
       </c>
-      <c r="C119" s="47" t="s">
+      <c r="C120" s="47" t="s">
         <v>368</v>
       </c>
-      <c r="D119" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E119" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="F119" s="47" t="s">
+      <c r="D120" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E120" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F120" s="47" t="s">
         <v>369</v>
       </c>
-      <c r="G119" s="28"/>
-      <c r="L119" s="28"/>
-      <c r="Q119" s="28"/>
-    </row>
-    <row r="120" spans="1:19" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A120" s="27" t="s">
+      <c r="G120" s="28"/>
+      <c r="L120" s="28"/>
+      <c r="Q120" s="28"/>
+    </row>
+    <row r="121" spans="1:19" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A121" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="B120" s="27" t="s">
+      <c r="B121" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C120" s="27" t="s">
+      <c r="C121" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="D120" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E120" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F120" s="27" t="s">
+      <c r="D121" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="G120" s="28"/>
-      <c r="H120" s="27"/>
-      <c r="I120" s="27"/>
-      <c r="J120" s="27"/>
-      <c r="K120" s="27"/>
-      <c r="L120" s="28"/>
-      <c r="M120" s="27"/>
-      <c r="Q120" s="28"/>
-    </row>
-    <row r="121" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A121" s="2" t="s">
+      <c r="G121" s="28"/>
+      <c r="H121" s="27"/>
+      <c r="I121" s="27"/>
+      <c r="J121" s="27"/>
+      <c r="K121" s="27"/>
+      <c r="L121" s="28"/>
+      <c r="M121" s="27"/>
+      <c r="Q121" s="28"/>
+    </row>
+    <row r="122" spans="1:19" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A122" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D121" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E121" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F121" s="2" t="s">
+      <c r="D122" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="G121" s="21"/>
-      <c r="L121" s="21"/>
-      <c r="M121" s="17"/>
-      <c r="N121" s="17"/>
-      <c r="O121" s="17"/>
-      <c r="P121" s="17"/>
-      <c r="Q121" s="28"/>
-      <c r="R121" s="2" t="s">
+      <c r="G122" s="21"/>
+      <c r="L122" s="21"/>
+      <c r="M122" s="17"/>
+      <c r="N122" s="17"/>
+      <c r="O122" s="17"/>
+      <c r="P122" s="17"/>
+      <c r="Q122" s="28"/>
+      <c r="R122" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="R122"/>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.4">
       <c r="R123"/>
@@ -5514,6 +5546,9 @@
     </row>
     <row r="143" spans="18:18" x14ac:dyDescent="0.4">
       <c r="R143"/>
+    </row>
+    <row r="144" spans="18:18" x14ac:dyDescent="0.4">
+      <c r="R144"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5521,15 +5556,15 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1"/>
     <hyperlink ref="F21" r:id="rId2"/>
-    <hyperlink ref="F62" r:id="rId3"/>
+    <hyperlink ref="F63" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>

<commit_message>
Kadaster: de default instelling voor nativescalars aangepast.
De default instelling is nu "no" (natives worden niet herkend).

Minor, moet wel worden gecommuniceerd,
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="377">
   <si>
     <t>Name</t>
   </si>
@@ -1300,7 +1300,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1399,6 +1399,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1732,10 +1738,10 @@
   <dimension ref="A1:S144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1945,16 +1951,16 @@
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="50" t="b">
+      <c r="D7" s="52" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1972,10 +1978,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -3232,16 +3238,16 @@
       </c>
     </row>
     <row r="48" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="50" t="s">
+      <c r="A48" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="50" t="s">
+      <c r="C48" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="50" t="b">
+      <c r="D48" s="52" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="2" t="b">
@@ -3259,10 +3265,10 @@
       <c r="Q48" s="28"/>
     </row>
     <row r="49" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="50"/>
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
       <c r="G49" s="21"/>
       <c r="L49" s="21"/>
       <c r="M49" s="17"/>
@@ -4036,17 +4042,17 @@
         <v>0</v>
       </c>
       <c r="G77" s="21"/>
-      <c r="H77" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I77" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="J77" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="K77" s="31" t="s">
-        <v>25</v>
+      <c r="H77" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="I77" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="J77" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="K77" s="50" t="s">
+        <v>363</v>
       </c>
       <c r="L77" s="21"/>
       <c r="M77" s="45" t="s">
@@ -4153,14 +4159,20 @@
       <c r="E81" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="F81" s="42" t="s">
-        <v>4</v>
-      </c>
+      <c r="F81" s="42"/>
       <c r="G81" s="28"/>
-      <c r="H81" s="42"/>
-      <c r="I81" s="42"/>
-      <c r="J81" s="42"/>
-      <c r="K81" s="42"/>
+      <c r="H81" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="K81" s="51" t="s">
+        <v>16</v>
+      </c>
       <c r="L81" s="28"/>
       <c r="M81" s="42" t="s">
         <v>16</v>
@@ -4247,17 +4259,17 @@
         <v>0</v>
       </c>
       <c r="G84" s="21"/>
-      <c r="H84" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I84" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J84" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K84" s="17" t="s">
-        <v>25</v>
+      <c r="H84" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="I84" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="J84" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="K84" s="50" t="s">
+        <v>363</v>
       </c>
       <c r="L84" s="21"/>
       <c r="M84" s="45" t="s">
@@ -4894,17 +4906,17 @@
         <v>0</v>
       </c>
       <c r="G106" s="21"/>
-      <c r="H106" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="I106" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J106" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K106" s="17" t="s">
-        <v>25</v>
+      <c r="H106" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="I106" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="J106" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="K106" s="50" t="s">
+        <v>363</v>
       </c>
       <c r="L106" s="21"/>
       <c r="M106" s="18" t="s">
@@ -5355,17 +5367,17 @@
         <v>1</v>
       </c>
       <c r="G119" s="28"/>
-      <c r="H119" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="I119" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="J119" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="K119" s="43" t="s">
-        <v>25</v>
+      <c r="H119" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="I119" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="J119" s="50" t="s">
+        <v>363</v>
+      </c>
+      <c r="K119" s="50" t="s">
+        <v>363</v>
       </c>
       <c r="L119" s="28"/>
       <c r="M119" s="45" t="s">

</xml_diff>

<commit_message>
Kadaster: Create MIM format is nu onderdeel van regtest.
Minor.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="381">
   <si>
     <t>Name</t>
   </si>
@@ -1753,10 +1753,10 @@
   <dimension ref="A1:U145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H93" sqref="H93:T93"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2918,9 +2918,13 @@
         <v>16</v>
       </c>
       <c r="G33" s="28"/>
-      <c r="L33" s="52"/>
+      <c r="L33" s="52" t="s">
+        <v>4</v>
+      </c>
       <c r="M33" s="28"/>
-      <c r="R33" s="52"/>
+      <c r="R33" s="52" t="s">
+        <v>4</v>
+      </c>
       <c r="S33" s="28"/>
     </row>
     <row r="34" spans="1:20" s="49" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
[Kadaster} Kadaster gaat over op MIM 1.1.1
Hiervoor de configuraties aangepast, cm en cs, en stylesheets voor
canoniseren en valideren.

Minor, is uitbreiding van Kadaster validaties.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="385">
   <si>
     <t>Name</t>
   </si>
@@ -1068,9 +1068,6 @@
     <t>3.2.2</t>
   </si>
   <si>
-    <t>NEN3610_GML322PROFILE_ENV</t>
-  </si>
-  <si>
     <t>creategmlprofile</t>
   </si>
   <si>
@@ -1116,9 +1113,6 @@
     <t>Should an EA toolbox be generated?</t>
   </si>
   <si>
-    <t>KadasterMIM11</t>
-  </si>
-  <si>
     <t>fullrespec</t>
   </si>
   <si>
@@ -1168,6 +1162,24 @@
   </si>
   <si>
     <t>Should a regression test be performed on the results of this run?</t>
+  </si>
+  <si>
+    <t>KadasterMIM111</t>
+  </si>
+  <si>
+    <t>MIM111_GML322PROFILE_ENV</t>
+  </si>
+  <si>
+    <t>mimformatversion</t>
+  </si>
+  <si>
+    <t>v1|v2</t>
+  </si>
+  <si>
+    <t>The version of the MIM compiler</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1324,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1411,6 +1423,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1750,13 +1768,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U145"/>
+  <dimension ref="A1:U146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1768,8 +1786,7 @@
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
     <col min="7" max="7" width="5.4609375" style="24" customWidth="1"/>
-    <col min="8" max="9" width="14.765625" customWidth="1"/>
-    <col min="10" max="10" width="14.3046875" customWidth="1"/>
+    <col min="8" max="10" width="15.765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.765625" customWidth="1"/>
     <col min="12" max="12" width="14.765625" customWidth="1"/>
     <col min="13" max="13" width="5.4609375" style="24" customWidth="1"/>
@@ -1854,7 +1871,7 @@
         <v>306</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M2" s="20"/>
       <c r="N2" s="3" t="s">
@@ -1870,7 +1887,7 @@
         <v>310</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="S2" s="20"/>
       <c r="T2" s="5"/>
@@ -1986,16 +2003,16 @@
       <c r="S6" s="28"/>
     </row>
     <row r="7" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53" t="b">
+      <c r="D7" s="55" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -2015,10 +2032,10 @@
       </c>
     </row>
     <row r="8" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
+      <c r="A8" s="55"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
       <c r="G8" s="21"/>
       <c r="L8" s="52"/>
       <c r="M8" s="21"/>
@@ -2619,13 +2636,13 @@
     </row>
     <row r="27" spans="1:20" s="44" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="44" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B27" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D27" s="44" t="b">
         <v>0</v>
@@ -2669,13 +2686,13 @@
     </row>
     <row r="28" spans="1:20" s="41" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D28" s="41" t="b">
         <v>0</v>
@@ -2900,13 +2917,13 @@
     </row>
     <row r="33" spans="1:20" s="48" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="48" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B33" s="48" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D33" s="48" t="b">
         <v>0</v>
@@ -2929,14 +2946,14 @@
     </row>
     <row r="34" spans="1:20" s="49" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>373</v>
+      </c>
+      <c r="C34" s="49" t="s">
         <v>374</v>
       </c>
-      <c r="B34" s="49" t="s">
-        <v>375</v>
-      </c>
-      <c r="C34" s="49" t="s">
-        <v>376</v>
-      </c>
       <c r="D34" s="49" t="b">
         <v>0</v>
       </c>
@@ -2944,7 +2961,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G34" s="28"/>
       <c r="L34" s="52"/>
@@ -3399,16 +3416,16 @@
       </c>
     </row>
     <row r="48" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="53" t="s">
+      <c r="A48" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="53" t="s">
+      <c r="B48" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="53" t="s">
+      <c r="C48" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="53" t="b">
+      <c r="D48" s="55" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="2" t="b">
@@ -3428,10 +3445,10 @@
       <c r="S48" s="28"/>
     </row>
     <row r="49" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="53"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
+      <c r="A49" s="55"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
       <c r="G49" s="21"/>
       <c r="L49" s="52"/>
       <c r="M49" s="21"/>
@@ -3739,13 +3756,13 @@
     </row>
     <row r="60" spans="1:20" s="46" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A60" s="46" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B60" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="46" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D60" s="46" t="b">
         <v>0</v>
@@ -3899,13 +3916,13 @@
     </row>
     <row r="65" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B65" t="s">
         <v>82</v>
       </c>
       <c r="C65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -3914,7 +3931,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G65" s="28"/>
       <c r="M65" s="28"/>
@@ -3922,22 +3939,22 @@
     </row>
     <row r="66" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B66" t="s">
         <v>82</v>
       </c>
       <c r="C66" t="s">
+        <v>352</v>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
         <v>353</v>
-      </c>
-      <c r="D66" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" t="s">
-        <v>354</v>
       </c>
       <c r="G66" s="28"/>
       <c r="M66" s="28"/>
@@ -4160,7 +4177,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>347</v>
+        <v>380</v>
       </c>
       <c r="G74" s="21"/>
       <c r="L74" s="52"/>
@@ -4248,38 +4265,21 @@
       <c r="E77" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F77" s="53" t="s">
+        <v>379</v>
+      </c>
       <c r="G77" s="21"/>
-      <c r="H77" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="I77" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="J77" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="K77" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="L77" s="52" t="s">
-        <v>363</v>
-      </c>
+      <c r="H77" s="50"/>
+      <c r="I77" s="53"/>
+      <c r="J77" s="50"/>
+      <c r="K77" s="50"/>
+      <c r="L77" s="52"/>
       <c r="M77" s="21"/>
-      <c r="N77" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="O77" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="P77" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q77" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="R77" s="52" t="s">
-        <v>363</v>
-      </c>
+      <c r="N77" s="45"/>
+      <c r="O77" s="45"/>
+      <c r="P77" s="45"/>
+      <c r="Q77" s="45"/>
+      <c r="R77" s="52"/>
       <c r="S77" s="28"/>
     </row>
     <row r="78" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4311,13 +4311,13 @@
     </row>
     <row r="79" spans="1:20" s="48" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A79" s="48" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B79" s="48" t="s">
         <v>10</v>
       </c>
       <c r="C79" s="48" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D79" s="48" t="b">
         <v>0</v>
@@ -4334,130 +4334,124 @@
       <c r="R79" s="52"/>
       <c r="S79" s="28"/>
     </row>
-    <row r="80" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A80" s="7" t="s">
+    <row r="80" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="54" t="s">
+        <v>381</v>
+      </c>
+      <c r="B80" s="54" t="s">
+        <v>382</v>
+      </c>
+      <c r="C80" s="54" t="s">
+        <v>383</v>
+      </c>
+      <c r="D80" s="54" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" s="54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" s="54" t="s">
+        <v>384</v>
+      </c>
+      <c r="G80" s="28"/>
+      <c r="M80" s="28"/>
+      <c r="S80" s="28"/>
+    </row>
+    <row r="81" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B81" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C81" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D80" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" s="21"/>
-      <c r="M80" s="21"/>
-      <c r="S80" s="28"/>
-      <c r="T80" s="7" t="s">
+      <c r="D81" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" s="21"/>
+      <c r="M81" s="21"/>
+      <c r="S81" s="28"/>
+      <c r="T81" s="7" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="81" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="42" t="s">
+    <row r="82" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="42" t="s">
+        <v>354</v>
+      </c>
+      <c r="B82" s="42" t="s">
         <v>355</v>
       </c>
-      <c r="B81" s="42" t="s">
+      <c r="C82" s="42" t="s">
         <v>356</v>
       </c>
-      <c r="C81" s="42" t="s">
-        <v>357</v>
-      </c>
-      <c r="D81" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" s="42"/>
-      <c r="G81" s="28"/>
-      <c r="H81" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="I81" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="J81" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="K81" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="L81" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M81" s="28"/>
-      <c r="N81" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="O81" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="P81" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q81" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="R81" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="S81" s="28"/>
-    </row>
-    <row r="82" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A82" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D82" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G82" s="21"/>
-      <c r="L82" s="52"/>
-      <c r="M82" s="21"/>
-      <c r="N82" s="17"/>
-      <c r="O82" s="17"/>
-      <c r="P82" s="17"/>
-      <c r="Q82" s="17"/>
-      <c r="R82" s="52"/>
+      <c r="D82" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="42"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="J82" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="K82" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="L82" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="M82" s="28"/>
+      <c r="N82" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="O82" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="P82" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q82" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="R82" s="52" t="s">
+        <v>16</v>
+      </c>
       <c r="S82" s="28"/>
     </row>
     <row r="83" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>78</v>
+        <v>264</v>
       </c>
       <c r="D83" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G83" s="21"/>
       <c r="L83" s="52"/>
@@ -4469,517 +4463,499 @@
       <c r="R83" s="52"/>
       <c r="S83" s="28"/>
     </row>
-    <row r="84" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G84" s="21"/>
+      <c r="L84" s="52"/>
+      <c r="M84" s="21"/>
+      <c r="N84" s="17"/>
+      <c r="O84" s="17"/>
+      <c r="P84" s="17"/>
+      <c r="Q84" s="17"/>
+      <c r="R84" s="52"/>
+      <c r="S84" s="28"/>
+    </row>
+    <row r="85" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D84" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G84" s="21"/>
-      <c r="H84" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="I84" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="J84" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="K84" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="L84" s="52" t="s">
-        <v>363</v>
-      </c>
-      <c r="M84" s="21"/>
-      <c r="N84" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="O84" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="P84" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q84" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="R84" s="52" t="s">
-        <v>363</v>
-      </c>
-      <c r="S84" s="28"/>
-    </row>
-    <row r="85" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A85" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="D85" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F85" s="2" t="s">
-        <v>152</v>
+      <c r="F85" s="50" t="s">
+        <v>379</v>
       </c>
       <c r="G85" s="21"/>
+      <c r="I85" s="50"/>
+      <c r="J85" s="50"/>
+      <c r="K85" s="50"/>
       <c r="L85" s="52"/>
       <c r="M85" s="21"/>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
-      <c r="P85" s="17"/>
-      <c r="Q85" s="17"/>
+      <c r="N85" s="45"/>
+      <c r="O85" s="45"/>
+      <c r="P85" s="45"/>
+      <c r="Q85" s="45"/>
       <c r="R85" s="52"/>
       <c r="S85" s="28"/>
     </row>
-    <row r="86" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="7" t="s">
+    <row r="86" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G86" s="21"/>
+      <c r="L86" s="52"/>
+      <c r="M86" s="21"/>
+      <c r="N86" s="17"/>
+      <c r="O86" s="17"/>
+      <c r="P86" s="17"/>
+      <c r="Q86" s="17"/>
+      <c r="R86" s="52"/>
+      <c r="S86" s="28"/>
+    </row>
+    <row r="87" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="B87" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C87" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D86" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E86" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F86" s="7" t="s">
+      <c r="D87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G86" s="21"/>
-      <c r="M86" s="21"/>
-      <c r="S86" s="28"/>
-      <c r="T86" s="7" t="s">
+      <c r="G87" s="21"/>
+      <c r="M87" s="21"/>
+      <c r="S87" s="28"/>
+      <c r="T87" s="7" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="87" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D87" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" s="2" t="s">
+      <c r="D88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G87" s="21"/>
-      <c r="L87" s="52"/>
-      <c r="M87" s="21"/>
-      <c r="N87" s="17"/>
-      <c r="O87" s="17"/>
-      <c r="P87" s="17"/>
-      <c r="Q87" s="17"/>
-      <c r="R87" s="52"/>
-      <c r="S87" s="28"/>
-    </row>
-    <row r="88" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A88" s="7" t="s">
+      <c r="G88" s="21"/>
+      <c r="L88" s="52"/>
+      <c r="M88" s="21"/>
+      <c r="N88" s="17"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="17"/>
+      <c r="Q88" s="17"/>
+      <c r="R88" s="52"/>
+      <c r="S88" s="28"/>
+    </row>
+    <row r="89" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A89" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B89" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C89" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D88" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" s="7" t="s">
+      <c r="D89" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="G88" s="21"/>
-      <c r="M88" s="21"/>
-      <c r="S88" s="28"/>
-      <c r="T88" s="8" t="s">
+      <c r="G89" s="21"/>
+      <c r="M89" s="21"/>
+      <c r="S89" s="28"/>
+      <c r="T89" s="8" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="89" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D89" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G89" s="21"/>
-      <c r="H89" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I89" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J89" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="K89" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="L89" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="M89" s="21"/>
-      <c r="N89" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="O89" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="P89" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q89" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="R89" s="52" t="s">
-        <v>243</v>
-      </c>
-      <c r="S89" s="28"/>
     </row>
     <row r="90" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" s="21"/>
+      <c r="H90" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J90" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K90" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L90" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="M90" s="21"/>
+      <c r="N90" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="O90" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="P90" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q90" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="R90" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="S90" s="28"/>
+    </row>
+    <row r="91" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="2" t="s">
+      <c r="D91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G90" s="21"/>
-      <c r="L90" s="52"/>
-      <c r="M90" s="21"/>
-      <c r="N90" s="17"/>
-      <c r="O90" s="17"/>
-      <c r="P90" s="17"/>
-      <c r="Q90" s="17"/>
-      <c r="R90" s="52"/>
-      <c r="S90" s="28"/>
-    </row>
-    <row r="91" spans="1:20" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A91" s="7" t="s">
+      <c r="G91" s="21"/>
+      <c r="L91" s="52"/>
+      <c r="M91" s="21"/>
+      <c r="N91" s="17"/>
+      <c r="O91" s="17"/>
+      <c r="P91" s="17"/>
+      <c r="Q91" s="17"/>
+      <c r="R91" s="52"/>
+      <c r="S91" s="28"/>
+    </row>
+    <row r="92" spans="1:20" s="7" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A92" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B92" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C92" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D91" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E91" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" s="7" t="s">
+      <c r="D92" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="G91" s="21"/>
-      <c r="M91" s="21"/>
-      <c r="S91" s="28"/>
-      <c r="T91" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="92" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A92" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D92" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="G92" s="21"/>
       <c r="M92" s="21"/>
       <c r="S92" s="28"/>
-      <c r="T92" s="7" t="s">
+      <c r="T92" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A93" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D93" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" s="21"/>
+      <c r="M93" s="21"/>
+      <c r="S93" s="28"/>
+      <c r="T93" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="93" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="35" t="s">
-        <v>379</v>
-      </c>
-      <c r="B93" s="35" t="s">
+    <row r="94" spans="1:20" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A94" s="35" t="s">
+        <v>377</v>
+      </c>
+      <c r="B94" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C93" s="35" t="s">
-        <v>380</v>
-      </c>
-      <c r="D93" s="35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="G93" s="28"/>
-      <c r="H93" s="35"/>
-      <c r="I93" s="35"/>
-      <c r="J93" s="35"/>
-      <c r="K93" s="35"/>
-      <c r="L93" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="M93" s="36"/>
-      <c r="N93" s="35"/>
-      <c r="O93" s="35"/>
-      <c r="P93" s="35"/>
-      <c r="Q93" s="35"/>
-      <c r="R93" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="S93" s="36"/>
-      <c r="T93" s="35"/>
-    </row>
-    <row r="94" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A94" s="2" t="s">
+      <c r="C94" s="35" t="s">
+        <v>378</v>
+      </c>
+      <c r="D94" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" s="28"/>
+      <c r="H94" s="35"/>
+      <c r="I94" s="35"/>
+      <c r="J94" s="35"/>
+      <c r="K94" s="35"/>
+      <c r="L94" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="M94" s="36"/>
+      <c r="N94" s="35"/>
+      <c r="O94" s="35"/>
+      <c r="P94" s="35"/>
+      <c r="Q94" s="35"/>
+      <c r="R94" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="S94" s="36"/>
+      <c r="T94" s="35"/>
+    </row>
+    <row r="95" spans="1:20" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D94" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F94" s="2" t="s">
+      <c r="D95" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G94" s="21"/>
-      <c r="L94" s="52"/>
-      <c r="M94" s="21"/>
-      <c r="N94" s="17"/>
-      <c r="O94" s="17"/>
-      <c r="P94" s="17"/>
-      <c r="Q94" s="17"/>
-      <c r="R94" s="52"/>
-      <c r="S94" s="28"/>
-    </row>
-    <row r="95" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="2" t="s">
+      <c r="G95" s="21"/>
+      <c r="L95" s="52"/>
+      <c r="M95" s="21"/>
+      <c r="N95" s="17"/>
+      <c r="O95" s="17"/>
+      <c r="P95" s="17"/>
+      <c r="Q95" s="17"/>
+      <c r="R95" s="52"/>
+      <c r="S95" s="28"/>
+    </row>
+    <row r="96" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G95" s="21"/>
-      <c r="H95" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K95" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L95" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="M95" s="21"/>
-      <c r="N95" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O95" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="P95" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q95" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R95" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="S95" s="28"/>
-    </row>
-    <row r="96" spans="1:20" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A96" s="2" t="s">
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" s="21"/>
+      <c r="H96" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K96" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L96" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="M96" s="21"/>
+      <c r="N96" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O96" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="P96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q96" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="R96" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="S96" s="28"/>
+    </row>
+    <row r="97" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B97" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D96" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G96" s="21"/>
-      <c r="L96" s="52"/>
-      <c r="M96" s="21"/>
-      <c r="N96" s="17"/>
-      <c r="O96" s="17"/>
-      <c r="P96" s="17"/>
-      <c r="Q96" s="17"/>
-      <c r="R96" s="52"/>
-      <c r="S96" s="28"/>
-      <c r="T96" s="8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="97" spans="1:21" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A97" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B97" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C97" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D97" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F97" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="G97" s="28"/>
+      <c r="D97" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G97" s="21"/>
       <c r="L97" s="52"/>
-      <c r="M97" s="28"/>
+      <c r="M97" s="21"/>
+      <c r="N97" s="17"/>
+      <c r="O97" s="17"/>
+      <c r="P97" s="17"/>
+      <c r="Q97" s="17"/>
       <c r="R97" s="52"/>
       <c r="S97" s="28"/>
       <c r="T97" s="8" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="98" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A98" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D98" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="G98" s="21"/>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" s="32" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A98" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D98" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F98" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="G98" s="28"/>
       <c r="L98" s="52"/>
-      <c r="M98" s="21"/>
-      <c r="N98" s="17"/>
-      <c r="O98" s="17"/>
-      <c r="P98" s="17"/>
-      <c r="Q98" s="17"/>
+      <c r="M98" s="28"/>
       <c r="R98" s="52"/>
       <c r="S98" s="28"/>
-    </row>
-    <row r="99" spans="1:21" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A99" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="B99" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="C99" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="D99" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="6" t="s">
-        <v>289</v>
+      <c r="T98" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A99" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D99" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>290</v>
       </c>
       <c r="G99" s="21"/>
       <c r="L99" s="52"/>
@@ -4991,30 +4967,26 @@
       <c r="R99" s="52"/>
       <c r="S99" s="28"/>
     </row>
-    <row r="100" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B100" t="s">
-        <v>10</v>
-      </c>
-      <c r="C100" t="s">
-        <v>329</v>
-      </c>
-      <c r="D100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>25</v>
+    <row r="100" spans="1:21" s="14" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A100" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="G100" s="21"/>
-      <c r="H100" s="17"/>
-      <c r="I100" s="17"/>
-      <c r="J100" s="17"/>
-      <c r="K100" s="17"/>
       <c r="L100" s="52"/>
       <c r="M100" s="21"/>
       <c r="N100" s="17"/>
@@ -5024,78 +4996,82 @@
       <c r="R100" s="52"/>
       <c r="S100" s="28"/>
     </row>
-    <row r="101" spans="1:21" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
-        <v>327</v>
+    <row r="101" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A101" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="B101" t="s">
         <v>10</v>
       </c>
       <c r="C101" t="s">
+        <v>329</v>
+      </c>
+      <c r="D101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G101" s="21"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="17"/>
+      <c r="J101" s="17"/>
+      <c r="K101" s="17"/>
+      <c r="L101" s="52"/>
+      <c r="M101" s="21"/>
+      <c r="N101" s="17"/>
+      <c r="O101" s="17"/>
+      <c r="P101" s="17"/>
+      <c r="Q101" s="17"/>
+      <c r="R101" s="52"/>
+      <c r="S101" s="28"/>
+    </row>
+    <row r="102" spans="1:21" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
+        <v>327</v>
+      </c>
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" t="s">
         <v>328</v>
       </c>
-      <c r="D101" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" t="b">
-        <v>1</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" t="s">
         <v>25</v>
       </c>
-      <c r="G101" s="28"/>
-      <c r="M101" s="28"/>
-      <c r="S101" s="28"/>
-      <c r="T101"/>
-      <c r="U101"/>
-    </row>
-    <row r="102" spans="1:21" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="2" t="s">
+      <c r="G102" s="28"/>
+      <c r="M102" s="28"/>
+      <c r="S102" s="28"/>
+      <c r="T102"/>
+      <c r="U102"/>
+    </row>
+    <row r="103" spans="1:21" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D102" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G102" s="21"/>
-      <c r="L102" s="52"/>
-      <c r="M102" s="21"/>
-      <c r="N102" s="17"/>
-      <c r="O102" s="17"/>
-      <c r="P102" s="17"/>
-      <c r="Q102" s="17"/>
-      <c r="R102" s="52"/>
-      <c r="S102" s="28"/>
-    </row>
-    <row r="103" spans="1:21" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
-      <c r="A103" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="D103" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F103" s="6" t="s">
-        <v>241</v>
+      <c r="F103" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G103" s="21"/>
       <c r="L103" s="52"/>
@@ -5106,19 +5082,16 @@
       <c r="Q103" s="17"/>
       <c r="R103" s="52"/>
       <c r="S103" s="28"/>
-      <c r="T103" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="104" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="104" spans="1:21" s="2" customFormat="1" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D104" s="2" t="b">
         <v>0</v>
@@ -5126,8 +5099,8 @@
       <c r="E104" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F104" s="2" t="s">
-        <v>16</v>
+      <c r="F104" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="G104" s="21"/>
       <c r="L104" s="52"/>
@@ -5138,22 +5111,28 @@
       <c r="Q104" s="17"/>
       <c r="R104" s="52"/>
       <c r="S104" s="28"/>
-    </row>
-    <row r="105" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="T104" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
-        <v>208</v>
+        <v>106</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>209</v>
+        <v>107</v>
       </c>
       <c r="D105" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E105" s="2" t="b">
         <v>1</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G105" s="21"/>
       <c r="L105" s="52"/>
@@ -5164,28 +5143,22 @@
       <c r="Q105" s="17"/>
       <c r="R105" s="52"/>
       <c r="S105" s="28"/>
-      <c r="T105" s="8" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="106" spans="1:21" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+    </row>
+    <row r="106" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>108</v>
+        <v>208</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="D106" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="G106" s="21"/>
       <c r="L106" s="52"/>
@@ -5197,97 +5170,86 @@
       <c r="R106" s="52"/>
       <c r="S106" s="28"/>
       <c r="T106" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.4">
+      <c r="A107" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D107" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E107" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G107" s="21"/>
+      <c r="L107" s="52"/>
+      <c r="M107" s="21"/>
+      <c r="N107" s="17"/>
+      <c r="O107" s="17"/>
+      <c r="P107" s="17"/>
+      <c r="Q107" s="17"/>
+      <c r="R107" s="52"/>
+      <c r="S107" s="28"/>
+      <c r="T107" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="107" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A108" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D107" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E107" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G107" s="21"/>
-      <c r="H107" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="I107" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="J107" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="K107" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="L107" s="52" t="s">
-        <v>363</v>
-      </c>
-      <c r="M107" s="21"/>
-      <c r="N107" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="O107" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="P107" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q107" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="R107" s="52" t="s">
-        <v>363</v>
-      </c>
-      <c r="S107" s="28"/>
-      <c r="T107" s="2" t="s">
+      <c r="D108" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E108" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="G108" s="21"/>
+      <c r="H108" s="50"/>
+      <c r="I108" s="50"/>
+      <c r="J108" s="50"/>
+      <c r="K108" s="50"/>
+      <c r="L108" s="52"/>
+      <c r="M108" s="21"/>
+      <c r="N108" s="18"/>
+      <c r="O108" s="45"/>
+      <c r="P108" s="45"/>
+      <c r="Q108" s="45"/>
+      <c r="R108" s="52"/>
+      <c r="S108" s="28"/>
+      <c r="T108" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="108" spans="1:21" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A108" s="7" t="s">
+    <row r="109" spans="1:21" s="7" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A109" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="B109" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C109" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D108" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E108" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="G108" s="21"/>
-      <c r="M108" s="21"/>
-      <c r="S108" s="28"/>
-      <c r="T108" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B109" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="D109" s="7" t="b">
         <v>1</v>
@@ -5302,97 +5264,73 @@
       <c r="M109" s="21"/>
       <c r="S109" s="28"/>
       <c r="T109" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="110" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D110" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E110" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="G110" s="21"/>
       <c r="M110" s="21"/>
       <c r="S110" s="28"/>
       <c r="T110" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D111" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G111" s="21"/>
+      <c r="M111" s="21"/>
+      <c r="S111" s="28"/>
+      <c r="T111" s="7" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="111" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D111" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E111" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G111" s="21"/>
-      <c r="H111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K111" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L111" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="M111" s="21"/>
-      <c r="N111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="O111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q111" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R111" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="S111" s="28"/>
     </row>
     <row r="112" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D112" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112" s="2" t="b">
         <v>1</v>
@@ -5433,23 +5371,23 @@
     </row>
     <row r="113" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D113" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G113" s="21"/>
       <c r="H113" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>4</v>
@@ -5465,7 +5403,7 @@
       </c>
       <c r="M113" s="21"/>
       <c r="N113" s="17" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O113" s="17" t="s">
         <v>4</v>
@@ -5481,158 +5419,155 @@
       </c>
       <c r="S113" s="28"/>
     </row>
-    <row r="114" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C114" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D114" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G114" s="21"/>
+      <c r="H114" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K114" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L114" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="M114" s="21"/>
+      <c r="N114" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q114" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="R114" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="S114" s="28"/>
+    </row>
+    <row r="115" spans="1:21" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A115" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D114" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E114" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G114" s="21"/>
-      <c r="L114" s="52"/>
-      <c r="M114" s="21"/>
-      <c r="N114" s="17"/>
-      <c r="O114" s="17"/>
-      <c r="P114" s="17"/>
-      <c r="Q114" s="17"/>
-      <c r="R114" s="52"/>
-      <c r="S114" s="28"/>
-    </row>
-    <row r="115" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A115" t="s">
+      <c r="D115" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G115" s="21"/>
+      <c r="L115" s="52"/>
+      <c r="M115" s="21"/>
+      <c r="N115" s="17"/>
+      <c r="O115" s="17"/>
+      <c r="P115" s="17"/>
+      <c r="Q115" s="17"/>
+      <c r="R115" s="52"/>
+      <c r="S115" s="28"/>
+    </row>
+    <row r="116" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
         <v>330</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>5</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C116" t="s">
         <v>331</v>
       </c>
-      <c r="D115" t="b">
-        <v>0</v>
-      </c>
-      <c r="E115" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" t="s">
-        <v>4</v>
-      </c>
-      <c r="G115" s="28"/>
-      <c r="H115"/>
-      <c r="I115"/>
-      <c r="J115"/>
-      <c r="K115"/>
-      <c r="L115"/>
-      <c r="M115" s="28"/>
-      <c r="N115"/>
-      <c r="O115"/>
-      <c r="P115"/>
-      <c r="Q115"/>
-      <c r="R115"/>
-      <c r="S115" s="24"/>
-      <c r="T115"/>
-      <c r="U115"/>
-    </row>
-    <row r="116" spans="1:21" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A116" s="7" t="s">
+      <c r="D116" t="b">
+        <v>0</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" t="s">
+        <v>4</v>
+      </c>
+      <c r="G116" s="28"/>
+      <c r="H116"/>
+      <c r="I116"/>
+      <c r="J116"/>
+      <c r="K116"/>
+      <c r="L116"/>
+      <c r="M116" s="28"/>
+      <c r="N116"/>
+      <c r="O116"/>
+      <c r="P116"/>
+      <c r="Q116"/>
+      <c r="R116"/>
+      <c r="S116" s="24"/>
+      <c r="T116"/>
+      <c r="U116"/>
+    </row>
+    <row r="117" spans="1:21" s="7" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A117" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B116" s="7" t="s">
+      <c r="B117" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C117" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D116" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F116" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G116" s="21"/>
-      <c r="M116" s="21"/>
-      <c r="S116" s="28"/>
-      <c r="T116" s="7" t="s">
+      <c r="D117" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G117" s="21"/>
+      <c r="M117" s="21"/>
+      <c r="S117" s="28"/>
+      <c r="T117" s="7" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="117" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D117" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G117" s="21"/>
-      <c r="H117" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K117" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L117" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="M117" s="21"/>
-      <c r="N117" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="O117" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P117" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q117" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="R117" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="S117" s="28"/>
-      <c r="T117" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="118" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
-        <v>277</v>
+        <v>129</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D118" s="2" t="b">
         <v>1</v>
@@ -5673,175 +5608,207 @@
         <v>4</v>
       </c>
       <c r="S118" s="28"/>
+      <c r="T118" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="119" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G119" s="21"/>
+      <c r="H119" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K119" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L119" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="M119" s="21"/>
+      <c r="N119" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O119" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P119" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q119" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="R119" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="S119" s="28"/>
+    </row>
+    <row r="120" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D119" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E119" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F119" s="2" t="s">
+      <c r="D120" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G119" s="21"/>
-      <c r="L119" s="52"/>
-      <c r="M119" s="21"/>
-      <c r="N119" s="17"/>
-      <c r="O119" s="17"/>
-      <c r="P119" s="17"/>
-      <c r="Q119" s="17"/>
-      <c r="R119" s="52"/>
-      <c r="S119" s="28"/>
-    </row>
-    <row r="120" spans="1:21" s="43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A120" s="43" t="s">
+      <c r="G120" s="21"/>
+      <c r="L120" s="52"/>
+      <c r="M120" s="21"/>
+      <c r="N120" s="17"/>
+      <c r="O120" s="17"/>
+      <c r="P120" s="17"/>
+      <c r="Q120" s="17"/>
+      <c r="R120" s="52"/>
+      <c r="S120" s="28"/>
+    </row>
+    <row r="121" spans="1:21" s="43" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="43" t="s">
+        <v>358</v>
+      </c>
+      <c r="B121" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="B120" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C120" s="43" t="s">
-        <v>360</v>
-      </c>
-      <c r="D120" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E120" s="43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G120" s="28"/>
-      <c r="H120" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="I120" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="J120" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="K120" s="50" t="s">
-        <v>363</v>
-      </c>
-      <c r="L120" s="52" t="s">
-        <v>363</v>
-      </c>
-      <c r="M120" s="28"/>
-      <c r="N120" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="O120" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="P120" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q120" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="R120" s="52" t="s">
-        <v>363</v>
-      </c>
-      <c r="S120" s="28"/>
-    </row>
-    <row r="121" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="47" t="s">
-        <v>366</v>
-      </c>
-      <c r="B121" s="47" t="s">
-        <v>367</v>
-      </c>
-      <c r="C121" s="47" t="s">
-        <v>368</v>
-      </c>
-      <c r="D121" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E121" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="F121" s="47" t="s">
-        <v>369</v>
+      <c r="D121" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="50" t="s">
+        <v>379</v>
       </c>
       <c r="G121" s="28"/>
+      <c r="I121" s="50"/>
+      <c r="J121" s="50"/>
+      <c r="K121" s="50"/>
       <c r="L121" s="52"/>
       <c r="M121" s="28"/>
+      <c r="N121" s="45"/>
+      <c r="O121" s="45"/>
+      <c r="P121" s="45"/>
+      <c r="Q121" s="45"/>
       <c r="R121" s="52"/>
       <c r="S121" s="28"/>
     </row>
-    <row r="122" spans="1:21" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A122" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="B122" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C122" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="D122" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E122" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F122" s="27" t="s">
-        <v>298</v>
+    <row r="122" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="47" t="s">
+        <v>364</v>
+      </c>
+      <c r="B122" s="47" t="s">
+        <v>365</v>
+      </c>
+      <c r="C122" s="47" t="s">
+        <v>366</v>
+      </c>
+      <c r="D122" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E122" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="47" t="s">
+        <v>367</v>
       </c>
       <c r="G122" s="28"/>
-      <c r="H122" s="27"/>
-      <c r="I122" s="27"/>
-      <c r="J122" s="27"/>
-      <c r="K122" s="27"/>
       <c r="L122" s="52"/>
       <c r="M122" s="28"/>
-      <c r="N122" s="27"/>
       <c r="R122" s="52"/>
       <c r="S122" s="28"/>
     </row>
-    <row r="123" spans="1:21" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A123" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D123" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E123" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="G123" s="21"/>
+    <row r="123" spans="1:21" s="26" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A123" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="B123" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123" s="27" t="s">
+        <v>297</v>
+      </c>
+      <c r="D123" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E123" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F123" s="27" t="s">
+        <v>298</v>
+      </c>
+      <c r="G123" s="28"/>
+      <c r="H123" s="27"/>
+      <c r="I123" s="27"/>
+      <c r="J123" s="27"/>
+      <c r="K123" s="27"/>
       <c r="L123" s="52"/>
-      <c r="M123" s="21"/>
-      <c r="N123" s="17"/>
-      <c r="O123" s="17"/>
-      <c r="P123" s="17"/>
-      <c r="Q123" s="17"/>
+      <c r="M123" s="28"/>
+      <c r="N123" s="27"/>
       <c r="R123" s="52"/>
       <c r="S123" s="28"/>
-      <c r="T123" s="2" t="s">
+    </row>
+    <row r="124" spans="1:21" s="2" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A124" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D124" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E124" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G124" s="21"/>
+      <c r="L124" s="52"/>
+      <c r="M124" s="21"/>
+      <c r="N124" s="17"/>
+      <c r="O124" s="17"/>
+      <c r="P124" s="17"/>
+      <c r="Q124" s="17"/>
+      <c r="R124" s="52"/>
+      <c r="S124" s="28"/>
+      <c r="T124" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="T124"/>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.4">
       <c r="T125"/>
@@ -5905,6 +5872,9 @@
     </row>
     <row r="145" spans="20:20" x14ac:dyDescent="0.4">
       <c r="T145"/>
+    </row>
+    <row r="146" spans="20:20" x14ac:dyDescent="0.4">
+      <c r="T146"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Kadaster setting createjsonschemavariant gezet op "plainjson".
Was "Kadaster", maar dat is onjuist.

Bugfix.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/Kadaster/props/Kadaster.xlsx
+++ b/src/main/resources/input/Kadaster/props/Kadaster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\Kadaster\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769A6B3F-1ED2-4656-9B34-A834DB2EB201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0347220-9A3A-4A5E-9182-3FC48F2D8DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kadaster" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="388">
   <si>
     <t>Name</t>
   </si>
@@ -1187,6 +1187,9 @@
   </si>
   <si>
     <t>xml</t>
+  </si>
+  <si>
+    <t>plainjson</t>
   </si>
 </sst>
 </file>
@@ -1682,10 +1685,10 @@
   <dimension ref="A1:U147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A80" sqref="A80"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2693,35 +2696,35 @@
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="M32" s="16"/>
       <c r="N32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>25</v>
+        <v>387</v>
       </c>
       <c r="S32" s="16"/>
       <c r="T32" s="2" t="s">

</xml_diff>